<commit_message>
wk2, alter schedule fmt
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/ADS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Finals Week</t>
   </si>
@@ -44,36 +44,13 @@
     <t>Prepare</t>
   </si>
   <si>
-    <t>Materials</t>
-  </si>
-  <si>
     <t>Assignments</t>
   </si>
   <si>
     <t>Topics</t>
   </si>
   <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Version Control, Team collaboration, R Programming</t>
-  </si>
-  <si>
-    <t>Join our Slack Channel
-* Install the Slack app for your phone
-* Update R Studio</t>
-  </si>
-  <si>
     <t>Social Media for Academics</t>
-  </si>
-  <si>
-    <t>Start an academic/professional webpage (index, about, cv, blog)</t>
-  </si>
-  <si>
-    <t>Workflow automation using make files</t>
   </si>
   <si>
     <t xml:space="preserve">* Be familiar with modern team collaboration and version control tools 
@@ -83,62 +60,85 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Connect to slack team. Join the #r4ds and #git channels. Link to your github account name in the #git channel. 
-* r4ds programming assignment (submit link to .md file in BBL by due date)
-</t>
-  </si>
-  <si>
     <t>* [HappygitwithR Ch 1-16](http://happygitwithr.com/)
 * Github assignment repo [link](https://classroom.github.com/a/5I9Qnnbl)
 * [r4ds CH 17-21.5](http://r4ds.had.co.nz/program-intro.html)</t>
   </si>
   <si>
-    <t>* [Blogdown](https://bookdown.org/yihui/blogdown/)
-* [Alice Hills Tutorial](https://alison.rbind.io/post/up-and-running-with-blogdown/)</t>
-  </si>
-  <si>
-    <r>
-      <t>* Look over the following websites for structure/appearance [Alison Hill](https://alison.rbind.io/) [CSUC DSI](datascience.csuchico.edu) [ESPM 157](</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://espm-157.carlboettiger.info/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>), [Rbind](https://support.rbind.io/), [Simply Statistics](https://simplystatistics.org/)</t>
-    </r>
-  </si>
-  <si>
     <t>* Create an professional online presence
 * Connect with the current state of DS</t>
   </si>
   <si>
-    <t>* Introduction and orientation to Slack and Github 
-* Take control of Assignment repo</t>
-  </si>
-  <si>
-    <t>* Practice your R programming skills by working through r4ds.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* We're going to use Hugo/Blogdown to create a professional looking website. </t>
+    <t xml:space="preserve">* Start reading the blogdown tutorials and looking for DS sources of interest. </t>
+  </si>
+  <si>
+    <t>Topic1</t>
+  </si>
+  <si>
+    <t>Topic2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Introduction and orientation to Slack and Github 
+* Take control of Assignment repo (link under materials). This provides you a repo and a starting template for your homework.
+* Practice your R programming skills by working through r4ds Ch 17-21.5
+* Most homework will be submitted through this repo. Direct links to the *.md file that you want me to review will be submitted via BBL for easy gradebook entry. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Join our Slack Channel [csuc-ads-s18](https://join.slack.com/t/csuc-ads-s18/shared_invite/enQtMjk3MTIyOTMxMjE2LWQwYjIxYmRlYmU1NzI0N2U1ODE2MmFlYzJkYWEwZjViZDRkMDkyMDBkNTNjNzNmNWY2M2ZiMmE0MTNjNGVkNzM)
+* Install the Slack app for your phone and/or computer
+* Update R &amp; R Studio (if done &lt; 6mo ago)
+* If you're new to Git - I recommend using Sourcetree as your external client (yes you have to make an atlassian account, but that's ok. It opens availability to their other useful software products as well) 
+* Get the textbook - [Weapons of Math Destruction](https://www.amazon.com/Weapons-Math-Destruction-Increases-Inequality/dp/0553418815). There is  1 copy available in the Library -- Someone go check this out for the semester and share! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* You don't know what you don’t know.
+* We're going to explore the current world of DS by finding and following people in the world doing DS in an area that interests you. 
+* Find a data science, data visualization, data story, data SOMETHING blog, podcast, twitter feed (or two) to follow. You will be sharing stories weekly, so you may need to find more than one source if your first choice does not update frequently enough.
+</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Follow the tutorials provided to build your website using blogdown. Minimum information includes an 'about' paragraph. 
+* Edit your pinned slack introduction message to include the link to your website. 
+* Tell us a little bit about your DS sources (blog/podcast/twitter) in #state-of-ds. You won't start blogging until next week. </t>
+  </si>
+  <si>
+    <t>Version Control with git, Team collaboration with slack, Intermediate R Programming concepts.</t>
+  </si>
+  <si>
+    <t>* Join all visable Slack channels. 
+* Introduce yourself in #introductions (Name/major/year/github handle/other info you want to share). Pin this message to this board. 
+* r4ds programming assignment</t>
+  </si>
+  <si>
+    <t>Predictive Analytics Lifecycle (I-III): Get, Explore, Clean. Then automate all the things!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Add your CV to your website and create one blog post. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Recap the predictive analytcs life cycle (PAL). 
+* We'll discuss why you may want to automate script files as opposed to (say) clicking the "knit" button. 
+* </t>
+  </si>
+  <si>
+    <t>* [Blogdown](https://bookdown.org/yihui/blogdown/)
+* [Alice Hills Tutorial](https://alison.rbind.io/post/up-and-running-with-blogdown/)
+* [Curation vs Creation](https://www.agorapulse.com/blog/lets-clear-content-creation-vs-content-curation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* You're going to use Hugo/Blogdown to create a professional looking website. 
+* Each week you will write a post about something in the DS world that you found interseting. It doesn't have to be a long or involved post.
+* This is about practicing writing for a public audience. The more you write the better you'll get. 
+* Wait.. why the heck should I create a website? The internet is scary! </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -190,7 +190,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,13 +205,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +366,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -383,32 +389,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="89" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="89" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="90">
@@ -500,11 +509,16 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -837,35 +851,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="27" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="24.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.25" style="5" customWidth="1"/>
+    <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="39.75" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.25" style="5" customWidth="1"/>
+    <col min="9" max="9" width="30.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>7</v>
+      <c r="C1" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -873,77 +887,77 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="105" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    </row>
+    <row r="2" spans="1:9" ht="204.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>41661</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="F2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>41668</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="C3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -951,17 +965,21 @@
         <f t="shared" si="0"/>
         <v>41675</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -977,7 +995,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -993,7 +1011,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1009,7 +1027,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1025,7 +1043,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1042,17 +1060,17 @@
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1067,7 +1085,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1083,7 +1101,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1094,12 +1112,12 @@
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="14"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1115,7 +1133,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1131,7 +1149,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1147,7 +1165,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1163,7 +1181,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add wk5 and 6
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Finals Week</t>
   </si>
@@ -82,11 +83,6 @@
     <t>References</t>
   </si>
   <si>
-    <t xml:space="preserve">* Follow the tutorials provided to build your website using blogdown. Minimum information includes an 'about' paragraph. 
-* Edit your pinned slack introduction message to include the link to your website. 
-* Tell us a little bit about your DS sources (blog/podcast/twitter) in #state-of-ds. You won't start blogging until next week. </t>
-  </si>
-  <si>
     <t>Version Control with git, Team collaboration with slack, Intermediate R Programming concepts.</t>
   </si>
   <si>
@@ -116,9 +112,6 @@
     <t xml:space="preserve">* Demonstrate a deeper understanding of the underworkings behind linear models. </t>
   </si>
   <si>
-    <t>* R4DS Exercises 24.2.3 (all), 24.3.5 (#1, one of #3-#5, #6, #7)</t>
-  </si>
-  <si>
     <t>* [Software Carpentry Shell Novice lesson](http://swcarpentry.github.io/shell-novice/)
 * [Software Carpentry Make Novice lesson](http://swcarpentry.github.io/make-novice/)
 * [Example of when/why to use make files](https://dzone.com/articles/makefiles-rlatex-projects)
@@ -132,13 +125,6 @@
 * Work through at least one of the three toy pipelines from the [Stat 545](http://stat545.com/automation00_index.html) website. </t>
   </si>
   <si>
-    <t xml:space="preserve">* Using the gapminder data set, explore the question "How does life expectancy change over time for each country?"  Automate your entire workflow including data acquisition as a separate R file.  and write a tutorial/walk through as a blog post. Share your post under #assignments and drop a note in BBL when you are done. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* All exercises in 23.2.1 (#1, #2) , 23.3.3 (#1, #3, #4),  23.4.5 (#1, #3, #4). Add this assignment to your github repo as a new RMD file. 
-* Write a blog post about something you found interesting in the DS world this past week. </t>
-  </si>
-  <si>
     <t xml:space="preserve">* Join our Slack Channel [csuc-ads-s18](https://join.slack.com/t/csuc-ads-s18/shared_invite/enQtMjk3MTIyOTMxMjE2LWQwYjIxYmRlYmU1NzI0N2U1ODE2MmFlYzJkYWEwZjViZDRkMDkyMDBkNTNjNzNmNWY2M2ZiMmE0MTNjNGVkNzM)
 * Install the Slack app for your phone and/or computer
 * Update R &amp; R Studio (if done &lt; 6mo ago)
@@ -157,11 +143,6 @@
 * Most homework will be submitted through this repo. Direct links to the *.md file that you want me to review will be submitted via BBL for easy gradebook entry. </t>
   </si>
   <si>
-    <t>* Join all visible Slack channels. 
-* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. 
-* r4ds programming assignment</t>
-  </si>
-  <si>
     <t xml:space="preserve">* You're going to use Hugo/Blogdown to create a professional looking website. 
 * Each week you will write a post about something in the DS world that you found interesting. It doesn't have to be a long or involved post.
 * This is about practicing writing for a public audience. The more you write the better you'll get. 
@@ -174,37 +155,135 @@
     <t>Data Analytics Lifecycle: Model (Basics)</t>
   </si>
   <si>
-    <t>Data Analytics Lifecycle: Model (Building)</t>
-  </si>
-  <si>
-    <t>Data Analytics Lifecycle: Model (Validation)</t>
-  </si>
-  <si>
-    <t>* Partition a data set into training and testing sets. 
-* Fit models using cross-validation techniques</t>
-  </si>
-  <si>
-    <t>Supervised Machine Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Fit a variety of supervised machine learning models. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Your blog post this week should revolve around Supervised ML methods. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* What's the difference between Supervised vs Unsupervised models? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* More discussion on the differnece and use of training and testing data. 
-* How do we implement a cross-validation procedure? </t>
+    <t>Introduction to Statistical Learning</t>
+  </si>
+  <si>
+    <t>* Follow the tutorials provided to build your website using blogdown. Minimum information includes an 'about' paragraph. (Due Mon 2/5)
+* Edit your pinned slack introduction message to include the link to your website.
+* Tell us a little bit about your DS sources (blog/podcast/twitter) in #state-of-ds.  (Due Mon 2/5)</t>
+  </si>
+  <si>
+    <t>R4DS #1</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>PR R4DS #1</t>
+  </si>
+  <si>
+    <t>Peer Review</t>
+  </si>
+  <si>
+    <t>Blogdown</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t>Find Blogs</t>
+  </si>
+  <si>
+    <t>Gapminder</t>
+  </si>
+  <si>
+    <t>PR Gapminder</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>* Join all visible Slack channels. 
+* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. (Due Tue 1/23)
+* R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
+* Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)</t>
+  </si>
+  <si>
+    <t>* ISLR MOOC [Video lectures](http://www.dataschool.io/15-hours-of-expert-machine-learning-videos/)
+* [Materials from DSO/IOM 530 at USC](https://www.alsharif.info/iom530)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* We're going to use the textbook "Introduction to Statistical Learning" - a leading book in the field to lead us through an introduction to the world of machine learning. 
+* There will also be associated videos for you to watch as well from the textbook authors. 
+* The slides linked in the reference section are from an offering of a ML class at USC using this book. Consider them another learning tool. 
+* Rememer, for much of this class i'm a guide on the side. Pointing you at things to learn, giving you the space and support to learn it. Others have explained the material much better than I could, so let's let them deliver the lecture content and I'll provide the support. 
+* This means that you'll have to spend some dedicated time reading the textbook. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Download the [PDF of ISLR](http://www-bcf.usc.edu/~gareth/ISL/)
+* Watch ISLR Videos: Ch 1 &amp; 2
+* Read ISLR Ch 1 &amp; CH 2
+* Be prepared to answer questions during class. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What is f? 
+* Examples of supervised/unsupervised, regression/clustering/classification, parametric/non-parametric models. 
+* Why would we ever choose to use a more restrictive method instead of a very flexible approach?
+* What is the primary measure of model fit for regression models? 
+* What's the difference between training and testing data? Why do we need both? 
+* What is overfitting? 
+* If we don't have a testing data set, what method can we use to estimate the MSE of the testing data? 
+* What is the bias-variance tradeoff? 
+* What is the primary measure of model fit for classification models? 
+* Name two classification models 
+* Name a benefit of using a KNN model. 
+* What happens to the accuracy/bias of the model as the K increases? Why? </t>
+  </si>
+  <si>
+    <t>* R4DS HW #2:  23.2.1 (#1, #2) , 23.3.3 (#1, #3, #4),  23.4.5 (#1, #3, #4). Add this assignment to your github repo as a new RMD file. (Due Sat 2/17)
+* Peer Review R4DS HW #2 (Due Mon 2/19)</t>
+  </si>
+  <si>
+    <t>* Using the gapminder data set, explore the question "How does life expectancy change over time for each country?"  Automate your entire workflow including data acquisition as a separate R file.  Write a tutorial/walk through as a separate RMD file. (Due Sat 2/10)
+* Peer review 1 classmates file using github (Due Mon 2/12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* ISLR Chapter 2 Exercises: #1, #2, #4 (Write this up as a blog post), #10 Explore the Boston data set. Write this up as a separate assignment in your github repo. (Due Sat 2/24)
+* Peer review Boston exploration via forking &amp; writing issues in github. (Due Mon 2/25)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Describe the difference between training and testing data sets
+* Describe the differnece between a parametric and non-parametric model
+* Identify  and describe situations where classification, regression, and clustering models are appropriate. 
+* Explain the concept of overfitting, and bias-variance tradeoff. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Everything starts with linear regression, and then moves outward. 
+* In 315/456 we cared more about interpreting models and understanding the effects covariates had on outcomes. Here we're more interested in using the models to make predictions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Under what circumstances will the parametric approach outperform a non-parametric approach? 
+* What is the curse of dimensionality? </t>
+  </si>
+  <si>
+    <t>* ISLR Chapter 3 Exercises: #4,  #15 (Due Sat 3/3)
+* Peer review via github (Due Mon3/5)</t>
+  </si>
+  <si>
+    <t>* Read ISLR Chapter 3.5</t>
+  </si>
+  <si>
+    <t>Prediction using Regression Models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -254,8 +333,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,8 +373,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -338,8 +430,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,8 +537,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -484,8 +592,21 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="90" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="6" borderId="4" xfId="90" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="91">
+    <cellStyle name="Calculation" xfId="90" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -920,8 +1041,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -929,10 +1050,10 @@
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="2" width="12.625" customWidth="1"/>
     <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="38.25" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.75" style="5" customWidth="1"/>
     <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="39.75" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.25" style="5" customWidth="1"/>
+    <col min="8" max="8" width="41.25" style="5" customWidth="1"/>
     <col min="9" max="9" width="30.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -973,23 +1094,23 @@
         <v>41661</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,16 +1131,16 @@
         <v>10</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1031,23 +1152,23 @@
         <v>41675</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1059,25 +1180,25 @@
         <v>41682</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -1085,15 +1206,25 @@
         <v>41689</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="I6" s="4" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1105,20 +1236,24 @@
         <v>41696</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1126,21 +1261,13 @@
         <f t="shared" si="0"/>
         <v>41703</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -1300,4 +1427,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BCBD9-52BC-4762-BCE3-C0E2C27CCA7A}">
+  <dimension ref="B3:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" style="18" customWidth="1"/>
+    <col min="4" max="4" width="10.375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="19">
+        <v>41667</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="19">
+        <v>41669</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="19">
+        <v>41674</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="18">
+        <v>2</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="19">
+        <v>41674</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="19">
+        <v>41681</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="18">
+        <v>4</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="19">
+        <v>41683</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add up to wk 8 and rebulid
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
   <si>
     <t>Finals Week</t>
   </si>
@@ -86,11 +86,6 @@
     <t>Version Control with git, Team collaboration with slack, Intermediate R Programming concepts.</t>
   </si>
   <si>
-    <t>* [Blogdown](https://bookdown.org/yihui/blogdown/)
-* [Alice Hills Tutorial](https://alison.rbind.io/post/up-and-running-with-blogdown/)
-* [Curation vs Creation](https://www.agorapulse.com/blog/lets-clear-content-creation-vs-content-curation)</t>
-  </si>
-  <si>
     <t>* Review the [notes](notes.html) on the data analytics lifecycle
 * Review the notes from [Stat 545](http://stat545.com/automation01_slides/index.html) on automation</t>
   </si>
@@ -143,12 +138,6 @@
 * Most homework will be submitted through this repo. Direct links to the *.md file that you want me to review will be submitted via BBL for easy gradebook entry. </t>
   </si>
   <si>
-    <t xml:space="preserve">* You're going to use Hugo/Blogdown to create a professional looking website. 
-* Each week you will write a post about something in the DS world that you found interesting. It doesn't have to be a long or involved post.
-* This is about practicing writing for a public audience. The more you write the better you'll get. 
-* Wait.. why the heck should I create a website? The internet is scary! </t>
-  </si>
-  <si>
     <t>Data Analytics Lifecycle: Get, Clean, Explore. Then automate all the things!</t>
   </si>
   <si>
@@ -169,27 +158,12 @@
     <t>Assignment</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Due</t>
-  </si>
-  <si>
     <t>PR R4DS #1</t>
   </si>
   <si>
-    <t>Peer Review</t>
-  </si>
-  <si>
-    <t>Blogdown</t>
-  </si>
-  <si>
     <t>Discussion</t>
   </si>
   <si>
-    <t>Find Blogs</t>
-  </si>
-  <si>
     <t>Gapminder</t>
   </si>
   <si>
@@ -197,9 +171,6 @@
   </si>
   <si>
     <t>Project</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>%</t>
@@ -269,21 +240,133 @@
 * What is the curse of dimensionality? </t>
   </si>
   <si>
+    <t>* Read ISLR Chapter 3.5</t>
+  </si>
+  <si>
+    <t>Prediction using Regression Models</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>* Read ISLR Chapter 4 (Intro), 4.1, 4.35, 4.4, 4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What are the three most widely used classifying models? What is the fourth one this chapter talks about? 
+* When would we choose a linear discriminant analysis model over logistic regression? 
+* Briefly explain how a LDA works. What is linear about it? 
+* What is the table at the top of 145 called? 
+* What is one reason the example model on the `default` data had such low sensitivity? How was it improved? 
+* What's the difference bewtween LDA and QDA? When would we choose one over the other? 
+* What patterns are you seeing / what are the take home messages from figure 4.10 &amp; 4.11? </t>
+  </si>
+  <si>
+    <t>Read through the lab (ISLR 4.6) and replicate on your own.</t>
+  </si>
+  <si>
     <t>* ISLR Chapter 3 Exercises: #4,  #15 (Due Sat 3/3)
-* Peer review via github (Due Mon3/5)</t>
-  </si>
-  <si>
-    <t>* Read ISLR Chapter 3.5</t>
-  </si>
-  <si>
-    <t>Prediction using Regression Models</t>
+* Peer review via github (Due Mon 3/5)</t>
+  </si>
+  <si>
+    <t>* ISLR Chapter 4 Exercises: #5,  # 13 (Due Sat 3/10)
+* Peer Review via Github (Due Mon 3/12)</t>
+  </si>
+  <si>
+    <t>* Implement each of four commonly used classifying models. 
+* Explain a situation where a classification model is warrented
+* Identify the best model from a group of competing models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Create and evaluate a prediction model using linear regression. 
+* Identify cases where a non-parametric approach would be more appropriate than a parametric approach. </t>
+  </si>
+  <si>
+    <t>Catgory</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Create website</t>
+  </si>
+  <si>
+    <t>R4DS #2</t>
+  </si>
+  <si>
+    <t>PR R4DS #2</t>
+  </si>
+  <si>
+    <t>ISLR Ch 2</t>
+  </si>
+  <si>
+    <t>PR ISLR Ch 2</t>
+  </si>
+  <si>
+    <t>Share Blogs</t>
+  </si>
+  <si>
+    <t>ISLR Ch 3</t>
+  </si>
+  <si>
+    <t>PR ISLR Ch 3</t>
+  </si>
+  <si>
+    <t>ISLR Ch 4</t>
+  </si>
+  <si>
+    <t>PR ISLR Ch 4</t>
+  </si>
+  <si>
+    <t>Blog Posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* You're going to use Hugo/Blogdown to create a professional looking website. 
+* Several times throughout the semester you will write a post about something in the DS world that you found interesting. It doesn't have to be a long or involved post.
+* This is about practicing writing for a public audience. The more you write the better you'll get. 
+* Wait.. why the heck should I create a website? The internet is scary! </t>
+  </si>
+  <si>
+    <t>Boston Project Dashboard</t>
+  </si>
+  <si>
+    <t>Dissemination and reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Plotly: https://plot.ly/r/ 
+* User Guide for R: https://plot.ly/r/user-guide/ </t>
+  </si>
+  <si>
+    <t>* Refresh on your Shiny skills. Probably update the package. 
+* Optional: Learn Plotly. Note, it's stand alone but there are instructions on how to use it with R</t>
+  </si>
+  <si>
+    <t>* Convey results of the prediction model back to a non-technical audience
+ * Integrate projects into your webpage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Take one of the last two assignments on creating prediction models using the Boston data set, address any peer feedback and turn into dynamic prediction model using Shiny. 
+* Create a dashboard for prediction 
+* Allow the user to see predictions for different covariate patterns. 
+* Add some interactiveness to your app using Plotly
+* Add as a project to personal webpage. 
+</t>
+  </si>
+  <si>
+    <t>* Dashboard Project (Due Friday 3/30)</t>
+  </si>
+  <si>
+    <t>* [Blogdown](https://bookdown.org/yihui/blogdown/)
+* [Curation vs Creation](https://www.agorapulse.com/blog/lets-clear-content-creation-vs-content-curation)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -334,15 +417,30 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,13 +471,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -431,22 +524,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -537,9 +635,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -595,18 +695,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="90" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="6" borderId="4" xfId="90" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="90" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="92" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="91">
-    <cellStyle name="Calculation" xfId="90" builtinId="22"/>
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -650,6 +764,7 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 2" xfId="91" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -696,7 +811,9 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Percent" xfId="90" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1041,8 +1158,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1100,20 +1217,20 @@
         <v>8</v>
       </c>
       <c r="E2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1131,16 +1248,16 @@
         <v>10</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1152,23 +1269,23 @@
         <v>41675</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1180,21 +1297,21 @@
         <v>41682</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1206,29 +1323,29 @@
         <v>41689</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
       <c r="B7" s="3">
@@ -1236,54 +1353,80 @@
         <v>41696</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    </row>
+    <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>41703</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="G8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>41710</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="C9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
@@ -1309,7 +1452,9 @@
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -1431,142 +1576,838 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BCBD9-52BC-4762-BCE3-C0E2C27CCA7A}">
-  <dimension ref="B3:J10"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9" style="18"/>
+    <col min="1" max="1" width="9" style="25"/>
+    <col min="2" max="2" width="32.25" style="25" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="9" style="25"/>
+    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="10" style="18" customWidth="1"/>
+    <col min="8" max="8" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="18" t="s">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="18">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="18">
+        <f>SUMIF($C$2:$C$84,F2,$D$2:$D$84)</f>
+        <v>70</v>
+      </c>
+      <c r="H2" s="21">
+        <f>G2/$G$6</f>
+        <v>0.34825870646766172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="18">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="18">
+        <f>SUMIF($C$2:$C$84,F3,$D$2:$D$84)</f>
+        <v>51</v>
+      </c>
+      <c r="H3" s="21">
+        <f>G3/$G$6</f>
+        <v>0.2537313432835821</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="18">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="18">
+        <f>SUMIF($C$2:$C$84,F4,$D$2:$D$84)</f>
+        <v>30</v>
+      </c>
+      <c r="H4" s="21">
+        <f>G4/$G$6</f>
+        <v>0.14925373134328357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="18">
+        <f>SUMIF($C$2:$C$84,F5,$D$2:$D$84)</f>
+        <v>50</v>
+      </c>
+      <c r="H5" s="21">
+        <f>G5/$G$6</f>
+        <v>0.24875621890547264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="20" t="s">
+      <c r="C6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="18">
+        <v>10</v>
+      </c>
+      <c r="G6" s="22">
+        <f>SUM(G2:G5)</f>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>4</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>5</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="18">
+        <v>5</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="18">
+        <v>10</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>6</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="18">
+        <v>5</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>7</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="18">
+        <v>10</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>7</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="18">
+        <v>5</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="18">
-        <v>1</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="19">
-        <v>41667</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
-        <v>2</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="D16" s="18">
+        <v>50</v>
+      </c>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="19">
-        <v>41669</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="18">
-        <v>2</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="19">
-        <v>41674</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="18">
-        <v>2</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="19">
-        <v>41674</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="18">
-        <v>3</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="19">
-        <v>41681</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18">
-        <v>4</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="19">
-        <v>41683</v>
-      </c>
+      <c r="D17" s="18">
+        <v>50</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="23"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="23"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="23"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="23"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="23"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="23"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="23"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="23"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="23"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="23"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="23"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="23"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="23"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="23"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="23"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="26"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="26"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="23"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="23"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="23"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="23"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="23"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="23"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="24"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="24"/>
+      <c r="G79"/>
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="24"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="G81"/>
+      <c r="H81"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
+      <c r="G82"/>
+      <c r="H82"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="G83"/>
+      <c r="H83"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
+      <c r="G84"/>
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="27"/>
+      <c r="G85"/>
+      <c r="H85"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="G86"/>
+      <c r="H86"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="G87"/>
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="G88"/>
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="28"/>
+      <c r="B93" s="28"/>
+      <c r="D93" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add external notes on classifiers
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>Finals Week</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Topics</t>
-  </si>
-  <si>
-    <t>Social Media for Academics</t>
   </si>
   <si>
     <t xml:space="preserve">* Be familiar with modern team collaboration and version control tools 
@@ -358,8 +355,67 @@
     <t>* Dashboard Project (Due Friday 3/30)</t>
   </si>
   <si>
+    <t>Final Project</t>
+  </si>
+  <si>
     <t>* [Blogdown](https://bookdown.org/yihui/blogdown/)
-* [Curation vs Creation](https://www.agorapulse.com/blog/lets-clear-content-creation-vs-content-curation)</t>
+* [Curation vs Creation](https://www.agorapulse.com/blog/lets-clear-content-creation-vs-content-curation)
+* http://varianceexplained.org/r/start-blog/</t>
+  </si>
+  <si>
+    <t>Social Media for Data Scientists</t>
+  </si>
+  <si>
+    <t>Dead Week</t>
+  </si>
+  <si>
+    <t>Ethics of ML algorithms, Resampling Methods</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 3-4 (MB)</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 5-6 (AS)</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 7-8 (RA)</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 9-10 (RAD)</t>
+  </si>
+  <si>
+    <t>Tree based methods</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Intro, Ch 1-2 (RAD)
+* ISLR Chapter 5
+* Install the caret package</t>
+  </si>
+  <si>
+    <t>* Describe how the bootstratp method differs from cross-validation
+* Implement cross-validation technique to assess model performance</t>
+  </si>
+  <si>
+    <t>*https://cran.r-project.org/web/packages/caret/vignettes/caret.pdf
+* https://topepo.github.io/caret/
+* Notes from [[MATH 456 S16]](notes/lec10_Classifiers_456_S16.pdf)</t>
+  </si>
+  <si>
+    <t>* Name one reason resampling techniques are used in statistical learning
+* Describe the overall or general process of model validation
+* What are the two primary methods of cross-validation? 
+* Which method above is nearly unbaiased? Why?
+* What is the primary driver of the bias-variance tradeoff in cross-validation? 
+* Describe how the bootstrap method differs from cross-validation</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>Other Tools</t>
+  </si>
+  <si>
+    <t>Parallel processing, batch jobs</t>
   </si>
 </sst>
 </file>
@@ -455,12 +511,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -468,6 +518,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,21 +718,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="89" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -686,10 +727,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -718,6 +759,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1158,8 +1214,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1175,13 +1231,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1190,190 +1246,190 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>14</v>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>41661</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
-        <v>38</v>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>41668</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>29</v>
+      <c r="G3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <f t="shared" si="0"/>
         <v>41675</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14" t="s">
-        <v>44</v>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>41682</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
+      <c r="C5" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>41689</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>28</v>
+      <c r="C6" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>41696</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>50</v>
+      <c r="C7" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="3">
@@ -1381,27 +1437,27 @@
         <v>41703</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="3">
@@ -1409,54 +1465,64 @@
         <v>41710</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="G9" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>41724</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="C11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1464,9 +1530,13 @@
         <f t="shared" si="0"/>
         <v>41731</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
@@ -1480,15 +1550,19 @@
         <f t="shared" si="0"/>
         <v>41738</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1496,9 +1570,13 @@
         <f t="shared" si="0"/>
         <v>41745</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
@@ -1512,9 +1590,13 @@
         <f t="shared" si="0"/>
         <v>41752</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4"/>
@@ -1528,7 +1610,9 @@
         <f t="shared" si="0"/>
         <v>41759</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
@@ -1544,7 +1628,9 @@
         <f t="shared" si="0"/>
         <v>41766</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
@@ -1579,837 +1665,848 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="25"/>
-    <col min="2" max="2" width="32.25" style="25" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="9" style="25"/>
+    <col min="1" max="1" width="9" style="20"/>
+    <col min="2" max="2" width="32.25" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9" style="20"/>
     <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="10" style="18" customWidth="1"/>
-    <col min="8" max="8" width="9" style="18"/>
+    <col min="7" max="7" width="10" style="13" customWidth="1"/>
+    <col min="8" max="8" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>37</v>
+      <c r="H1" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="18">
+      <c r="D2" s="13">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="18">
+        <v>30</v>
+      </c>
+      <c r="G2" s="13">
         <f>SUMIF($C$2:$C$84,F2,$D$2:$D$84)</f>
         <v>70</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="16">
         <f>G2/$G$6</f>
-        <v>0.34825870646766172</v>
+        <v>0.2788844621513944</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="13">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="18">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="G3" s="13">
         <f>SUMIF($C$2:$C$84,F3,$D$2:$D$84)</f>
         <v>51</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="16">
         <f>G3/$G$6</f>
-        <v>0.2537313432835821</v>
+        <v>0.20318725099601595</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="18">
+      <c r="B4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="13">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="18">
+        <v>60</v>
+      </c>
+      <c r="G4" s="13">
         <f>SUMIF($C$2:$C$84,F4,$D$2:$D$84)</f>
         <v>30</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="16">
         <f>G4/$G$6</f>
-        <v>0.14925373134328357</v>
+        <v>0.11952191235059761</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="13">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="13">
+        <f>SUMIF($C$2:$C$84,F5,$D$2:$D$84)</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="16">
+        <f>G5/$G$6</f>
+        <v>0.39840637450199201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="13">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17">
+        <f>SUM(G2:G5)</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>4</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>4</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="13">
+        <v>5</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>6</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="18">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="18">
-        <f>SUMIF($C$2:$C$84,F5,$D$2:$D$84)</f>
+      <c r="C12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="13">
+        <v>10</v>
+      </c>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="13">
+        <v>5</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>7</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="13">
+        <v>10</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>7</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="13">
+        <v>5</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>8</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="13">
         <v>50</v>
       </c>
-      <c r="H5" s="21">
-        <f>G5/$G$6</f>
-        <v>0.24875621890547264</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
-        <v>3</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="18">
-        <v>10</v>
-      </c>
-      <c r="G6" s="22">
-        <f>SUM(G2:G5)</f>
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>3</v>
-      </c>
-      <c r="B7" s="18" t="s">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="13">
+        <v>50</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>4</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>4</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
-        <v>5</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
-        <v>5</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="18">
-        <v>5</v>
-      </c>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>6</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="18">
-        <v>10</v>
-      </c>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
-        <v>6</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="18">
-        <v>5</v>
-      </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
-        <v>7</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="18">
-        <v>10</v>
-      </c>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
-        <v>7</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="18">
-        <v>5</v>
-      </c>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
-        <v>15</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="D18" s="13">
         <v>50</v>
       </c>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
-        <v>8</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="18">
-        <v>50</v>
-      </c>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="23"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="23"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="23"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="23"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="23"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="23"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="18"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="23"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="23"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="23"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="18"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="23"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="18"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="23"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="18"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="23"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="18"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="23"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="23"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="18"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="23"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="23"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="18"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="23"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="18"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="23"/>
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="18"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="26"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="21"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="26"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="21"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="23"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="18"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="23"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="18"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="23"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="18"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="23"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="18"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="23"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="18"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="23"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="18"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
+      <c r="A72" s="22"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
+      <c r="A75" s="22"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="24"/>
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="19"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="27"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="24"/>
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="19"/>
       <c r="G79"/>
       <c r="H79"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="24"/>
+      <c r="A80" s="22"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="19"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
       <c r="G81"/>
       <c r="H81"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
       <c r="G82"/>
       <c r="H82"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
       <c r="G83"/>
       <c r="H83"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
       <c r="G84"/>
       <c r="H84"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
+      <c r="A85" s="22"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
       <c r="G85"/>
       <c r="H85"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="27"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
+      <c r="A86" s="22"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
       <c r="G86"/>
       <c r="H86"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
-      <c r="B87" s="27"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
+      <c r="A87" s="22"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
       <c r="G87"/>
       <c r="H87"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
+      <c r="A88" s="22"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
       <c r="G88"/>
       <c r="H88"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
+      <c r="A89" s="22"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
-      <c r="B90" s="27"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
+      <c r="A90" s="22"/>
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="27"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
+      <c r="A91" s="22"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="27"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
+      <c r="A92" s="22"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
-      <c r="B93" s="28"/>
-      <c r="D93" s="28"/>
+      <c r="A93" s="23"/>
+      <c r="B93" s="23"/>
+      <c r="D93" s="23"/>
     </row>
   </sheetData>
+  <sortState ref="A2:D93">
+    <sortCondition ref="A2:A93"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add syllabus and textbook. rebuild
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
   <si>
     <t>Finals Week</t>
   </si>
@@ -372,18 +372,6 @@
     <t>Ethics of ML algorithms, Resampling Methods</t>
   </si>
   <si>
-    <t>* Read WOMD: Ch 3-4 (MB)</t>
-  </si>
-  <si>
-    <t>* Read WOMD: Ch 5-6 (AS)</t>
-  </si>
-  <si>
-    <t>* Read WOMD: Ch 7-8 (RA)</t>
-  </si>
-  <si>
-    <t>* Read WOMD: Ch 9-10 (RAD)</t>
-  </si>
-  <si>
     <t>Tree based methods</t>
   </si>
   <si>
@@ -415,7 +403,57 @@
     <t>Other Tools</t>
   </si>
   <si>
-    <t>Parallel processing, batch jobs</t>
+    <t>* Read WOMD: Ch 3-4 (MB)
+* [When Data Science Destabilizes Democracy and Facilitates Genocide](http://www.fast.ai/2017/11/02/ethics/)</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 5-6 (AS)
+* [More than a Million Pro-Repeal Net Neutrality Comments were Likely Faked](https://hackernoon.com/more-than-a-million-pro-repeal-net-neutrality-comments-were-likely-faked-e9f0e3ed36a6)</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 7-8 (RA)
+* [Activision Patents Matchmaking That Encourages Players To Buy Microtransactions](https://kotaku.com/activision-patents-matchmaking-that-encourages-players-1819630937)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 9-10 (RAD)
+* Compare [[this article on practical tips for success with ML]](https://www.datanami.com/2018/01/17/practical-tips-success-machine-learning/) with this post on [[google automating ML]](https://www.datanami.com/2018/01/17/google-automate-machine-learning-automl-service/)</t>
+  </si>
+  <si>
+    <t>* ML homework</t>
+  </si>
+  <si>
+    <t>* Big data homework</t>
+  </si>
+  <si>
+    <t>Working on a computing cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Write a script to send to a remote server to perform an analysis. 
+* Write a script that utilizes more than one computing core. </t>
+  </si>
+  <si>
+    <t>* cluster computing homework</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>PR ML</t>
+  </si>
+  <si>
+    <t>Big data</t>
+  </si>
+  <si>
+    <t>PR big data</t>
+  </si>
+  <si>
+    <t>cluster computing</t>
+  </si>
+  <si>
+    <t>PR Cluster computing</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1252,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1506,23 +1544,23 @@
         <v>84</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1531,18 +1569,20 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1551,18 +1591,20 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1571,18 +1613,22 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="E14" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1591,11 +1637,11 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
@@ -1614,7 +1660,9 @@
         <v>80</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4"/>
@@ -1665,7 +1713,7 @@
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1721,11 +1769,11 @@
       </c>
       <c r="G2" s="13">
         <f>SUMIF($C$2:$C$84,F2,$D$2:$D$84)</f>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H2" s="16">
         <f>G2/$G$6</f>
-        <v>0.2788844621513944</v>
+        <v>0.33783783783783783</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1750,7 +1798,7 @@
       </c>
       <c r="H3" s="16">
         <f>G3/$G$6</f>
-        <v>0.20318725099601595</v>
+        <v>0.17229729729729729</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,11 +1819,11 @@
       </c>
       <c r="G4" s="13">
         <f>SUMIF($C$2:$C$84,F4,$D$2:$D$84)</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H4" s="16">
         <f>G4/$G$6</f>
-        <v>0.11952191235059761</v>
+        <v>0.15202702702702703</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1800,7 +1848,7 @@
       </c>
       <c r="H5" s="16">
         <f>G5/$G$6</f>
-        <v>0.39840637450199201</v>
+        <v>0.33783783783783783</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1818,7 +1866,7 @@
       </c>
       <c r="G6" s="17">
         <f>SUM(G2:G5)</f>
-        <v>251</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1969,71 +2017,119 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" s="13">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
+        <v>10</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="13">
+        <v>5</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>11</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="13">
+        <v>10</v>
+      </c>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>11</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="13">
+        <v>5</v>
+      </c>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>12</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>12</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>15</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>16</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C24" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D24" s="13">
         <v>50</v>
       </c>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>

</xml_diff>

<commit_message>
add reading to week 1, upd schedule
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/ADS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="109">
   <si>
     <t>Finals Week</t>
   </si>
@@ -171,12 +171,6 @@
   </si>
   <si>
     <t>%</t>
-  </si>
-  <si>
-    <t>* Join all visible Slack channels. 
-* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. (Due Tue 1/23)
-* R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
-* Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)</t>
   </si>
   <si>
     <t>* ISLR MOOC [Video lectures](http://www.dataschool.io/15-hours-of-expert-machine-learning-videos/)
@@ -455,11 +449,24 @@
   <si>
     <t>PR Cluster computing</t>
   </si>
+  <si>
+    <t xml:space="preserve">* Describe your Data Scientist profile. What are your strengths? 
+* Using the [Data Camp infographic](https://www.datacamp.com/community/tutorials/data-science-industry-infographic) - Where do you see yourself fitting in ?
+* How would you explain to someone what "Big Data" is? 
+* How would you explain to someone what a model is? </t>
+  </si>
+  <si>
+    <t>* Join all visible Slack channels. 
+* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. (Due Tue 1/23)
+* R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
+* Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)
+* Be prepared to answer DDS topic questions in class next Tuesday.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -904,9 +911,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Percent" xfId="90" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
     <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1248,27 +1255,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="39.75" style="5" customWidth="1"/>
-    <col min="8" max="8" width="41.25" style="5" customWidth="1"/>
-    <col min="9" max="9" width="30.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="39.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="41.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="313" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1319,12 +1326,14 @@
       <c r="G2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="I2" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1333,7 +1342,7 @@
         <v>41668</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
@@ -1342,13 +1351,13 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>28</v>
@@ -1379,10 +1388,10 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="170" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1405,7 +1414,7 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1420,25 +1429,25 @@
         <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1447,26 +1456,26 @@
         <v>41696</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="196" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1475,26 +1484,26 @@
         <v>41703</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1503,26 +1512,26 @@
         <v>41710</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="G9" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="25"/>
       <c r="C10" s="24"/>
@@ -1533,7 +1542,7 @@
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="144" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1541,26 +1550,26 @@
         <v>41724</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="66" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1569,20 +1578,20 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="92" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1591,20 +1600,20 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="79" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1613,22 +1622,22 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1637,18 +1646,18 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1657,18 +1666,18 @@
         <v>41759</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1677,7 +1686,7 @@
         <v>41766</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1686,7 +1695,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1709,23 +1718,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39BCBD9-52BC-4762-BCE3-C0E2C27CCA7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="20"/>
-    <col min="2" max="2" width="32.25" style="20" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9" style="20"/>
-    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="20"/>
+    <col min="2" max="2" width="32.1640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="20"/>
+    <col min="5" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="13" customWidth="1"/>
-    <col min="8" max="8" width="9" style="13"/>
+    <col min="8" max="8" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1736,16 +1745,16 @@
         <v>30</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="F1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>36</v>
@@ -1776,7 +1785,7 @@
         <v>0.33783783783783783</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="13">
         <v>5</v>
@@ -1801,12 +1810,12 @@
         <v>0.17229729729729729</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>30</v>
@@ -1815,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="13">
         <f>SUMIF($C$2:$C$84,F4,$D$2:$D$84)</f>
@@ -1826,12 +1835,12 @@
         <v>0.15202702702702703</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>32</v>
@@ -1851,7 +1860,7 @@
         <v>0.33783783783783783</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>3</v>
       </c>
@@ -1869,7 +1878,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>3</v>
       </c>
@@ -1877,18 +1886,18 @@
         <v>34</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>30</v>
@@ -1897,26 +1906,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>30</v>
@@ -1925,27 +1934,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>5</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="13">
         <v>5</v>
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>6</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>30</v>
@@ -1955,27 +1964,27 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>6</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="13">
         <v>5</v>
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>7</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>30</v>
@@ -1985,27 +1994,27 @@
       </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>7</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="13">
         <v>5</v>
       </c>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>8</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>35</v>
@@ -2015,12 +2024,12 @@
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>10</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>30</v>
@@ -2030,27 +2039,27 @@
       </c>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>10</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="13">
         <v>5</v>
       </c>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>11</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>30</v>
@@ -2060,27 +2069,27 @@
       </c>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>11</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="13">
         <v>5</v>
       </c>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>12</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>30</v>
@@ -2089,26 +2098,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <v>12</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>15</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>32</v>
@@ -2117,12 +2126,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>16</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>35</v>
@@ -2131,247 +2140,247 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="18"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="18"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="18"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="18"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="18"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="18"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
       <c r="E60" s="18"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
       <c r="E61" s="18"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -2381,7 +2390,7 @@
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -2391,106 +2400,106 @@
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="21"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="21"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="18"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
       <c r="E67" s="18"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="18"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
       <c r="E69" s="18"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="18"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="18"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="22"/>
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="22"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="22"/>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="22"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
       <c r="D75" s="22"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="22"/>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
       <c r="D76" s="22"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="22"/>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="22"/>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
       <c r="D78" s="22"/>
       <c r="E78" s="19"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="22"/>
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
@@ -2499,14 +2508,14 @@
       <c r="G79"/>
       <c r="H79"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
       <c r="D80" s="22"/>
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="22"/>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
@@ -2514,7 +2523,7 @@
       <c r="G81"/>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
@@ -2522,7 +2531,7 @@
       <c r="G82"/>
       <c r="H82"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="22"/>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
@@ -2530,7 +2539,7 @@
       <c r="G83"/>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="22"/>
       <c r="B84" s="22"/>
       <c r="C84" s="22"/>
@@ -2538,7 +2547,7 @@
       <c r="G84"/>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="22"/>
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
@@ -2546,7 +2555,7 @@
       <c r="G85"/>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="22"/>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
@@ -2554,7 +2563,7 @@
       <c r="G86"/>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="22"/>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
@@ -2562,7 +2571,7 @@
       <c r="G87"/>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="22"/>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
@@ -2570,31 +2579,31 @@
       <c r="G88"/>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="22"/>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
       <c r="D89" s="22"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="22"/>
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
       <c r="D90" s="22"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="22"/>
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
       <c r="D91" s="22"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="22"/>
       <c r="B92" s="22"/>
       <c r="C92" s="22"/>
       <c r="D92" s="22"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="23"/>
       <c r="B93" s="23"/>
       <c r="D93" s="23"/>

</xml_diff>

<commit_message>
update schedule and wk4
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/ADS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38400" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
   <si>
     <t>Finals Week</t>
   </si>
@@ -71,20 +71,10 @@
     <t>Topic2</t>
   </si>
   <si>
-    <t xml:space="preserve">* You don't know what you don’t know.
-* We're going to explore the current world of DS by finding and following people in the world doing DS in an area that interests you. 
-* Find a data science, data visualization, data story, data SOMETHING blog, podcast, twitter feed (or two) to follow. You will be sharing stories weekly, so you may need to find more than one source if your first choice does not update frequently enough.
-</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
     <t>Version Control with git, Team collaboration with slack, Intermediate R Programming concepts.</t>
-  </si>
-  <si>
-    <t>* Review the [notes](notes.html) on the data analytics lifecycle
-* Review the notes from [Stat 545](http://stat545.com/automation01_slides/index.html) on automation</t>
   </si>
   <si>
     <t xml:space="preserve">* Create a reproducible data analytics workflow using a make file. 
@@ -98,9 +88,6 @@
 </t>
   </si>
   <si>
-    <t>* [R4DS CH 22-23](http://r4ds.had.co.nz/model-intro.html)</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Demonstrate a deeper understanding of the underworkings behind linear models. </t>
   </si>
   <si>
@@ -124,11 +111,6 @@
 * Get the textbook - [Weapons of Math Destruction](https://www.amazon.com/Weapons-Math-Destruction-Increases-Inequality/dp/0553418815). There is  1 copy available in the Library -- Someone go check this out for the semester and share! </t>
   </si>
   <si>
-    <t>* [HappygitwithR Ch 1-16](http://happygitwithr.com/)
-* GitHub assignment repo [link](https://classroom.github.com/a/5I9Qnnbl)
-* [R4DS CH 17-21.5](http://r4ds.had.co.nz/program-intro.html)</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Introduction and orientation to Slack and GitHub 
 * Take control of Assignment repo (link under materials). This provides you a repo and a starting template for your homework.
 * Practice your R programming skills by working through r4ds Ch 17-21.5
@@ -138,15 +120,7 @@
     <t>Data Analytics Lifecycle: Get, Clean, Explore. Then automate all the things!</t>
   </si>
   <si>
-    <t>Data Analytics Lifecycle: Model (Basics)</t>
-  </si>
-  <si>
     <t>Introduction to Statistical Learning</t>
-  </si>
-  <si>
-    <t>* Follow the tutorials provided to build your website using blogdown. Minimum information includes an 'about' paragraph. (Due Mon 2/5)
-* Edit your pinned slack introduction message to include the link to your website.
-* Tell us a little bit about your DS sources (blog/podcast/twitter) in #state-of-ds.  (Due Mon 2/5)</t>
   </si>
   <si>
     <t>R4DS #1</t>
@@ -208,10 +182,6 @@
 * Peer Review R4DS HW #2 (Due Mon 2/19)</t>
   </si>
   <si>
-    <t>* Using the gapminder data set, explore the question "How does life expectancy change over time for each country?"  Automate your entire workflow including data acquisition as a separate R file.  Write a tutorial/walk through as a separate RMD file. (Due Sat 2/10)
-* Peer review 1 classmates file using github (Due Mon 2/12)</t>
-  </si>
-  <si>
     <t xml:space="preserve">* ISLR Chapter 2 Exercises: #1, #2, #4 (Write this up as a blog post), #10 Explore the Boston data set. Write this up as a separate assignment in your github repo. (Due Sat 2/24)
 * Peer review Boston exploration via forking &amp; writing issues in github. (Due Mon 2/25)
 </t>
@@ -456,17 +426,66 @@
 * How would you explain to someone what a model is? </t>
   </si>
   <si>
-    <t>* Join all visible Slack channels. 
-* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. (Due Tue 1/23)
+    <t>Slack Introductions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Join all visible Slack channels. 
+* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. (Due Thu 1/25)
 * R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
+* Read DDS CH 1&amp; 2 (Due Tue 1/30) 
 * Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)
-* Be prepared to answer DDS topic questions in class next Tuesday.</t>
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* You don't know what you don’t know.
+* We're going to explore the current world of DS by finding and following people in the world doing DS in an area that interests you. 
+* Find a data science, data visualization, data story, data SOMETHING blog, podcast, twitter feed (or two) to follow. 
+* You are assigned to write at least 8 blog posts throughout the semester, so you may need to find more than one source if your first choice does not update frequently enough.
+* Discuss answers from Last week's reading from Doing Data Science
+</t>
+  </si>
+  <si>
+    <t>* [HappygitwithR Ch 1-16](http://happygitwithr.com/)
+* GitHub assignment repo [link](https://classroom.github.com/a/5I9Qnnbl)
+* [R4DS CH 17-21.5](http://r4ds.had.co.nz/program-intro.html)
+* Doing Data Science: Chapter 1-2</t>
+  </si>
+  <si>
+    <t>Data Analytics Lifecycle: Model (Basics), Algorithms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [R4DS CH 22-23](http://r4ds.had.co.nz/model-intro.html)
+</t>
+  </si>
+  <si>
+    <t>* DDS Chapter 3</t>
+  </si>
+  <si>
+    <t>* DDS Chapter 5</t>
+  </si>
+  <si>
+    <t>* DDS Ch 3 (Read 51-57, 80-81, 90-91, skim the rest.)</t>
+  </si>
+  <si>
+    <t>* Review the [notes](notes.html) on the data analytics lifecycle. (Recap from IDS)
+* Review the notes from [Stat 545](http://stat545.com/automation01_slides/index.html) on automation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Follow the tutorials provided to build your website using blogdown. Minimum information includes an 'about' paragraph. (Due Mon 2/5)
+* Edit your pinned slack introduction message to include the link to your website.
+* Tell us a little bit about your DS sources (blog/podcast/twitter) in #state-of-ds.  (Due Mon 2/5)
+* Skim the TOC of DDS and pick a case study you want to read (Ch 4-14) . Post your selection in #readings by (Sun 2/4). Be prepared to share an overview of this case study next Thursday. </t>
+  </si>
+  <si>
+    <t>* Using the gapminder data set, explore the question "How does life expectancy change over time for each country?"  Automate your entire workflow including data acquisition as a separate R file.  Write a tutorial/walk through as a separate RMD file. (Due Sat 2/10)
+* Peer review 1 classmates file using github (Due Mon 2/12)
+* Pick a new (to you) case study to share next thursday (Post in #readings by Sun 2/10).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -911,9 +930,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
     <cellStyle name="Percent" xfId="90" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
     <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1255,27 +1274,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="41.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="39.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="41.125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="30.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1292,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
@@ -1304,7 +1323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="313" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1312,28 +1331,28 @@
         <v>41661</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1342,7 +1361,7 @@
         <v>41668</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
@@ -1351,16 +1370,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1372,26 +1391,26 @@
         <v>41675</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="170" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1400,21 +1419,23 @@
         <v>41682</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1426,28 +1447,28 @@
         <v>41689</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1456,26 +1477,28 @@
         <v>41696</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="G7" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="196" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1484,26 +1507,28 @@
         <v>41703</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="G8" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1512,26 +1537,26 @@
         <v>41710</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
       <c r="B10" s="25"/>
       <c r="C10" s="24"/>
@@ -1542,7 +1567,7 @@
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" ht="144" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1550,26 +1575,26 @@
         <v>41724</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="66" thickBot="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1578,20 +1603,20 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="92" thickBot="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1600,20 +1625,20 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="79" thickBot="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1622,22 +1647,22 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="131" thickBot="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1646,18 +1671,18 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1666,18 +1691,18 @@
         <v>41759</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1686,7 +1711,7 @@
         <v>41766</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1695,7 +1720,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1718,23 +1743,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="20"/>
-    <col min="2" max="2" width="32.1640625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="20"/>
-    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="20"/>
+    <col min="2" max="2" width="32.125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="20"/>
+    <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="13" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="13"/>
+    <col min="8" max="8" width="8.875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1742,22 +1767,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1765,622 +1790,630 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="13">
-        <f>SUMIF($C$2:$C$84,F2,$D$2:$D$84)</f>
+        <f>SUMIF($C$2:$C$85,F2,$D$2:$D$85)</f>
         <v>100</v>
       </c>
       <c r="H2" s="16">
         <f>G2/$G$6</f>
-        <v>0.33783783783783783</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.33670033670033672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D3" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G3" s="13">
-        <f>SUMIF($C$2:$C$84,F3,$D$2:$D$84)</f>
-        <v>51</v>
+        <f>SUMIF($C$2:$C$85,F3,$D$2:$D$85)</f>
+        <v>52</v>
       </c>
       <c r="H3" s="16">
         <f>G3/$G$6</f>
-        <v>0.17229729729729729</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.17508417508417509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D4" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G4" s="13">
-        <f>SUMIF($C$2:$C$84,F4,$D$2:$D$84)</f>
+        <f>SUMIF($C$2:$C$85,F4,$D$2:$D$85)</f>
         <v>45</v>
       </c>
       <c r="H4" s="16">
         <f>G4/$G$6</f>
-        <v>0.15202702702702703</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.15151515151515152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D5" s="13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G5" s="13">
-        <f>SUMIF($C$2:$C$84,F5,$D$2:$D$84)</f>
+        <f>SUMIF($C$2:$C$85,F5,$D$2:$D$85)</f>
         <v>100</v>
       </c>
       <c r="H5" s="16">
         <f>G5/$G$6</f>
-        <v>0.33783783783783783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0.33670033670033672</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G6" s="17">
         <f>SUM(G2:G5)</f>
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D7" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>3</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
-        <v>4</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D9" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>4</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
-        <v>5</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>5</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D11" s="13">
+        <v>10</v>
+      </c>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>5</v>
       </c>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
-        <v>6</v>
-      </c>
       <c r="B12" s="13" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D12" s="13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>6</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D13" s="13">
+        <v>10</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>6</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="13">
         <v>5</v>
       </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
-        <v>7</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="13">
-        <v>10</v>
-      </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>7</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D15" s="13">
+        <v>10</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>7</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="13">
         <v>5</v>
       </c>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="13">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <v>8</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="13">
+      <c r="B17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="13">
         <v>50</v>
       </c>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="13">
-        <v>10</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="13">
-        <v>10</v>
-      </c>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>10</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D18" s="13">
+        <v>10</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>10</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="13">
         <v>5</v>
       </c>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
-        <v>11</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="13">
-        <v>10</v>
-      </c>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>11</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D20" s="13">
+        <v>10</v>
+      </c>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>11</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="13">
         <v>5</v>
       </c>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="13">
-        <v>12</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>12</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D22" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>12</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>15</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
-        <v>16</v>
-      </c>
       <c r="B24" s="13" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D24" s="13">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>16</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="18"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="18"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="18"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="18"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="18"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="18"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
       <c r="E60" s="18"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
       <c r="E61" s="18"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -2390,7 +2423,7 @@
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -2400,106 +2433,106 @@
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="21"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="21"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="18"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
       <c r="E67" s="18"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="18"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
       <c r="E69" s="18"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="18"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="18"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="22"/>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="22"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
       <c r="D75" s="22"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
       <c r="D76" s="22"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="22"/>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="22"/>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
       <c r="D78" s="22"/>
       <c r="E78" s="19"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
@@ -2508,14 +2541,14 @@
       <c r="G79"/>
       <c r="H79"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
       <c r="D80" s="22"/>
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
@@ -2523,7 +2556,7 @@
       <c r="G81"/>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
@@ -2531,7 +2564,7 @@
       <c r="G82"/>
       <c r="H82"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
@@ -2539,7 +2572,7 @@
       <c r="G83"/>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="22"/>
       <c r="C84" s="22"/>
@@ -2547,7 +2580,7 @@
       <c r="G84"/>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
@@ -2555,7 +2588,7 @@
       <c r="G85"/>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
@@ -2563,7 +2596,7 @@
       <c r="G86"/>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
@@ -2571,7 +2604,7 @@
       <c r="G87"/>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="22"/>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
@@ -2579,38 +2612,44 @@
       <c r="G88"/>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="22"/>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
       <c r="D89" s="22"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="22"/>
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
       <c r="D90" s="22"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="22"/>
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
       <c r="D91" s="22"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
       <c r="B92" s="22"/>
       <c r="C92" s="22"/>
       <c r="D92" s="22"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="23"/>
-      <c r="B93" s="23"/>
-      <c r="D93" s="23"/>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="22"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="23"/>
+      <c r="B94" s="23"/>
+      <c r="D94" s="23"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D93">
-    <sortCondition ref="A2:A93"/>
+  <sortState ref="A2:D94">
+    <sortCondition ref="A2:A94"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bold due dates in schedule
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -178,15 +178,6 @@
 * What happens to the accuracy/bias of the model as the K increases? Why? </t>
   </si>
   <si>
-    <t>* R4DS HW #2:  23.2.1 (#1, #2) , 23.3.3 (#1, #3, #4),  23.4.5 (#1, #3, #4). Add this assignment to your github repo as a new RMD file. (Due Sat 2/17)
-* Peer Review R4DS HW #2 (Due Mon 2/19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* ISLR Chapter 2 Exercises: #1, #2, #4 (Write this up as a blog post), #10 Explore the Boston data set. Write this up as a separate assignment in your github repo. (Due Sat 2/24)
-* Peer review Boston exploration via forking &amp; writing issues in github. (Due Mon 2/25)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Describe the difference between training and testing data sets
 * Describe the differnece between a parametric and non-parametric model
 * Identify  and describe situations where classification, regression, and clustering models are appropriate. 
@@ -429,14 +420,6 @@
     <t>Slack Introductions</t>
   </si>
   <si>
-    <t xml:space="preserve">* Join all visible Slack channels. 
-* Introduce yourself in #introductions (Name/major/year/GitHub handle/other info you want to share). Pin this message to this board. (Due Thu 1/25)
-* R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
-* Read DDS CH 1&amp; 2 (Due Tue 1/30) 
-* Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">* You don't know what you don’t know.
 * We're going to explore the current world of DS by finding and following people in the world doing DS in an area that interests you. 
 * Find a data science, data visualization, data story, data SOMETHING blog, podcast, twitter feed (or two) to follow. 
@@ -473,13 +456,32 @@
   <si>
     <t xml:space="preserve">* Follow the tutorials provided to build your website using blogdown. Minimum information includes an 'about' paragraph. (Due Mon 2/5)
 * Edit your pinned slack introduction message to include the link to your website.
-* Tell us a little bit about your DS sources (blog/podcast/twitter) in #state-of-ds.  (Due Mon 2/5)
+* Tell us a little bit about your DS sources,  i.e. blog/podcast/twitter,  in #state-of-ds.  (Due Mon 2/5)
 * Skim the TOC of DDS and pick a case study you want to read (Ch 4-14) . Post your selection in #readings by (Sun 2/4). Be prepared to share an overview of this case study next Thursday. </t>
   </si>
   <si>
     <t>* Using the gapminder data set, explore the question "How does life expectancy change over time for each country?"  Automate your entire workflow including data acquisition as a separate R file.  Write a tutorial/walk through as a separate RMD file. (Due Sat 2/10)
 * Peer review 1 classmates file using github (Due Mon 2/12)
-* Pick a new (to you) case study to share next thursday (Post in #readings by Sun 2/10).</t>
+* Pick a new case study to share next thursday (Post in #readings by Sun 2/10).</t>
+  </si>
+  <si>
+    <t>* R4DS HW #2:  23.2.1 #1, #2 , 23.3.3 #1, #3, #4,  23.4.5 #1, #3, #4. Add this assignment to your github repo as a new RMD file. (Due Sat 2/17)
+* Peer Review R4DS HW #2 (Due Mon 2/19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* ISLR Ch2 Exercises: #1, #2 (Due Sat 2/24)
+* ISLR Ch 2 #4 Write this up as a blog post (Due Sat 2/24)
+* ISLR Ch 2 #10 Explore the Boston data set. Write this up as a separate assignment in your github repo. (Due Sat 2/24)
+* Peer review Boston exploration via forking &amp; writing issues in github. (Due Mon 2/25)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Join all visible Slack channels. 
+* Introduce yourself in #introductions. Include things like name/major/year/GitHub handle/other info you want to share. Pin this message to this board. (Due Thu 1/25)
+* R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
+* Read DDS CH 1&amp; 2 (Due Tue 1/30) 
+* Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)
+</t>
   </si>
 </sst>
 </file>
@@ -1277,9 +1279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1293,7 @@
     <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="39.625" style="5" customWidth="1"/>
     <col min="8" max="8" width="41.125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="30.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="35.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1340,19 +1342,19 @@
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1361,7 +1363,7 @@
         <v>41668</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
@@ -1370,16 +1372,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1397,7 +1399,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>17</v>
@@ -1407,7 +1409,7 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1419,23 +1421,23 @@
         <v>41682</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1450,7 +1452,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>33</v>
@@ -1465,7 +1467,7 @@
         <v>34</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1477,25 +1479,25 @@
         <v>41696</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
@@ -1507,25 +1509,25 @@
         <v>41703</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1537,23 +1539,23 @@
         <v>41710</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1575,23 +1577,23 @@
         <v>41724</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1603,17 +1605,17 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
@@ -1625,17 +1627,17 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1647,19 +1649,19 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1671,11 +1673,11 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
@@ -1691,11 +1693,11 @@
         <v>41759</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
@@ -1711,7 +1713,7 @@
         <v>41766</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1770,16 +1772,16 @@
         <v>24</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>30</v>
@@ -1790,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>26</v>
@@ -1843,13 +1845,13 @@
         <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="13">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G4" s="13">
         <f>SUMIF($C$2:$C$85,F4,$D$2:$D$85)</f>
@@ -1865,7 +1867,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>24</v>
@@ -1890,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>26</v>
@@ -1925,7 +1927,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="13">
         <v>5</v>
@@ -1936,7 +1938,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>24</v>
@@ -1950,10 +1952,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="13">
         <v>5</v>
@@ -1964,7 +1966,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>24</v>
@@ -1979,10 +1981,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" s="13">
         <v>5</v>
@@ -1994,7 +1996,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>24</v>
@@ -2009,10 +2011,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="13">
         <v>5</v>
@@ -2024,7 +2026,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>24</v>
@@ -2039,10 +2041,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="13">
         <v>5</v>
@@ -2054,7 +2056,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>29</v>
@@ -2069,7 +2071,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>24</v>
@@ -2084,10 +2086,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" s="13">
         <v>5</v>
@@ -2099,7 +2101,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>24</v>
@@ -2114,10 +2116,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="13">
         <v>5</v>
@@ -2128,7 +2130,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>24</v>
@@ -2142,10 +2144,10 @@
         <v>12</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D23" s="13">
         <v>5</v>
@@ -2156,7 +2158,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>26</v>
@@ -2170,7 +2172,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
update schedule, possibly bork repo
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,17 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="38400" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -216,14 +213,6 @@
     <t>Read through the lab (ISLR 4.6) and replicate on your own.</t>
   </si>
   <si>
-    <t>* ISLR Chapter 3 Exercises: #4,  #15 (Due Sat 3/3)
-* Peer review via github (Due Mon 3/5)</t>
-  </si>
-  <si>
-    <t>* ISLR Chapter 4 Exercises: #5,  # 13 (Due Sat 3/10)
-* Peer Review via Github (Due Mon 3/12)</t>
-  </si>
-  <si>
     <t>* Implement each of four commonly used classifying models. 
 * Explain a situation where a classification model is warrented
 * Identify the best model from a group of competing models</t>
@@ -469,13 +458,6 @@
 * Peer Review R4DS HW #2 (Due Mon 2/19)</t>
   </si>
   <si>
-    <t xml:space="preserve">* ISLR Ch2 Exercises: #1, #2 (Due Sat 2/24)
-* ISLR Ch 2 #4 Write this up as a blog post (Due Sat 2/24)
-* ISLR Ch 2 #10 Explore the Boston data set. Write this up as a separate assignment in your github repo. (Due Sat 2/24)
-* Peer review Boston exploration via forking &amp; writing issues in github. (Due Mon 2/25)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">* Join all visible Slack channels. 
 * Introduce yourself in #introductions. Include things like name/major/year/GitHub handle/other info you want to share. Pin this message to this board. (Due Thu 1/25)
 * R4DS HW #1 . Put a link in the #assignments channel when complete. (Due Mon 1/29)
@@ -483,11 +465,24 @@
 * Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">* ISLR Ch2 Exercises: #1, #2,  #4 (Write this up as a blog post), #10 (Due Mon 2/24)
+* Peer review Boston exploration via forking &amp; writing issues in github. (Due Wed 2/25)
+</t>
+  </si>
+  <si>
+    <t>* ISLR Chapter 3 Exercises: #4,  #15 (Due Mon 3/3)
+* Peer review via github (Due Wed 3/5)</t>
+  </si>
+  <si>
+    <t>* ISLR Chapter 4 Exercises: #5,  # 13 (Due Mon 3/10)
+* Peer Review via Github (Due Wed 3/12)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -932,9 +927,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Percent" xfId="90" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
     <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1276,27 +1271,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="41.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="2" width="12.58203125" customWidth="1"/>
+    <col min="4" max="4" width="25.08203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.58203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="39.58203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="41.08203125" style="5" customWidth="1"/>
     <col min="9" max="9" width="35.25" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="300.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1342,19 +1337,19 @@
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="175.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1363,7 +1358,7 @@
         <v>41668</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
@@ -1372,19 +1367,19 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1399,7 +1394,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>17</v>
@@ -1409,10 +1404,10 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="163" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1421,26 +1416,26 @@
         <v>41682</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1467,10 +1462,10 @@
         <v>34</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1482,13 +1477,13 @@
         <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>36</v>
@@ -1497,10 +1492,10 @@
         <v>37</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="188" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1512,13 +1507,13 @@
         <v>40</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>42</v>
@@ -1527,10 +1522,10 @@
         <v>43</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="125.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1539,26 +1534,26 @@
         <v>41710</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="24"/>
       <c r="B10" s="25"/>
       <c r="C10" s="24"/>
@@ -1569,7 +1564,7 @@
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="138" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1577,26 +1572,26 @@
         <v>41724</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="63" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1605,20 +1600,20 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="88" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1627,20 +1622,20 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1649,22 +1644,22 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="125.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1673,18 +1668,18 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1693,18 +1688,18 @@
         <v>41759</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1713,7 +1708,7 @@
         <v>41766</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1722,7 +1717,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1745,26 +1740,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="20"/>
-    <col min="2" max="2" width="32.125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="20"/>
-    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="20"/>
+    <col min="2" max="2" width="32.08203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="20"/>
+    <col min="5" max="5" width="5.08203125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="13" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="13"/>
+    <col min="8" max="8" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1772,27 +1767,27 @@
         <v>24</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>26</v>
@@ -1812,7 +1807,7 @@
         <v>0.33670033670033672</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -1837,7 +1832,7 @@
         <v>0.17508417508417509</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1845,13 +1840,13 @@
         <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="13">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="13">
         <f>SUMIF($C$2:$C$85,F4,$D$2:$D$85)</f>
@@ -1862,12 +1857,12 @@
         <v>0.15151515151515152</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="13">
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>24</v>
@@ -1887,12 +1882,12 @@
         <v>0.33670033670033672</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>26</v>
@@ -1905,7 +1900,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13">
         <v>3</v>
       </c>
@@ -1919,7 +1914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="13">
         <v>3</v>
       </c>
@@ -1927,18 +1922,18 @@
         <v>28</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>24</v>
@@ -1947,26 +1942,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>4</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <v>5</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>24</v>
@@ -1976,27 +1971,27 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13">
         <v>5</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="13">
         <v>5</v>
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="13">
         <v>6</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>24</v>
@@ -2006,27 +2001,27 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="13">
         <v>6</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" s="13">
         <v>5</v>
       </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="13">
         <v>7</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>24</v>
@@ -2036,27 +2031,27 @@
       </c>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="13">
         <v>7</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" s="13">
         <v>5</v>
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="13">
         <v>8</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>29</v>
@@ -2066,12 +2061,12 @@
       </c>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="13">
         <v>10</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>24</v>
@@ -2081,27 +2076,27 @@
       </c>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="13">
         <v>10</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" s="13">
         <v>5</v>
       </c>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>11</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>24</v>
@@ -2111,26 +2106,26 @@
       </c>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="13">
         <v>11</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="13">
         <v>12</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>24</v>
@@ -2139,26 +2134,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="13">
         <v>12</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="13">
         <v>15</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>26</v>
@@ -2167,12 +2162,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="13">
         <v>16</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>29</v>
@@ -2181,241 +2176,241 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="18"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="18"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
       <c r="E55" s="18"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="18"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="18"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
       <c r="E59" s="18"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
       <c r="E60" s="18"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
       <c r="E61" s="18"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -2425,7 +2420,7 @@
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -2435,106 +2430,106 @@
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
       <c r="E64" s="21"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
       <c r="E65" s="21"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
       <c r="E66" s="18"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
       <c r="E67" s="18"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="18"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
       <c r="E69" s="18"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="18"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
       <c r="E71" s="18"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="22"/>
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="22"/>
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
       <c r="D75" s="22"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="22"/>
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
       <c r="D76" s="22"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="22"/>
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="22"/>
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
       <c r="D78" s="22"/>
       <c r="E78" s="19"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="22"/>
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
@@ -2543,14 +2538,14 @@
       <c r="G79"/>
       <c r="H79"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
       <c r="D80" s="22"/>
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="22"/>
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
@@ -2558,7 +2553,7 @@
       <c r="G81"/>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
@@ -2566,7 +2561,7 @@
       <c r="G82"/>
       <c r="H82"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="22"/>
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
@@ -2574,7 +2569,7 @@
       <c r="G83"/>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="22"/>
       <c r="B84" s="22"/>
       <c r="C84" s="22"/>
@@ -2582,7 +2577,7 @@
       <c r="G84"/>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="22"/>
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
@@ -2590,7 +2585,7 @@
       <c r="G85"/>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="22"/>
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
@@ -2598,7 +2593,7 @@
       <c r="G86"/>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="22"/>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
@@ -2606,7 +2601,7 @@
       <c r="G87"/>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="22"/>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
@@ -2614,37 +2609,37 @@
       <c r="G88"/>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="22"/>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
       <c r="D89" s="22"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="22"/>
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
       <c r="D90" s="22"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="22"/>
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
       <c r="D91" s="22"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="22"/>
       <c r="B92" s="22"/>
       <c r="C92" s="22"/>
       <c r="D92" s="22"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="22"/>
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
       <c r="D93" s="22"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="23"/>
       <c r="B94" s="23"/>
       <c r="D94" s="23"/>

</xml_diff>

<commit_message>
add wk9 and 10
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9C0272-C8E2-49DB-97E8-CDF844AF67EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="38400" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +16,7 @@
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="121">
   <si>
     <t>Finals Week</t>
   </si>
@@ -307,9 +308,6 @@
 </t>
   </si>
   <si>
-    <t>* Dashboard Project (Due Friday 3/30)</t>
-  </si>
-  <si>
     <t>Final Project</t>
   </si>
   <si>
@@ -337,11 +335,6 @@
   <si>
     <t>* Describe how the bootstratp method differs from cross-validation
 * Implement cross-validation technique to assess model performance</t>
-  </si>
-  <si>
-    <t>*https://cran.r-project.org/web/packages/caret/vignettes/caret.pdf
-* https://topepo.github.io/caret/
-* Notes from [[MATH 456 S16]](notes/lec10_Classifiers_456_S16.pdf)</t>
   </si>
   <si>
     <t>* Name one reason resampling techniques are used in statistical learning
@@ -358,10 +351,6 @@
     <t>Other Tools</t>
   </si>
   <si>
-    <t>* Read WOMD: Ch 3-4 (MB)
-* [When Data Science Destabilizes Democracy and Facilitates Genocide](http://www.fast.ai/2017/11/02/ethics/)</t>
-  </si>
-  <si>
     <t>* Read WOMD: Ch 5-6 (AS)
 * [More than a Million Pro-Repeal Net Neutrality Comments were Likely Faked](https://hackernoon.com/more-than-a-million-pro-repeal-net-neutrality-comments-were-likely-faked-e9f0e3ed36a6)</t>
   </si>
@@ -375,9 +364,6 @@
   <si>
     <t>* Read WOMD: Ch 9-10 (RAD)
 * Compare [[this article on practical tips for success with ML]](https://www.datanami.com/2018/01/17/practical-tips-success-machine-learning/) with this post on [[google automating ML]](https://www.datanami.com/2018/01/17/google-automate-machine-learning-automl-service/)</t>
-  </si>
-  <si>
-    <t>* ML homework</t>
   </si>
   <si>
     <t>* Big data homework</t>
@@ -482,6 +468,59 @@
 * Read DDS CH 1&amp; 2 (Due Tue 1/30) 
 * Peer review 1 clasmates work by forking their repo, modify their code, then doing a pull request (Due Wed 1/31)
 </t>
+  </si>
+  <si>
+    <t>ISLR Ch 5</t>
+  </si>
+  <si>
+    <t>PR ISLR Ch 5</t>
+  </si>
+  <si>
+    <t>* ISLR Chapter 8
+* Read WOMD: Ch 3-4 (MB)
+* [When Data Science Destabilizes Democracy and Facilitates Genocide](http://www.fast.ai/2017/11/02/ethics/)</t>
+  </si>
+  <si>
+    <t>Robin share WOMD Intro &amp; Ch 1-2</t>
+  </si>
+  <si>
+    <t>Robin share WOMD Ch 9-10</t>
+  </si>
+  <si>
+    <t>Mitch share WOMD Ch 3-4 &amp; extra story</t>
+  </si>
+  <si>
+    <t>Aaron share WOMD CH 5-6 &amp; extra story</t>
+  </si>
+  <si>
+    <t>Ricardo share WOMD Ch 7-8 &amp; extra story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Define terminology: terminal node, internal node, branch, leaf
+* Explain how recursive binary splitting works, and why its considered top down and greedy. 
+* Why is pruning necessary? 
+* What is the optimization critiera for regression trees? For classification trees? 
+* Advantages and disadvantages of trees
+* bagging is a general-purpose procedure for reducing _(bias/variance)____ of a statistical learning method
+* Explain how bagging works
+* What is an out of bag error estimate? Why do we care about it? 
+* Bagging improves prediction accuracy at the expense of ______
+* How is the Gini index used to generate a summary measure of importance for each predictor? 
+* What's the difference between Random Forests and bagged trees? 
+* How is boosting a sequential method? 
+* What are the three tuning parameters for boosting? </t>
+  </si>
+  <si>
+    <t>* ISLR Ch 8 #5, #7, #9</t>
+  </si>
+  <si>
+    <t>* https://cran.r-project.org/web/packages/caret/vignettes/caret.pdf
+* https://topepo.github.io/caret/
+* Notes from [[MATH 456 S16]](notes/lec10_Classifiers_456_S16.pdf)</t>
+  </si>
+  <si>
+    <t>* ISLR Ch 5: #3, #5
+* Blog post about something in the Data Science news lately</t>
   </si>
 </sst>
 </file>
@@ -562,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,6 +629,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +806,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -840,6 +885,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1280,8 +1328,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1342,16 +1390,16 @@
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1363,7 +1411,7 @@
         <v>41668</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
@@ -1372,16 +1420,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1399,7 +1447,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>17</v>
@@ -1409,7 +1457,7 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1421,23 +1469,23 @@
         <v>41682</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1467,7 +1515,7 @@
         <v>34</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1488,7 +1536,7 @@
         <v>38</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>36</v>
@@ -1518,7 +1566,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>42</v>
@@ -1554,9 +1602,7 @@
         <v>68</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
@@ -1577,26 +1623,28 @@
         <v>41724</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="I11" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="294" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1605,17 +1653,21 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="I12" s="4" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
@@ -1627,17 +1679,19 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="I13" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1649,19 +1703,21 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="I14" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1673,15 +1729,17 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1693,11 +1751,11 @@
         <v>41759</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
@@ -1713,7 +1771,7 @@
         <v>41766</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1746,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1792,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>26</v>
@@ -1804,12 +1862,12 @@
         <v>24</v>
       </c>
       <c r="G2" s="13">
-        <f>SUMIF($C$2:$C$85,F2,$D$2:$D$85)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
+        <v>110</v>
       </c>
       <c r="H2" s="16">
         <f>G2/$G$6</f>
-        <v>0.33670033670033672</v>
+        <v>0.41984732824427479</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1829,12 +1887,12 @@
         <v>26</v>
       </c>
       <c r="G3" s="13">
-        <f>SUMIF($C$2:$C$85,F3,$D$2:$D$85)</f>
+        <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
         <v>52</v>
       </c>
       <c r="H3" s="16">
         <f>G3/$G$6</f>
-        <v>0.17508417508417509</v>
+        <v>0.19847328244274809</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1854,12 +1912,12 @@
         <v>50</v>
       </c>
       <c r="G4" s="13">
-        <f>SUMIF($C$2:$C$85,F4,$D$2:$D$85)</f>
-        <v>45</v>
+        <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
+        <v>50</v>
       </c>
       <c r="H4" s="16">
         <f>G4/$G$6</f>
-        <v>0.15151515151515152</v>
+        <v>0.19083969465648856</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1879,12 +1937,12 @@
         <v>29</v>
       </c>
       <c r="G5" s="13">
-        <f>SUMIF($C$2:$C$85,F5,$D$2:$D$85)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
+        <v>50</v>
       </c>
       <c r="H5" s="16">
         <f>G5/$G$6</f>
-        <v>0.33670033670033672</v>
+        <v>0.19083969465648856</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1902,7 +1960,7 @@
       </c>
       <c r="G6" s="17">
         <f>SUM(G2:G5)</f>
-        <v>297</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2051,57 +2109,55 @@
       </c>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
         <v>8</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="29"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>9</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="20">
+        <v>10</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>9</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="D19" s="20">
+        <v>5</v>
+      </c>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>10</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="13">
-        <v>10</v>
-      </c>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
-        <v>10</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="13">
-        <v>5</v>
-      </c>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <v>11</v>
-      </c>
       <c r="B20" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>24</v>
@@ -2111,12 +2167,12 @@
       </c>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>50</v>
@@ -2124,13 +2180,14 @@
       <c r="D21" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>24</v>
@@ -2138,13 +2195,14 @@
       <c r="D22" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>50</v>
@@ -2153,71 +2211,87 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
+        <v>12</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>12</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
         <v>15</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B26" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D26" s="13">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
         <v>16</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="B27" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D27" s="13">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -2258,7 +2332,6 @@
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
@@ -2271,6 +2344,7 @@
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
+      <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
@@ -2301,14 +2375,12 @@
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
@@ -2421,9 +2493,6 @@
       <c r="C62" s="13"/>
       <c r="D62" s="13"/>
       <c r="E62" s="18"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
@@ -2431,37 +2500,40 @@
       <c r="C63" s="13"/>
       <c r="D63" s="13"/>
       <c r="E63" s="18"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
-      <c r="E64" s="21"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
-      <c r="E65" s="21"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
-      <c r="E66" s="18"/>
+      <c r="E66" s="21"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
-      <c r="E67" s="18"/>
+      <c r="E67" s="21"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
@@ -2496,18 +2568,20 @@
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
+      <c r="E72" s="18"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="18"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="22"/>
@@ -2532,16 +2606,12 @@
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
       <c r="D78" s="22"/>
-      <c r="E78" s="19"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="22"/>
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
       <c r="D79" s="22"/>
-      <c r="E79" s="19"/>
-      <c r="G79"/>
-      <c r="H79"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
@@ -2555,6 +2625,7 @@
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
       <c r="D81" s="22"/>
+      <c r="E81" s="19"/>
       <c r="G81"/>
       <c r="H81"/>
     </row>
@@ -2563,8 +2634,7 @@
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
       <c r="D82" s="22"/>
-      <c r="G82"/>
-      <c r="H82"/>
+      <c r="E82" s="19"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
@@ -2619,12 +2689,16 @@
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
       <c r="D89" s="22"/>
+      <c r="G89"/>
+      <c r="H89"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="22"/>
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
       <c r="D90" s="22"/>
+      <c r="G90"/>
+      <c r="H90"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="22"/>
@@ -2645,13 +2719,25 @@
       <c r="D93" s="22"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
-      <c r="B94" s="23"/>
-      <c r="D94" s="23"/>
+      <c r="A94" s="22"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="22"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="23"/>
+      <c r="B96" s="23"/>
+      <c r="D96" s="23"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D94">
-    <sortCondition ref="A2:A94"/>
+  <sortState ref="A2:D96">
+    <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add wk 10 and rebuild
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9C0272-C8E2-49DB-97E8-CDF844AF67EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C0F405-9E81-4F72-A172-18EB2E753C13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="38400" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,10 +351,6 @@
     <t>Other Tools</t>
   </si>
   <si>
-    <t>* Read WOMD: Ch 5-6 (AS)
-* [More than a Million Pro-Repeal Net Neutrality Comments were Likely Faked](https://hackernoon.com/more-than-a-million-pro-repeal-net-neutrality-comments-were-likely-faked-e9f0e3ed36a6)</t>
-  </si>
-  <si>
     <t>* Read WOMD: Ch 7-8 (RA)
 * [Activision Patents Matchmaking That Encourages Players To Buy Microtransactions](https://kotaku.com/activision-patents-matchmaking-that-encourages-players-1819630937)</t>
   </si>
@@ -511,16 +507,25 @@
 * What are the three tuning parameters for boosting? </t>
   </si>
   <si>
-    <t>* ISLR Ch 8 #5, #7, #9</t>
-  </si>
-  <si>
     <t>* https://cran.r-project.org/web/packages/caret/vignettes/caret.pdf
 * https://topepo.github.io/caret/
 * Notes from [[MATH 456 S16]](notes/lec10_Classifiers_456_S16.pdf)</t>
   </si>
   <si>
-    <t>* ISLR Ch 5: #3, #5
-* Blog post about something in the Data Science news lately</t>
+    <t>* ISLR Ch 5: #3, #5 (Due Mon 4/2)
+* Peer review via Github (Due Wed 4/4)
+* Blog post about something in the Data Science news lately (Due Mon 4/2)</t>
+  </si>
+  <si>
+    <t>* Read WOMD: Ch 5-6 (AS)
+* Data Camp Sparklyr Lesson
+* [More than a Million Pro-Repeal Net Neutrality Comments were Likely Faked](https://hackernoon.com/more-than-a-million-pro-repeal-net-neutrality-comments-were-likely-faked-e9f0e3ed36a6)</t>
+  </si>
+  <si>
+    <t>* ISLR Ch 8 #5, #7, #9 (Due Mon 4/9)
+* Peer Review via Github (Due Wed 4/11)
+* Blog post about Genocide reading (Due Mon 4/9)
+* Complete Data Camp Sparklyr lesson (Due Wed 4/11)</t>
   </si>
 </sst>
 </file>
@@ -1327,9 +1332,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1390,16 +1395,16 @@
         <v>19</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1423,13 +1428,13 @@
         <v>70</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1452,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>17</v>
@@ -1457,7 +1462,7 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,23 +1474,23 @@
         <v>41682</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1515,7 +1520,7 @@
         <v>34</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1536,7 +1541,7 @@
         <v>38</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>36</v>
@@ -1566,7 +1571,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>42</v>
@@ -1632,16 +1637,16 @@
         <v>75</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>77</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="294" thickBot="1" x14ac:dyDescent="0.3">
@@ -1657,20 +1662,20 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1683,15 +1688,15 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1703,21 +1708,21 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1733,12 +1738,12 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -1755,7 +1760,7 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
@@ -1850,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>26</v>
@@ -2127,7 +2132,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>24</v>
@@ -2142,7 +2147,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>50</v>
@@ -2157,7 +2162,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>24</v>
@@ -2172,7 +2177,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>50</v>
@@ -2187,7 +2192,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>24</v>
@@ -2202,7 +2207,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>50</v>
@@ -2216,7 +2221,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>24</v>
@@ -2230,7 +2235,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
finish? prep for wk1
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE777BD-31BA-4C73-8DC2-BDF37FB02E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FB543C-1AC0-44F7-BE66-9EFE0ED8676A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="141">
   <si>
     <t>Finals Week</t>
   </si>
@@ -481,10 +481,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t xml:space="preserve">[hw00: Getting Started](hw/hw00-getting-started.html) (Due Wed 1/22 )
-</t>
-  </si>
-  <si>
     <t>Read DDS Ch1</t>
   </si>
   <si>
@@ -516,10 +512,6 @@
   </si>
   <si>
     <t>Get approved for a Twiter Dev account</t>
-  </si>
-  <si>
-    <t>Read DDS Ch3
-Read ISLR Ch1, Ch2</t>
   </si>
   <si>
     <t>Read ISLR Chapter 3: Intro, 3.5</t>
@@ -543,10 +535,6 @@
     <t>Ethics of ML algorithms</t>
   </si>
   <si>
-    <t>* ISLR Chapter 5
-* Install the caret package</t>
-  </si>
-  <si>
     <t>Read WMD: Intro, Ch 1-2</t>
   </si>
   <si>
@@ -582,23 +570,48 @@
     <t>Grade POLS Learn R HW (4 x 3 students ea. )</t>
   </si>
   <si>
-    <t>* [Lec00: Class Orientation](lec/lec00_orientation.html)</t>
-  </si>
-  <si>
-    <t>* [Lec01a - RMarkdown Websites](lec/lec01a_rmarkdown_website.html)
-* [Lec01b - Blogdown Websites](lec/lec01b_blogdown_website.html)</t>
-  </si>
-  <si>
-    <t>[hw01: Personal Website](hw/hw01-website.html) (Due 1/28 )</t>
-  </si>
-  <si>
     <t>POLS Project</t>
   </si>
   <si>
-    <t xml:space="preserve">Form DS collaboration teams with POLS students. </t>
-  </si>
-  <si>
-    <t>* [Lec02 - What is DS](lec/lec02-what-is-ds.html)</t>
+    <t>Interactive lecture 02 (Hack MD)</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Learning</t>
+  </si>
+  <si>
+    <t>DATA FEST!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [hw00: Getting Started](hw/hw00-getting-started.html) (Due Wed 1/22 )
+</t>
+  </si>
+  <si>
+    <t>* [hw01: Personal Website](hw/hw01-website.html) (Due 1/28 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Form DS collaboration teams with POLS students. </t>
+  </si>
+  <si>
+    <t>[Lec01a - RMarkdown Websites](lec/lec01a_rmarkdown_website.html)  
+[Lec01b - Blogdown Websites](lec/lec01b_blogdown_website.html)</t>
+  </si>
+  <si>
+    <t>[Lec00: Class Orientation](lec/lec00_orientation.html)</t>
+  </si>
+  <si>
+    <t>[Lec02 - What is DS](https://hackmd.io/@norcalbiostat/data485-lec02)</t>
+  </si>
+  <si>
+    <t>ISLR Chapter 5  
+Install the caret package</t>
+  </si>
+  <si>
+    <t>Read DDS Ch3  
+Read ISLR Ch1, Ch2</t>
+  </si>
+  <si>
+    <t>* Share a blog post or tweet in #state-of-ds (Due x/x )
+* Read the linked article,  and comment on someone elses post (Due x/x )</t>
   </si>
 </sst>
 </file>
@@ -872,7 +885,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -950,6 +963,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1388,11 +1404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1452,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -1449,17 +1465,17 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="10" t="s">
@@ -1467,7 +1483,7 @@
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>133</v>
@@ -1475,7 +1491,7 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -1484,24 +1500,28 @@
         <v>42397</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+        <v>137</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28"/>
       <c r="B5" s="3"/>
       <c r="C5" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1519,11 +1539,11 @@
         <v>42404</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -1535,12 +1555,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7:B22" si="0">B6+7</f>
+        <f t="shared" ref="B7:B21" si="0">B6+7</f>
         <v>42411</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4"/>
@@ -1555,10 +1575,12 @@
         <f t="shared" si="0"/>
         <v>42418</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
@@ -1574,30 +1596,30 @@
         <v>42425</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1615,10 +1637,10 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1633,54 +1655,60 @@
         <v>42439</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24">
+    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24">
         <f>B12+7</f>
         <v>42446</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C13" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="29">
+        <f>B13+7</f>
+        <v>42453</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
-        <v>41724</v>
+        <f t="shared" si="0"/>
+        <v>42460</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4"/>
@@ -1692,43 +1720,45 @@
     </row>
     <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
         <f t="shared" si="0"/>
-        <v>41731</v>
+        <v>42467</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="0"/>
-        <v>41738</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>42474</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="0"/>
-        <v>41745</v>
+        <v>42481</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4"/>
@@ -1740,11 +1770,11 @@
     </row>
     <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" si="0"/>
-        <v>41752</v>
+        <v>42488</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="4"/>
@@ -1756,13 +1786,15 @@
     </row>
     <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
-        <v>41759</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>42495</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
@@ -1772,14 +1804,14 @@
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
-        <v>41766</v>
+        <v>42502</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1787,24 +1819,6 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>41773</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2337,7 +2351,7 @@
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2356,7 +2370,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2375,7 +2389,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2394,7 +2408,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2413,7 +2427,7 @@
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2425,7 +2439,7 @@
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2433,7 +2447,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2441,7 +2455,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -2449,7 +2463,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2457,7 +2471,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2466,7 +2480,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>

</xml_diff>

<commit_message>
cleanup website instructions, add hw
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A884EA-B94E-46B8-A065-385739E4A60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2876F5-4579-4BA3-A43D-E8233B2720CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="570" windowWidth="25905" windowHeight="14430" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -502,9 +502,6 @@
     <t>Get historical twitter data (DEMO)</t>
   </si>
   <si>
-    <t>Get approved for a Twiter Dev account</t>
-  </si>
-  <si>
     <t>Read ISLR Chapter 3: Intro, 3.5</t>
   </si>
   <si>
@@ -529,101 +526,106 @@
     <t>Read WMD: Intro, Ch 1-2</t>
   </si>
   <si>
+    <t>Community Coding</t>
+  </si>
+  <si>
+    <t>DataFest</t>
+  </si>
+  <si>
+    <t>Reflect on DDS case study (n=5)</t>
+  </si>
+  <si>
+    <t>Share DDS Case study (n=1)</t>
+  </si>
+  <si>
+    <t>WMD Reflections</t>
+  </si>
+  <si>
+    <t>Blog posts (5) on external topics of interest</t>
+  </si>
+  <si>
+    <t>Comments on Blog posts</t>
+  </si>
+  <si>
+    <t>Grade POLS Learn R HW (4 x 3 students ea. )</t>
+  </si>
+  <si>
+    <t>POLS Project</t>
+  </si>
+  <si>
+    <t>Interactive lecture 02 (Hack MD)</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Learning</t>
+  </si>
+  <si>
+    <t>DATA FEST!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [hw00: Getting Started](hw/hw00-getting-started.html) (Due Wed 1/22 )
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Form DS collaboration teams with POLS students. </t>
+  </si>
+  <si>
+    <t>[Lec01a - RMarkdown Websites](lec/lec01a_rmarkdown_website.html)  
+[Lec01b - Blogdown Websites](lec/lec01b_blogdown_website.html)</t>
+  </si>
+  <si>
+    <t>[Lec00: Class Orientation](lec/lec00_orientation.html)</t>
+  </si>
+  <si>
+    <t>[Lec02 - What is DS](https://hackmd.io/@norcalbiostat/data485-lec02)</t>
+  </si>
+  <si>
+    <t>ISLR Chapter 5  
+Install the caret package</t>
+  </si>
+  <si>
+    <t>Read DDS Ch3  
+Read ISLR Ch1, Ch2</t>
+  </si>
+  <si>
+    <t>* [hw01: Personal Website](hw/hw01-website.html) (Due Wed 1/29 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [hw02: What is DS](hw/hw02-what-is-ds.html) (Due Mon 2/3 )
+</t>
+  </si>
+  <si>
+    <t>Mind MAP: What makes a good DS?</t>
+  </si>
+  <si>
+    <t>What is Data Science?  What's your DS path?</t>
+  </si>
+  <si>
+    <t>Share mind maps (20)</t>
+  </si>
+  <si>
+    <t>What is DS mind map</t>
+  </si>
+  <si>
+    <t>What is DS - hack notes</t>
+  </si>
+  <si>
+    <t>participation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lec00
 3-2-1 Bridge: What is Data Science? 
-Spend 2 min reviewing the course description. 
-Rank each category - write this down. 
+Spend 1 min reviewing the course description solo. Rank categories. 
+Share with table (3-5 min)
 What is missing, what do you want to add? 
-Do you want to re-rank? Write your final rankings in your LJ. </t>
-  </si>
-  <si>
-    <t>Community Coding</t>
-  </si>
-  <si>
-    <t>DataFest</t>
-  </si>
-  <si>
-    <t>Reflect on DDS case study (n=5)</t>
-  </si>
-  <si>
-    <t>Share DDS Case study (n=1)</t>
-  </si>
-  <si>
-    <t>WMD Reflections</t>
-  </si>
-  <si>
-    <t>Blog posts (5) on external topics of interest</t>
-  </si>
-  <si>
-    <t>Comments on Blog posts</t>
-  </si>
-  <si>
-    <t>Grade POLS Learn R HW (4 x 3 students ea. )</t>
-  </si>
-  <si>
-    <t>POLS Project</t>
-  </si>
-  <si>
-    <t>Interactive lecture 02 (Hack MD)</t>
-  </si>
-  <si>
-    <t>Intro to Statistical Learning</t>
-  </si>
-  <si>
-    <t>DATA FEST!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* [hw00: Getting Started](hw/hw00-getting-started.html) (Due Wed 1/22 )
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Form DS collaboration teams with POLS students. </t>
-  </si>
-  <si>
-    <t>[Lec01a - RMarkdown Websites](lec/lec01a_rmarkdown_website.html)  
-[Lec01b - Blogdown Websites](lec/lec01b_blogdown_website.html)</t>
-  </si>
-  <si>
-    <t>[Lec00: Class Orientation](lec/lec00_orientation.html)</t>
-  </si>
-  <si>
-    <t>[Lec02 - What is DS](https://hackmd.io/@norcalbiostat/data485-lec02)</t>
-  </si>
-  <si>
-    <t>ISLR Chapter 5  
-Install the caret package</t>
-  </si>
-  <si>
-    <t>Read DDS Ch3  
-Read ISLR Ch1, Ch2</t>
-  </si>
-  <si>
-    <t>Read DDS Ch1, 16</t>
-  </si>
-  <si>
-    <t>* [hw01: Personal Website](hw/hw01-website.html) (Due Wed 1/29 )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* [hw02: What is DS](hw/hw02-what-is-ds.html) (Due Mon 2/3 )
-</t>
-  </si>
-  <si>
-    <t>Mind MAP: What makes a good DS?</t>
-  </si>
-  <si>
-    <t>What is Data Science?  What's your DS path?</t>
-  </si>
-  <si>
-    <t>Share mind maps (20)</t>
-  </si>
-  <si>
-    <t>What is DS mind map</t>
-  </si>
-  <si>
-    <t>What is DS - hack notes</t>
-  </si>
-  <si>
-    <t>participation</t>
+Rerank if desired and record your final rankings in your LJ. </t>
+  </si>
+  <si>
+    <t>Read DDS Ch1, 16.   
+Review DS Research examples in the Social Science (Handout)</t>
+  </si>
+  <si>
+    <t>Get approved for a Twiter Dev account.    
+Read at least one SS paper in Google Drive and summarize data extraction/analysis</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1437,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1492,13 +1494,13 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -1510,10 +1512,10 @@
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -1527,26 +1529,26 @@
         <v>42397</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -1559,12 +1561,12 @@
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -1594,11 +1596,11 @@
         <v>42418</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4"/>
@@ -1614,30 +1616,30 @@
         <v>42425</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1673,11 +1675,11 @@
         <v>42439</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="4"/>
@@ -1709,11 +1711,11 @@
         <v>42453</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
@@ -1761,7 +1763,7 @@
         <v>42474</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2432,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2453,7 +2455,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2465,7 +2467,7 @@
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2473,7 +2475,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2481,7 +2483,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -2489,7 +2491,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2497,7 +2499,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2506,7 +2508,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -2517,7 +2519,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2528,10 +2530,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D14"/>
       <c r="G14"/>

</xml_diff>

<commit_message>
add wk2 and project page
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2876F5-4579-4BA3-A43D-E8233B2720CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0C10EB-36BF-434F-9206-D1415DCBEE88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,18 +576,12 @@
     <t>[Lec00: Class Orientation](lec/lec00_orientation.html)</t>
   </si>
   <si>
-    <t>[Lec02 - What is DS](https://hackmd.io/@norcalbiostat/data485-lec02)</t>
-  </si>
-  <si>
     <t>ISLR Chapter 5  
 Install the caret package</t>
   </si>
   <si>
     <t>Read DDS Ch3  
 Read ISLR Ch1, Ch2</t>
-  </si>
-  <si>
-    <t>* [hw01: Personal Website](hw/hw01-website.html) (Due Wed 1/29 )</t>
   </si>
   <si>
     <t xml:space="preserve">* [hw02: What is DS](hw/hw02-what-is-ds.html) (Due Mon 2/3 )
@@ -620,12 +614,18 @@
 Rerank if desired and record your final rankings in your LJ. </t>
   </si>
   <si>
-    <t>Read DDS Ch1, 16.   
-Review DS Research examples in the Social Science (Handout)</t>
-  </si>
-  <si>
     <t>Get approved for a Twiter Dev account.    
 Read at least one SS paper in Google Drive and summarize data extraction/analysis</t>
+  </si>
+  <si>
+    <t>* [hw01: Personal Website](hw/hw01-website.html) (Due Fri 1/31 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read DDS Ch1, 16.   </t>
+  </si>
+  <si>
+    <t>[Lec02 - What is DS](https://hackmd.io/@norcalbiostat/data485-lec02)  
+DS Research examples in the Social Science (Google Drive)</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1437,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1500,7 @@
         <v>127</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -1515,12 +1515,12 @@
         <v>129</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -1529,23 +1529,23 @@
         <v>42397</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
         <v>143</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>124</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1561,12 +1561,12 @@
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4"/>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="4"/>
@@ -2519,7 +2519,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2530,10 +2530,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D14"/>
       <c r="G14"/>

</xml_diff>

<commit_message>
clean up hw and add wk3
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA2BF5A-C0B3-41CB-9556-37EC8A431E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40138C-250D-4FF3-9A78-9F4F3BB90A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="161">
   <si>
     <t>Finals Week</t>
   </si>
@@ -487,9 +487,6 @@
     <t>Ref DDS Ch 5</t>
   </si>
   <si>
-    <t>Get historical twitter data (DEMO)</t>
-  </si>
-  <si>
     <t>Read ISLR Chapter 3: Intro, 3.5</t>
   </si>
   <si>
@@ -573,9 +570,6 @@
     <t>What is Data Science?  What's your DS path?</t>
   </si>
   <si>
-    <t>Share mind maps (20)</t>
-  </si>
-  <si>
     <t>What is DS - hack notes</t>
   </si>
   <si>
@@ -596,12 +590,6 @@
     <t xml:space="preserve">Read DDS Ch1, 16.   </t>
   </si>
   <si>
-    <t>HW1: R Markdown website</t>
-  </si>
-  <si>
-    <t>HW1: Blogdown website</t>
-  </si>
-  <si>
     <t>Slack Intro</t>
   </si>
   <si>
@@ -609,9 +597,6 @@
   </si>
   <si>
     <t>HW2: reflect on others share</t>
-  </si>
-  <si>
-    <t>HW2: What is DS mind map</t>
   </si>
   <si>
     <t>Grade POLS Learn R HW (4 x 2 students ea. )</t>
@@ -621,10 +606,6 @@
 Interactive lecture 02 (Hack MD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Finish HackMD Lec02 
-Mind MAP: What is the field of Data science? </t>
-  </si>
-  <si>
     <t xml:space="preserve">[Lec02 - What is DS](https://hackmd.io/@norcalbiostat/data485-lec02)  
 </t>
   </si>
@@ -642,18 +623,64 @@
 [Twitter collab notes ](https://hackmd.io/@norcalbiostat/data485-twitter)  </t>
   </si>
   <si>
-    <t xml:space="preserve">* Help turn the Twitter collab notes into a working tutorial. </t>
-  </si>
-  <si>
-    <t>Get approved for a Twiter Dev account.     
-Read through the links in the Twitter collab notes.</t>
-  </si>
-  <si>
     <t>Read DDS Ch2  
 Read at least one SS paper in Google Drive and prepare to share extraction/analysis</t>
   </si>
   <si>
     <t>Share POLS DS analysis</t>
+  </si>
+  <si>
+    <t>Finish HackMD Lec02 
+Mind MAP: What is the field of Data science? 
+Work in pairs for 10 min, share out to class 10 min</t>
+  </si>
+  <si>
+    <t>Get approved for a Twiter Dev account.     
+Read through the links in the Twitter collab notes.
+Read the example POLS DS projects in Google Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [hw03: Hello Twitter](hw/hw03-hello-twitter.html) (Due TBD )
+</t>
+  </si>
+  <si>
+    <t>Open work time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hackathon / open work time. </t>
+  </si>
+  <si>
+    <t>HW1: R Markdown website demo</t>
+  </si>
+  <si>
+    <t>HW1: Blogdown website demo</t>
+  </si>
+  <si>
+    <t>HW1: Personal website</t>
+  </si>
+  <si>
+    <t>HW3: Twitter tutorial for others</t>
+  </si>
+  <si>
+    <t>HW3: Historical twitter data demo</t>
+  </si>
+  <si>
+    <t>HW3: Sentiment analysis</t>
+  </si>
+  <si>
+    <t>What is DS mind map share out</t>
+  </si>
+  <si>
+    <t>Add info to class-logsitics repo via PR</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>communication</t>
+  </si>
+  <si>
+    <t>skills</t>
   </si>
 </sst>
 </file>
@@ -734,7 +761,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +783,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -938,7 +977,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1038,6 +1077,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1479,7 +1524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1524,7 +1569,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
       <c r="B2" s="3">
@@ -1536,18 +1581,18 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="3"/>
       <c r="C3" s="10" t="s">
         <v>99</v>
@@ -1556,18 +1601,18 @@
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -1575,27 +1620,27 @@
         <v>42397</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37">
         <v>3</v>
       </c>
       <c r="B5" s="3">
@@ -1603,22 +1648,24 @@
         <v>42404</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
@@ -1629,16 +1676,16 @@
         <v>42411</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="9" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -1651,11 +1698,11 @@
         <v>42418</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4"/>
@@ -1671,16 +1718,16 @@
         <v>42425</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -1688,13 +1735,13 @@
       <c r="A9" s="28"/>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1730,11 +1777,11 @@
         <v>42439</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="4"/>
@@ -1766,11 +1813,11 @@
         <v>42453</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
@@ -1818,7 +1865,7 @@
         <v>42474</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2385,14 +2432,14 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="34"/>
     <col min="2" max="2" width="38" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.375" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.875" style="19"/>
     <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
@@ -2428,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2449,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2470,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2491,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2509,12 +2556,14 @@
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6"/>
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
       <c r="D6"/>
       <c r="G6" s="16">
         <f>SUM(G2:G5)</f>
@@ -2523,44 +2572,50 @@
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
-        <v>2.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7"/>
+        <v>150</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
-        <v>2.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9"/>
+        <v>152</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10"/>
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2568,103 +2623,139 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11"/>
+        <v>156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>159</v>
+      </c>
       <c r="D11"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12"/>
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>158</v>
+      </c>
       <c r="D12"/>
       <c r="G12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13"/>
+        <v>135</v>
+      </c>
+      <c r="C13" t="s">
+        <v>159</v>
+      </c>
       <c r="D13"/>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14"/>
+        <v>153</v>
+      </c>
+      <c r="C14" t="s">
+        <v>159</v>
+      </c>
       <c r="D14"/>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15"/>
+        <v>154</v>
+      </c>
+      <c r="C15" t="s">
+        <v>160</v>
+      </c>
       <c r="D15"/>
       <c r="G15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
-        <v>9</v>
+        <v>3.3</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16"/>
+        <v>155</v>
+      </c>
+      <c r="C16" t="s">
+        <v>160</v>
+      </c>
       <c r="D16"/>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17"/>
+        <v>113</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
       <c r="D17"/>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18"/>
-      <c r="C18"/>
+      <c r="A18" s="31">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
       <c r="D18"/>
       <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19"/>
-      <c r="C19"/>
+      <c r="A19" s="31">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
       <c r="D19"/>
       <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20"/>
+      <c r="A20" s="31">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21"/>
-      <c r="C21"/>
+      <c r="A21" s="31">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>159</v>
+      </c>
       <c r="D21"/>
       <c r="G21"/>
     </row>
@@ -3174,7 +3265,7 @@
       <c r="D96" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D96">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
     <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
work on wk 5 part 1
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/ADS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0033B345-ED2A-D946-9467-66F137B7383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A17E95-B0F0-450F-8500-7CFD5A168D3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
     <sheet name="schedule_s18" sheetId="4" r:id="rId2"/>
     <sheet name="assignments" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="177">
   <si>
     <t>Finals Week</t>
   </si>
@@ -479,12 +487,6 @@
     <t>Ref DDS Ch 5</t>
   </si>
   <si>
-    <t>Read ISLR Chapter 3: Intro, 3.5</t>
-  </si>
-  <si>
-    <t>Linear Regression</t>
-  </si>
-  <si>
     <t>Resampling Methods</t>
   </si>
   <si>
@@ -663,27 +665,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Review POLS Learn R HW 3 (Due 3/3 )  
-Blog post &amp; response (Due 2/29 )  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Add questions: 
--- does KNN perform better than linear regression? 
--- when would you choose to perform KNN over LinReg?
-</t>
-  </si>
-  <si>
     <t>BSS Project Poster Session</t>
   </si>
   <si>
     <t>"I used to think… but now I think…"</t>
-  </si>
-  <si>
-    <t>Return to bridge. 
-Questions in ISLR Ch 2</t>
-  </si>
-  <si>
-    <t>ISLR Ch 1, 2</t>
   </si>
   <si>
     <t>Sleep! Play! Refresh!</t>
@@ -703,22 +688,53 @@
 </t>
   </si>
   <si>
-    <t>Share DDS Case study</t>
-  </si>
-  <si>
     <t>LJ entry - what from the reading stood out to you? What did you learn? 
 Intro to Real estate case study from DDS Ch 2</t>
   </si>
   <si>
-    <t>Summarize chosen DDS Case study on Tue  
-Read ISLR Ch1, Ch2 before Th</t>
-  </si>
-  <si>
     <t xml:space="preserve">Respond to Slack poll on POLS #reading, and prepare to share on Tue. </t>
   </si>
   <si>
     <t xml:space="preserve">[hw04: Real estate case study](https://classroom.github.com/a/2BmxOWsY) (Printed report due in class 2/25 )   
 Review POLS Learn R HW 2 (Due 2/25 )  </t>
+  </si>
+  <si>
+    <t>Share DDS Case study
+Return to bridge (time pending)</t>
+  </si>
+  <si>
+    <t>Summarize chosen DDS Case study on Tue  
+Read ISLR Ch1 before Th. 
+Prepare your part of HW5 before Th.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISLR Ch 1, 2  
+ISLR MOOC [Video lectures](http://auapps.american.edu/alberto/www/analytics/ISLRLectures.html)  
+[Materials from DSO/IOM 530 at USC](https://www.alsharif.info/iom530)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review POLS Learn R HW 3 (Due 3/3 )  
+Blog post &amp; response (Due 2/29 )  
+[hw05: Statistical Learning](hw/hw05-statistical-learning.html) (Due x/xx )   </t>
+  </si>
+  <si>
+    <t>Jigsaw lecture on ISLR Ch 2 by answering assigned questions from ISLR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Translate a business question into a mathematical model. 
+* Identify cases where a non-parametric approach would be more appropriate than a parametric approach. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISLR Ch 3. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Familarize yourself with the advertising data from Ch 2. </t>
+  </si>
+  <si>
+    <t>Part III hw 5</t>
+  </si>
+  <si>
+    <t>Finish Part I of HW 5</t>
   </si>
 </sst>
 </file>
@@ -1551,24 +1567,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
     <col min="6" max="6" width="39.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="41.83203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="37.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="41.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="37.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="31.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1613,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -1610,17 +1626,17 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36"/>
       <c r="B3" s="3"/>
       <c r="C3" s="10" t="s">
@@ -1630,17 +1646,17 @@
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="71" thickBot="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -1649,26 +1665,26 @@
         <v>42395</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="36">
         <v>3</v>
       </c>
@@ -1677,26 +1693,26 @@
         <v>42402</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>138</v>
-      </c>
       <c r="I5" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="71" thickBot="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -1705,27 +1721,27 @@
         <v>42409</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="9" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="85" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36">
         <v>5</v>
       </c>
       <c r="B7" s="3">
@@ -1733,26 +1749,26 @@
         <v>42416</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -1761,26 +1777,28 @@
         <v>42423</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="85" thickBot="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -1789,20 +1807,26 @@
         <v>42430</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="E9" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9" s="6"/>
+        <v>174</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>173</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -1824,7 +1848,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="24">
         <f t="shared" si="1"/>
@@ -1835,16 +1859,16 @@
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1853,18 +1877,18 @@
         <v>42451</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1873,18 +1897,18 @@
         <v>42458</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1893,7 +1917,7 @@
         <v>42465</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1902,7 +1926,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1911,7 +1935,7 @@
         <v>42472</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1920,7 +1944,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1929,7 +1953,7 @@
         <v>42479</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1937,10 +1961,10 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1956,7 +1980,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1974,7 +1998,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2003,23 +2027,23 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="41.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="35.1640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="39.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="41.125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="35.125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2048,7 +2072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="359" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -2077,7 +2101,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="211" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -2107,7 +2131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>3</v>
       </c>
@@ -2135,7 +2159,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="197" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
         <v>4</v>
       </c>
@@ -2163,7 +2187,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
         <v>5</v>
       </c>
@@ -2193,7 +2217,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>6</v>
       </c>
@@ -2223,7 +2247,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="225" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28">
         <v>7</v>
       </c>
@@ -2253,7 +2277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="155" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -2279,7 +2303,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="23"/>
@@ -2290,7 +2314,7 @@
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:9" ht="169" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2319,7 +2343,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="333" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="294" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2345,7 +2369,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2369,7 +2393,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="85" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2395,7 +2419,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2417,7 +2441,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2437,7 +2461,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2455,7 +2479,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -2485,19 +2509,19 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="34"/>
+    <col min="1" max="1" width="8.875" style="34"/>
     <col min="2" max="2" width="38" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="19"/>
-    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="19"/>
+    <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="12"/>
+    <col min="8" max="8" width="8.875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -2520,12 +2544,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2541,12 +2565,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2562,12 +2586,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2583,12 +2607,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2604,15 +2628,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31">
         <v>0.1</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D6"/>
       <c r="G6" s="16">
@@ -2620,467 +2644,467 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>1.2</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>1.3</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>3.2</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>3.3</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="17"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="31"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="17"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="17"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="17"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="17"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="17"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="17"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="17"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="31"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="17"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="31"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="17"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="31"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="17"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="31"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="17"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="31"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="17"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="31"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="17"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="31"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="17"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="31"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="17"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="31"/>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="17"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="31"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="17"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="31"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
@@ -3090,7 +3114,7 @@
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="31"/>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
@@ -3100,106 +3124,106 @@
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="31"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
       <c r="E66" s="20"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="31"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="20"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="31"/>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="17"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="17"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="31"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="17"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
       <c r="E71" s="17"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="31"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="17"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="17"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="31"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
       <c r="D75" s="21"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="32"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
       <c r="D76" s="21"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="32"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
       <c r="D77" s="21"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="32"/>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="32"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
       <c r="D79" s="21"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="32"/>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
       <c r="D80" s="21"/>
       <c r="E80" s="18"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="32"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
@@ -3208,14 +3232,14 @@
       <c r="G81"/>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="32"/>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
       <c r="D82" s="21"/>
       <c r="E82" s="18"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="32"/>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
@@ -3223,7 +3247,7 @@
       <c r="G83"/>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="32"/>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
@@ -3231,7 +3255,7 @@
       <c r="G84"/>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="32"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
@@ -3239,7 +3263,7 @@
       <c r="G85"/>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="32"/>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
@@ -3247,7 +3271,7 @@
       <c r="G86"/>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="32"/>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
@@ -3255,7 +3279,7 @@
       <c r="G87"/>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="32"/>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
@@ -3263,7 +3287,7 @@
       <c r="G88"/>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="32"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -3271,7 +3295,7 @@
       <c r="G89"/>
       <c r="H89"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="32"/>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -3279,43 +3303,43 @@
       <c r="G90"/>
       <c r="H90"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="32"/>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
       <c r="D91" s="21"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="32"/>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
       <c r="D92" s="21"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="32"/>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
       <c r="D93" s="21"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="32"/>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
       <c r="D94" s="21"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="32"/>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
       <c r="D95" s="21"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="33"/>
       <c r="B96" s="22"/>
       <c r="D96" s="22"/>
     </row>
   </sheetData>
-  <sortState ref="A2:C96">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
     <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
convert to wk9 notes
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20356"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11494A59-8C98-4D66-ADC1-5D707AD06BC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A1CAA0-636E-4B0F-AB37-C76F3C56CE1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,14 +22,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -38,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="188">
   <si>
     <t>Finals Week</t>
   </si>
@@ -742,15 +734,6 @@
     <t>Twitter project updates and next steps. Task identification</t>
   </si>
   <si>
-    <t>ISLR Ch 3
-[Class notes from 03-10](notes/wk8-notes-03-10-2020.html)
-[Class notes from 03-12](notes/wk8-notes-03-12-2020.html)</t>
-  </si>
-  <si>
-    <t>[Notes from 03-24](notes/wk9-notes-03-24-2020.html)
-[Class notes from 03-26](notes/wk9-notes-03-26-2020.html)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Review the notes from 3/24 even though we didn’t meet that day. </t>
   </si>
   <si>
@@ -774,6 +757,17 @@
   </si>
   <si>
     <t>NLP - Predictive analytics</t>
+  </si>
+  <si>
+    <t>ISLR Ch 3  
+[Class notes from 03-10](notes/wk8-notes-03-10-2020.html)  
+[Class notes from 03-12](notes/wk8-notes-03-12-2020.html)</t>
+  </si>
+  <si>
+    <t>[Week 9 Notes](notes/wk9-notes.html)</t>
+  </si>
+  <si>
+    <t>[Week 10 Notes](notes/wk10-notes.html)</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1632,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1911,7 +1905,7 @@
         <v>171</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
@@ -1946,17 +1940,17 @@
         <v>42451</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="H12" s="40" t="s">
         <v>170</v>
@@ -1972,7 +1966,10 @@
         <v>42458</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>170</v>
@@ -1992,7 +1989,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>102</v>
@@ -2010,11 +2007,11 @@
         <v>42472</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -2029,7 +2026,7 @@
         <v>42479</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -3420,7 +3417,7 @@
       <c r="D96" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
+  <sortState ref="A2:C96">
     <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix link in schedule to wk9 notes
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A1CAA0-636E-4B0F-AB37-C76F3C56CE1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875301AF-D67F-4ACF-8318-1F7FD5547FD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -760,14 +760,14 @@
   </si>
   <si>
     <t>ISLR Ch 3  
-[Class notes from 03-10](notes/wk8-notes-03-10-2020.html)  
-[Class notes from 03-12](notes/wk8-notes-03-12-2020.html)</t>
-  </si>
-  <si>
-    <t>[Week 9 Notes](notes/wk9-notes.html)</t>
-  </si>
-  <si>
-    <t>[Week 10 Notes](notes/wk10-notes.html)</t>
+[Class notes from 03-10](lec/wk8-notes-03-10-2020.html)  
+[Class notes from 03-12](lec/wk8-notes-03-12-2020.html)</t>
+  </si>
+  <si>
+    <t>[Week 9 Notes](lec/wk9-notes.html)</t>
+  </si>
+  <si>
+    <t>[Week 10 Notes](lec/wk10-notes.html)</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1632,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add starter notes for wk11
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DF6409-3142-4131-A028-C457CBC2723D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FF3080-A6ED-4FEB-B82C-CE272A89EA47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="18408" windowHeight="6252" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="191">
   <si>
     <t>Finals Week</t>
   </si>
@@ -473,9 +473,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Ref DDS Ch 5</t>
-  </si>
-  <si>
     <t>Read WMD: Intro, Ch 1-2</t>
   </si>
   <si>
@@ -747,9 +744,6 @@
     <t>NLP- Sentiment analysis</t>
   </si>
   <si>
-    <t>ISLR Chapter 4 (Intro), 4.1, 4.4, 4.5</t>
-  </si>
-  <si>
     <t>Cross-Validation, Bootstrap</t>
   </si>
   <si>
@@ -771,6 +765,21 @@
     <t>ISLR Ch 3  
 [Class notes from 03-10](lec/wk08-notes-03-10-2020.html)  
 [Class notes from 03-12](lec/wk08-notes-03-12-2020.html)</t>
+  </si>
+  <si>
+    <t>Watch at least one recap video (links in Wk 11 notes)</t>
+  </si>
+  <si>
+    <t>Finals week</t>
+  </si>
+  <si>
+    <t>[Classification Assignment]( ) (Due 04/18)</t>
+  </si>
+  <si>
+    <t>[Week 11 Notes](lec/wk11-notes.html)
+[lec03-classifiers Hack MD notes]()
+ISLR Chapter 4
+Doing Data Science Ch 5</t>
   </si>
 </sst>
 </file>
@@ -1634,23 +1643,23 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="25.09765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.59765625" style="5" customWidth="1"/>
     <col min="6" max="6" width="39.5" style="5" customWidth="1"/>
-    <col min="7" max="7" width="41.875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="37.625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="31.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="41.8984375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="37.59765625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="31.59765625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -1692,17 +1701,17 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36"/>
       <c r="B3" s="3"/>
       <c r="C3" s="10" t="s">
@@ -1712,17 +1721,17 @@
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36">
         <v>2</v>
       </c>
@@ -1731,26 +1740,26 @@
         <v>42395</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36">
         <v>3</v>
       </c>
@@ -1759,26 +1768,26 @@
         <v>42402</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36">
         <v>4</v>
       </c>
@@ -1787,26 +1796,26 @@
         <v>42409</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36">
         <v>5</v>
       </c>
@@ -1815,26 +1824,26 @@
         <v>42416</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36">
         <v>6</v>
       </c>
@@ -1843,24 +1852,24 @@
         <v>42423</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -1869,28 +1878,28 @@
         <v>42430</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="39">
         <v>8</v>
       </c>
@@ -1902,23 +1911,23 @@
         <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28"/>
       <c r="B11" s="24">
         <f t="shared" si="1"/>
@@ -1934,7 +1943,7 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28">
         <v>9</v>
       </c>
@@ -1943,24 +1952,24 @@
         <v>42451</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="H12" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28">
         <v>10</v>
       </c>
@@ -1969,20 +1978,20 @@
         <v>42458</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28">
         <v>11</v>
       </c>
@@ -1995,16 +2004,18 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>190</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28">
         <v>12</v>
       </c>
@@ -2013,17 +2024,17 @@
         <v>42472</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28">
         <v>13</v>
       </c>
@@ -2032,15 +2043,15 @@
         <v>42479</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2052,14 +2063,14 @@
         <v>57</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2068,18 +2079,18 @@
         <v>42493</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2088,18 +2099,20 @@
         <v>42500</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>102</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>188</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2110,24 +2123,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9095851B-4B9F-8945-8A91-05442CABAD87}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="D1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="39.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="41.125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="35.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="4" max="4" width="25.09765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.59765625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="26.8984375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="39.59765625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="41.09765625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="35.09765625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2156,7 +2169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="317.39999999999998" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -2185,7 +2198,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="185.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -2215,7 +2228,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28">
         <v>3</v>
       </c>
@@ -2243,7 +2256,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
         <v>4</v>
       </c>
@@ -2271,7 +2284,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28">
         <v>5</v>
       </c>
@@ -2301,7 +2314,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28">
         <v>6</v>
       </c>
@@ -2331,7 +2344,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="198.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28">
         <v>7</v>
       </c>
@@ -2361,7 +2374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="132.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28">
         <v>8</v>
       </c>
@@ -2387,7 +2400,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="23"/>
@@ -2398,7 +2411,7 @@
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2427,7 +2440,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="294" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="304.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2453,7 +2466,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2477,7 +2490,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2503,7 +2516,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="132.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2525,7 +2538,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2545,7 +2558,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2563,7 +2576,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -2593,19 +2606,19 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="34"/>
+    <col min="1" max="1" width="8.8984375" style="34"/>
     <col min="2" max="2" width="38" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="19"/>
-    <col min="5" max="5" width="5.125" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.8984375" style="19"/>
+    <col min="5" max="5" width="5.09765625" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="12"/>
+    <col min="8" max="8" width="8.8984375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -2628,12 +2641,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2649,12 +2662,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2670,12 +2683,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2691,12 +2704,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2712,15 +2725,15 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31">
         <v>0.1</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6"/>
       <c r="G6" s="16">
@@ -2728,467 +2741,467 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31">
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>1.2</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="31">
         <v>1.3</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
-        <v>116</v>
-      </c>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
         <v>2.2999999999999998</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
         <v>3.2</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>3.3</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="31"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="31"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="31"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="31"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="31"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="31"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="31"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="31"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="31"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="31"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="31"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="31"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="31"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="31"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="17"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="31"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="31"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="31"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="31"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="31"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="31"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="31"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="17"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="31"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="17"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="31"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="17"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="31"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="17"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="31"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="17"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="31"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="17"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="31"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="17"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="31"/>
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="17"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="31"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="17"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="31"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="17"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="31"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="17"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="31"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="17"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="31"/>
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="17"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="31"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="17"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="31"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="17"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="31"/>
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="17"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="31"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="17"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="31"/>
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
@@ -3198,7 +3211,7 @@
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="31"/>
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
@@ -3208,106 +3221,106 @@
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="31"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
       <c r="E66" s="20"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="31"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="20"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="31"/>
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="17"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="31"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="17"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="31"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="17"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="31"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
       <c r="E71" s="17"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="31"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="17"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="31"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="17"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="31"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="32"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
       <c r="D75" s="21"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="32"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
       <c r="D76" s="21"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="32"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
       <c r="D77" s="21"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="32"/>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="32"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
       <c r="D79" s="21"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="32"/>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
       <c r="D80" s="21"/>
       <c r="E80" s="18"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="32"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
@@ -3316,14 +3329,14 @@
       <c r="G81"/>
       <c r="H81"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="32"/>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
       <c r="D82" s="21"/>
       <c r="E82" s="18"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="32"/>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
@@ -3331,7 +3344,7 @@
       <c r="G83"/>
       <c r="H83"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="32"/>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
@@ -3339,7 +3352,7 @@
       <c r="G84"/>
       <c r="H84"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="32"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
@@ -3347,7 +3360,7 @@
       <c r="G85"/>
       <c r="H85"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="32"/>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
@@ -3355,7 +3368,7 @@
       <c r="G86"/>
       <c r="H86"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="32"/>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
@@ -3363,7 +3376,7 @@
       <c r="G87"/>
       <c r="H87"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="32"/>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
@@ -3371,7 +3384,7 @@
       <c r="G88"/>
       <c r="H88"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="32"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -3379,7 +3392,7 @@
       <c r="G89"/>
       <c r="H89"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="32"/>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -3387,37 +3400,37 @@
       <c r="G90"/>
       <c r="H90"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="32"/>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
       <c r="D91" s="21"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="32"/>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
       <c r="D92" s="21"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="32"/>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
       <c r="D93" s="21"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="32"/>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
       <c r="D94" s="21"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="32"/>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
       <c r="D95" s="21"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="33"/>
       <c r="B96" s="22"/>
       <c r="D96" s="22"/>

</xml_diff>

<commit_message>
add link to assignment
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C9D57E-DECA-44BA-969D-7ECA61CFEAFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16E10D9-5E3B-4E8C-AA17-6FD7A5CB540F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-120" windowWidth="18405" windowHeight="6255" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -791,7 +791,7 @@
 Doing Data Science Ch 5</t>
   </si>
   <si>
-    <t xml:space="preserve">[Classification Assignment]( ) (Due 04/18)  </t>
+    <t xml:space="preserve">[Classification Assignment](https://classroom.github.com/a/8AQxyAIa ) (Due 04/18)  </t>
   </si>
 </sst>
 </file>
@@ -1656,7 +1656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add wk14 and rebuild latest lec notes
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9D9E5F-8CD9-4ABC-ABA2-E2C90C2683A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049FE9C4-B36E-456C-AB42-69A8E5A53A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="18405" windowHeight="6255" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="197">
   <si>
     <t>Finals Week</t>
   </si>
@@ -473,9 +481,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Read WMD: Intro, Ch 1-2</t>
-  </si>
-  <si>
     <t>Community Coding</t>
   </si>
   <si>
@@ -715,13 +720,6 @@
 Read ISLR Ch 3.5</t>
   </si>
   <si>
-    <t>ISLR Ch 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethics of ML algorithms
-</t>
-  </si>
-  <si>
     <t>Twitter project updates and next steps. Task identification</t>
   </si>
   <si>
@@ -745,9 +743,6 @@
   </si>
   <si>
     <t>[Text analysis assignment](https://classroom.github.com/a/t2Wt4CIJ) (Draft due Tue 4/7, Final 4/9 )</t>
-  </si>
-  <si>
-    <t>NLP - Predictive analytics/Topic modeling</t>
   </si>
   <si>
     <t>[Week 9 Notes](lec/wk09-notes.html)</t>
@@ -761,16 +756,7 @@
     <t>Watch at least one recap video (links in Wk 11 notes)</t>
   </si>
   <si>
-    <t>Finals week</t>
-  </si>
-  <si>
     <t>Presentation slides- through Methods (Due 4/12 )</t>
-  </si>
-  <si>
-    <t>Presentation slides- through EDA/bivariate results (Due 4/26 )</t>
-  </si>
-  <si>
-    <t>Presentation slides-finish (Due 5/3 , PR 5/6 )</t>
   </si>
   <si>
     <t>[Week 11 Notes](lec/wk11-notes.html)  
@@ -797,6 +783,38 @@
   <si>
     <t>Presentation slides- through Univariate Results (Due 4/19 , PR 4/22)
 Resampling homework (Due 4/28 )</t>
+  </si>
+  <si>
+    <t>[Weapons of Math Destruction Discussion Questions](read/WMD_Discussion_Questions.html)
+[Notes on Tree based models](lec09-tree-models.html)</t>
+  </si>
+  <si>
+    <t>[Week 14 Notes](lec/wk14-notes.html)</t>
+  </si>
+  <si>
+    <t>Tree based methods
+Ethics</t>
+  </si>
+  <si>
+    <t>ISLR CH 8
+Weapons of Math Destruction</t>
+  </si>
+  <si>
+    <t>Final Presentations</t>
+  </si>
+  <si>
+    <t>Presentation slides-finish (Due 5/3 , PR 5/6 )
+Learning journal assignment (Due 5/7 )
+WMD Ch 2-3 reflection question (Due 5/8 )</t>
+  </si>
+  <si>
+    <t>Presentation slides- through EDA/bivariate results (Due 4/26 )
+WMD Intro-Ch1 reflection questions (Due 5/1 )</t>
+  </si>
+  <si>
+    <t>Final Presentation 6-8pm Wednesday
+WMD Ch 4-5 OR 6-7 reflection question (Due 5/15 )
+[CART assignment]() (Due 5/15 )</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1123,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1211,9 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1664,7 +1679,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1721,13 +1736,13 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I2" s="9"/>
     </row>
@@ -1741,14 +1756,14 @@
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1760,23 +1775,23 @@
         <v>42395</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1788,23 +1803,23 @@
         <v>42402</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1816,23 +1831,23 @@
         <v>42409</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1844,23 +1859,23 @@
         <v>42416</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1872,21 +1887,21 @@
         <v>42423</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1898,29 +1913,29 @@
         <v>42430</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39">
+      <c r="A10" s="38">
         <v>8</v>
       </c>
       <c r="B10" s="3">
@@ -1931,20 +1946,20 @@
         <v>34</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1972,20 +1987,20 @@
         <v>42451</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="H12" s="40" t="s">
-        <v>169</v>
+        <v>172</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>168</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -1998,16 +2013,16 @@
         <v>42458</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>169</v>
+      <c r="H13" s="39" t="s">
+        <v>168</v>
       </c>
       <c r="I13" s="4"/>
     </row>
@@ -2024,13 +2039,13 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -2044,17 +2059,17 @@
         <v>42472</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2067,11 +2082,11 @@
         <f>B15+7</f>
         <v>42479</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>193</v>
+      <c r="C16" s="40" t="s">
+        <v>186</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -2084,19 +2099,24 @@
         <f>B16+7</f>
         <v>42486</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="F17" s="6"/>
+      <c r="C17" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="G17" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H17" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="H17" s="40" t="s">
-        <v>194</v>
-      </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2104,20 +2124,19 @@
         <f>B17+7</f>
         <v>42493</v>
       </c>
-      <c r="C18" s="38" t="s">
-        <v>57</v>
+      <c r="C18" s="40" t="s">
+        <v>191</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="G18" s="4" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -2129,16 +2148,14 @@
         <v>42500</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
@@ -2154,8 +2171,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2676,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2697,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2718,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2739,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2760,10 +2777,10 @@
         <v>0.1</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6"/>
       <c r="G6" s="16">
@@ -2776,10 +2793,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D7"/>
     </row>
@@ -2788,10 +2805,10 @@
         <v>1.2</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8"/>
     </row>
@@ -2800,10 +2817,10 @@
         <v>1.3</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9"/>
     </row>
@@ -2812,10 +2829,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
         <v>114</v>
-      </c>
-      <c r="C10" t="s">
-        <v>115</v>
       </c>
       <c r="D10"/>
     </row>
@@ -2824,10 +2841,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11"/>
       <c r="G11"/>
@@ -2837,10 +2854,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12"/>
       <c r="G12"/>
@@ -2850,10 +2867,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13"/>
       <c r="G13"/>
@@ -2863,10 +2880,10 @@
         <v>3.1</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14"/>
       <c r="G14"/>
@@ -2876,10 +2893,10 @@
         <v>3.2</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15"/>
       <c r="G15"/>
@@ -2889,10 +2906,10 @@
         <v>3.3</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D16"/>
       <c r="G16"/>
@@ -2902,10 +2919,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17"/>
       <c r="G17"/>
@@ -2915,10 +2932,10 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18"/>
       <c r="H18" s="19"/>
@@ -2928,10 +2945,10 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19"/>
       <c r="H19" s="19"/>
@@ -2941,7 +2958,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2952,10 +2969,10 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D21"/>
       <c r="G21"/>
@@ -3466,7 +3483,7 @@
       <c r="D96" s="22"/>
     </row>
   </sheetData>
-  <sortState ref="A2:C96">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
     <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add lec09 question start
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049FE9C4-B36E-456C-AB42-69A8E5A53A3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508FCC5F-DEBF-4847-B3EF-78D2565D12C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="720" windowWidth="24135" windowHeight="15030" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -803,18 +803,18 @@
     <t>Final Presentations</t>
   </si>
   <si>
-    <t>Presentation slides-finish (Due 5/3 , PR 5/6 )
-Learning journal assignment (Due 5/7 )
-WMD Ch 2-3 reflection question (Due 5/8 )</t>
-  </si>
-  <si>
-    <t>Presentation slides- through EDA/bivariate results (Due 4/26 )
-WMD Intro-Ch1 reflection questions (Due 5/1 )</t>
-  </si>
-  <si>
     <t>Final Presentation 6-8pm Wednesday
 WMD Ch 4-5 OR 6-7 reflection question (Due 5/15 )
 [CART assignment]() (Due 5/15 )</t>
+  </si>
+  <si>
+    <t>Presentation slides- through EDA/bivariate results (Due 4/26 )
+WMD Intro-Ch1 reflection questions (Due 5/4 )</t>
+  </si>
+  <si>
+    <t>Presentation slides-finish (Due 5/3 , PR 5/6 )
+Learning journal assignment (Due 5/7 )
+WMD Ch 2-3 reflection question (Due 5/6 )</t>
   </si>
 </sst>
 </file>
@@ -1678,8 +1678,8 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2132,7 @@
         <v>189</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
@@ -2154,7 +2154,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -2171,7 +2171,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
first overhaul for spring 22
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7399464-1579-4796-8AAC-391D67558AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6DD67A-08AA-4C55-A3AB-B3E679BFE04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="720" windowWidth="24135" windowHeight="15030" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="schedule_s18" sheetId="4" r:id="rId2"/>
-    <sheet name="assignments" sheetId="3" r:id="rId3"/>
+    <sheet name="schedule_20" sheetId="5" r:id="rId2"/>
+    <sheet name="schedule_s18" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="167">
   <si>
     <t>Finals Week</t>
   </si>
@@ -128,18 +128,6 @@
   </si>
   <si>
     <t>Introduction to Statistical Learning</t>
-  </si>
-  <si>
-    <t>Assignment</t>
-  </si>
-  <si>
-    <t>Discussion</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>%</t>
   </si>
   <si>
     <t>* ISLR MOOC [Video lectures](http://www.dataschool.io/15-hours-of-expert-machine-learning-videos/)
@@ -226,15 +214,6 @@
   <si>
     <t xml:space="preserve">* Create and evaluate a prediction model using linear regression. 
 * Identify cases where a non-parametric approach would be more appropriate than a parametric approach. </t>
-  </si>
-  <si>
-    <t>Catgory</t>
-  </si>
-  <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>Learning</t>
   </si>
   <si>
     <t xml:space="preserve">* You're going to use Hugo/Blogdown to create a professional looking website. 
@@ -481,27 +460,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Community Coding</t>
-  </si>
-  <si>
-    <t>DataFest</t>
-  </si>
-  <si>
-    <t>Reflect on DDS case study (n=5)</t>
-  </si>
-  <si>
-    <t>Share DDS Case study (n=1)</t>
-  </si>
-  <si>
-    <t>WMD Reflections</t>
-  </si>
-  <si>
-    <t>Blog posts (5) on external topics of interest</t>
-  </si>
-  <si>
-    <t>Comments on Blog posts</t>
-  </si>
-  <si>
     <t>Intro to Statistical Learning</t>
   </si>
   <si>
@@ -513,12 +471,6 @@
   </si>
   <si>
     <t>What is Data Science?  What's your DS path?</t>
-  </si>
-  <si>
-    <t>What is DS - hack notes</t>
-  </si>
-  <si>
-    <t>participation</t>
   </si>
   <si>
     <t xml:space="preserve">Lec00
@@ -532,18 +484,6 @@
     <t xml:space="preserve">Read DDS Ch1, 16.   </t>
   </si>
   <si>
-    <t>Slack Intro</t>
-  </si>
-  <si>
-    <t>HW2: Share content</t>
-  </si>
-  <si>
-    <t>HW2: reflect on others share</t>
-  </si>
-  <si>
-    <t>Grade POLS Learn R HW (4 x 2 students ea. )</t>
-  </si>
-  <si>
     <t>Blogdown
 Interactive lecture 02 (Hack MD)</t>
   </si>
@@ -579,39 +519,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hackathon / open work time. </t>
-  </si>
-  <si>
-    <t>HW1: R Markdown website demo</t>
-  </si>
-  <si>
-    <t>HW1: Blogdown website demo</t>
-  </si>
-  <si>
-    <t>HW1: Personal website</t>
-  </si>
-  <si>
-    <t>HW3: Twitter tutorial for others</t>
-  </si>
-  <si>
-    <t>HW3: Historical twitter data demo</t>
-  </si>
-  <si>
-    <t>HW3: Sentiment analysis</t>
-  </si>
-  <si>
-    <t>What is DS mind map share out</t>
-  </si>
-  <si>
-    <t>Add info to class-logsitics repo via PR</t>
-  </si>
-  <si>
-    <t>knowledge</t>
-  </si>
-  <si>
-    <t>communication</t>
-  </si>
-  <si>
-    <t>skills</t>
   </si>
   <si>
     <t>Statistical Inference, Exploratory Data Analysis, and the Data Science Process</t>
@@ -816,14 +723,24 @@
 WMD Ch 4-5 OR 6-7 reflection question (Due 5/15 )
 CART assignment [[HTML]](hw09-CART-assignment.html)[[RMD]](hw09-CART-assignment.Rmd) (Due 5/15 )</t>
   </si>
+  <si>
+    <t>Showcase your work</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -872,33 +789,18 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -945,7 +847,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -997,26 +899,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
@@ -1028,219 +910,176 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="89" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="89" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="90" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="92" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="91" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="92">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1284,7 +1123,6 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Heading 2" xfId="91" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1329,11 +1167,11 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="91" xr:uid="{E2739FDE-9824-4AB0-B8BE-F333927EB0B9}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Percent" xfId="90" builtinId="5"/>
+    <cellStyle name="Normal 3" xfId="90" xr:uid="{F389B7EE-FBAE-444B-8207-B15B66A5DAE1}"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Total" xfId="92" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1675,11 +1513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1537,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>6</v>
@@ -1711,63 +1549,406 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>43124</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f>B2+7</f>
+        <v>43131</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f>B4+7</f>
+        <v>43138</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ref="B6:B19" si="0">B5+7</f>
+        <v>43145</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ref="B7:B12" si="1">B6+7</f>
+        <v>43152</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="1"/>
+        <v>43159</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="1"/>
+        <v>43166</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="1"/>
+        <v>43173</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="13">
+        <f t="shared" si="1"/>
+        <v>43180</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <v>9</v>
+      </c>
+      <c r="B12" s="18">
+        <f t="shared" si="1"/>
+        <v>43187</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B12+7</f>
+        <v>43194</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>43201</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>43208</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B15+7</f>
+        <v>43215</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B16+7</f>
+        <v>43222</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
+        <f>B17+7</f>
+        <v>43229</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>43236</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A93E5A-BA74-42D3-BD28-1405D627EC9E}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="39.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="41.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="37.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="31.625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>42388</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="3"/>
       <c r="C3" s="10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -1775,27 +1956,27 @@
         <v>42395</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="H4" s="9" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
       <c r="B5" s="3">
@@ -1803,209 +1984,209 @@
         <v>42402</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="4" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <f t="shared" ref="B6:B19" si="0">B5+7</f>
         <v>42409</v>
       </c>
-      <c r="C6" s="35" t="s">
-        <v>143</v>
+      <c r="C6" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="9" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7:B12" si="1">B6+7</f>
+        <f t="shared" si="0"/>
         <v>42416</v>
       </c>
-      <c r="C7" s="35" t="s">
-        <v>142</v>
+      <c r="C7" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="9" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36">
+      <c r="A8" s="20">
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42423</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="4" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42430</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>166</v>
+        <v>129</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38">
+      <c r="A10" s="22">
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42437</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="24">
-        <f t="shared" si="1"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="13">
+        <f t="shared" si="0"/>
         <v>42444</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="C11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28">
+      <c r="A12" s="17">
         <v>9</v>
       </c>
-      <c r="B12" s="29">
-        <f t="shared" si="1"/>
+      <c r="B12" s="18">
+        <f t="shared" si="0"/>
         <v>42451</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>168</v>
+        <v>141</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>137</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28">
+      <c r="A13" s="17">
         <v>10</v>
       </c>
       <c r="B13" s="3">
@@ -2013,21 +2194,21 @@
         <v>42458</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>168</v>
+        <v>146</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>137</v>
       </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28">
+      <c r="A14" s="17">
         <v>11</v>
       </c>
       <c r="B14" s="3">
@@ -2035,23 +2216,23 @@
         <v>42465</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G14" s="37" t="s">
-        <v>183</v>
+        <v>151</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>152</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28">
+      <c r="A15" s="17">
         <v>12</v>
       </c>
       <c r="B15" s="3">
@@ -2059,34 +2240,34 @@
         <v>42472</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>184</v>
+        <v>144</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28">
+      <c r="A16" s="17">
         <v>13</v>
       </c>
       <c r="B16" s="3">
         <f>B15+7</f>
         <v>42479</v>
       </c>
-      <c r="C16" s="40" t="s">
-        <v>186</v>
+      <c r="C16" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -2099,20 +2280,20 @@
         <f>B16+7</f>
         <v>42486</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>192</v>
+      <c r="C17" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>161</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>187</v>
+        <v>163</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>156</v>
       </c>
       <c r="I17" s="4"/>
     </row>
@@ -2124,19 +2305,19 @@
         <f>B17+7</f>
         <v>42493</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>191</v>
+      <c r="C18" s="24" t="s">
+        <v>160</v>
       </c>
       <c r="D18" s="4"/>
       <c r="F18" s="6" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2148,13 +2329,13 @@
         <v>42500</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="4" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -2166,13 +2347,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9095851B-4B9F-8945-8A91-05442CABAD87}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2204,7 +2385,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
@@ -2217,7 +2398,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="306.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
       <c r="B2" s="3">
@@ -2233,20 +2414,20 @@
         <v>18</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="179.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
       <c r="B3" s="3">
@@ -2254,7 +2435,7 @@
         <v>42397</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
@@ -2263,20 +2444,20 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="198.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
       <c r="B4" s="3">
@@ -2290,7 +2471,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>16</v>
@@ -2300,11 +2481,11 @@
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="166.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
       <c r="B5" s="3">
@@ -2312,27 +2493,27 @@
         <v>42411</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="268.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -2343,26 +2524,26 @@
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
       <c r="B7" s="3">
@@ -2370,29 +2551,29 @@
         <v>42425</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="192" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
       <c r="B8" s="3">
@@ -2400,29 +2581,29 @@
         <v>42432</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="9" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="3">
@@ -2430,33 +2611,33 @@
         <v>42439</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="141" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -2466,25 +2647,25 @@
         <v>41724</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="294" thickBot="1" x14ac:dyDescent="0.3">
@@ -2496,21 +2677,21 @@
         <v>41731</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2522,19 +2703,19 @@
         <v>41738</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
       <c r="H13" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2546,21 +2727,21 @@
         <v>41745</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2572,16 +2753,16 @@
         <v>41752</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -2594,11 +2775,11 @@
         <v>41759</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
@@ -2614,7 +2795,7 @@
         <v>41766</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2643,850 +2824,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H96"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.875" style="34"/>
-    <col min="2" max="2" width="38" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="19"/>
-    <col min="5" max="5" width="5.125" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="10" style="12" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="12">
-        <f>SUMIF($C$2:$C$87,F2,$D$2:$D$87)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="15" t="e">
-        <f>G2/$G$6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="12">
-        <f>SUMIF($C$2:$C$87,F3,$D$2:$D$87)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="15" t="e">
-        <f>G3/$G$6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="12">
-        <f>SUMIF($C$2:$C$87,F4,$D$2:$D$87)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="15" t="e">
-        <f>G4/$G$6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="12">
-        <f>SUMIF($C$2:$C$87,F5,$D$2:$D$87)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="15" t="e">
-        <f>G5/$G$6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6"/>
-      <c r="G6" s="16">
-        <f>SUM(G2:G5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
-        <v>1.2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>1.3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11"/>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12"/>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D13"/>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
-        <v>3.1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14"/>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
-        <v>3.2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" t="s">
-        <v>141</v>
-      </c>
-      <c r="D15"/>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
-        <v>3.3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16"/>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17"/>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18"/>
-      <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="31">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21"/>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="17"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="17"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="17"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="17"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="17"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="17"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="31"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="17"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="31"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="17"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="17"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="17"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="31"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="31"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="17"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="17"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="31"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="20"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="20"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="17"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="17"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="32"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="32"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="32"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="18"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="32"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
-      <c r="E81" s="18"/>
-      <c r="G81"/>
-      <c r="H81"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="32"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="18"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="32"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
-      <c r="G83"/>
-      <c r="H83"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="32"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
-      <c r="G84"/>
-      <c r="H84"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="32"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
-      <c r="G85"/>
-      <c r="H85"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
-      <c r="G86"/>
-      <c r="H86"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="32"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
-      <c r="G87"/>
-      <c r="H87"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="32"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
-      <c r="G88"/>
-      <c r="H88"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="32"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="21"/>
-      <c r="G89"/>
-      <c r="H89"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="32"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
-      <c r="G90"/>
-      <c r="H90"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="32"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="32"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="32"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="32"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="21"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="33"/>
-      <c r="B96" s="22"/>
-      <c r="D96" s="22"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
-    <sortCondition ref="A2:A96"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add project info,start wk5 content add eval criteria to week 4
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6EDDB9-BB6C-4E2D-A43C-0682E0CB39FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979832D6-52D5-42E5-BE21-DB2038BBEEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="171">
   <si>
     <t>SLO</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>ISLR Ch2 Exercises: 1, 2, 4 (one example each)</t>
-  </si>
-  <si>
-    <t>Forming a mathematical model to a business question.</t>
   </si>
   <si>
     <t>github classroom</t>
@@ -458,9 +455,6 @@
     <t>Real estate case study: Stakeholder report (draft)</t>
   </si>
   <si>
-    <t>Real estate case study: Stakeholder report (final as blog post)</t>
-  </si>
-  <si>
     <t>Create a data strategy to address a business question.</t>
   </si>
   <si>
@@ -498,22 +492,7 @@
     <t>https://hackmd.io/@norcalbiostat/whatisds</t>
   </si>
   <si>
-    <t>(Team Assignment - Don't accpet until Tuesday in class) https://classroom.github.com/a/KowEWfPm</t>
-  </si>
-  <si>
-    <t>Your website</t>
-  </si>
-  <si>
-    <t>Submit a PR to ADS website with student team roster</t>
-  </si>
-  <si>
     <t>https://github.com/norcalbiostat/ADS</t>
-  </si>
-  <si>
-    <t>Data485 Github organization</t>
-  </si>
-  <si>
-    <t>Create shared private repo, team expectations &amp; workflow in README</t>
   </si>
   <si>
     <t>Learning Journal, [RAT discussion guide](notes/RAT Discussion guide.pdf)</t>
@@ -523,12 +502,6 @@
   </si>
   <si>
     <t>Read Introduction and answer assigned question in HackMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete data security training.  
-1. Review the information on [this page](https://www.csuchico.edu/isec/data-protection/index.shtml)  
-2. Complete the Data Security and FERPA (Non-Level 1) training through [CSU Learn](https://www.csuchico.edu/hr/pdev/compliance-training.shtml)   
-3. Send a copy of your certificate to Dr. D. </t>
   </si>
   <si>
     <t>The New Jim Code</t>
@@ -567,6 +540,36 @@
   </si>
   <si>
     <t>[2](wk02-notes.html)</t>
+  </si>
+  <si>
+    <t>[5](wk05-notes.html)</t>
+  </si>
+  <si>
+    <t>[Jigsaw Notes: HackMD](https://hackmd.io/@norcalbiostat/rat-intro)</t>
+  </si>
+  <si>
+    <t>[Github classroom Team Assignment](https://classroom.github.com/a/KowEWfPm)</t>
+  </si>
+  <si>
+    <t>Send final report to Dr. D via Discord</t>
+  </si>
+  <si>
+    <t>Submit a PR to ADS website with student team roster on your assigned project page</t>
+  </si>
+  <si>
+    <t>Obtain shared private repo. Follow instructions in README</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github classroom link in Discord. Pay attention to naming request. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete data security training.  </t>
+  </si>
+  <si>
+    <t>Week 5 notes</t>
+  </si>
+  <si>
+    <t>Real estate case study: Final Stakeholder report. Evaluation rubric in week 4 notes.</t>
   </si>
 </sst>
 </file>
@@ -813,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -951,9 +954,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -975,9 +975,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -986,6 +983,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="92" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1083,7 +1101,37 @@
     <cellStyle name="Normal 3 2" xfId="91" xr:uid="{20B637C8-DD27-499C-BEC0-85B72C712ADD}"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1436,9 +1484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1504,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -1468,13 +1516,13 @@
         <v>0</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="30" t="s">
         <v>2</v>
@@ -1485,29 +1533,29 @@
     </row>
     <row r="2" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B2" s="32">
         <v>43124</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1516,76 +1564,76 @@
         <v>43126</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="37"/>
       <c r="I3" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B4" s="39">
         <v>43131</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>129</v>
-      </c>
       <c r="H4" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B5" s="32">
         <v>43138</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I5" s="43"/>
     </row>
@@ -1601,71 +1649,71 @@
       <c r="E6" s="44"/>
       <c r="F6" s="44"/>
       <c r="G6" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H6" s="44"/>
       <c r="I6" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B7" s="32">
         <v>43145</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="35">
+        <v>43147</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>161</v>
-      </c>
-      <c r="I7" s="43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="32">
-        <v>43147</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>5</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="43" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
@@ -1677,19 +1725,19 @@
       <c r="A10" s="31"/>
       <c r="B10" s="32"/>
       <c r="C10" s="43" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="43"/>
       <c r="I10" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="126" x14ac:dyDescent="0.25">
@@ -1698,13 +1746,13 @@
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="43" t="s">
         <v>109</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>110</v>
       </c>
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
@@ -1721,13 +1769,13 @@
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
@@ -1744,7 +1792,7 @@
       </c>
       <c r="D13" s="47"/>
       <c r="E13" s="43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F13" s="47"/>
       <c r="G13" s="43"/>
@@ -1761,7 +1809,7 @@
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
@@ -1777,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
@@ -1795,7 +1843,7 @@
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
@@ -1808,11 +1856,11 @@
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
@@ -1829,7 +1877,7 @@
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
@@ -1842,11 +1890,11 @@
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F19" s="43"/>
       <c r="G19" s="43"/>
@@ -1855,14 +1903,14 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="32"/>
       <c r="C20" s="43" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="43"/>
       <c r="F20" s="43"/>
@@ -1879,16 +1927,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBC2D3D-FE18-4FBF-825C-8A0A6D387E1B}">
-  <dimension ref="A1:R1055"/>
+  <dimension ref="A1:R1054"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="6"/>
-    <col min="2" max="2" width="9" style="10"/>
+    <col min="1" max="2" width="9" style="60"/>
     <col min="3" max="3" width="22.875" style="18" customWidth="1"/>
     <col min="4" max="4" width="46.625" style="13" customWidth="1"/>
     <col min="5" max="5" width="15.375" style="22" bestFit="1" customWidth="1"/>
@@ -1900,10 +1947,10 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>17</v>
@@ -1912,7 +1959,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>23</v>
@@ -1935,23 +1982,23 @@
       <c r="R1" s="11"/>
     </row>
     <row r="2" spans="1:18" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
-      <c r="B2" s="49">
+      <c r="B2" s="59">
         <v>1</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53" t="s">
+      <c r="D2" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="54">
+      <c r="E2" s="51"/>
+      <c r="F2" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="53">
         <v>43125</v>
       </c>
       <c r="H2" s="48">
@@ -1969,21 +2016,23 @@
       <c r="R2" s="11"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="48">
+      <c r="A3" s="59">
         <v>1</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="59">
         <v>2</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51" t="s">
+      <c r="C3" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="54">
+      <c r="E3" s="51"/>
+      <c r="F3" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="53">
         <v>43125</v>
       </c>
       <c r="H3" s="48">
@@ -2001,21 +2050,23 @@
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="48">
+      <c r="A4" s="59">
         <v>1</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="59">
         <v>3</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="54">
+      <c r="C4" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="51"/>
+      <c r="F4" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="53">
         <v>43125</v>
       </c>
       <c r="H4" s="48">
@@ -2033,21 +2084,23 @@
       <c r="R4" s="11"/>
     </row>
     <row r="5" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="48">
+      <c r="A5" s="59">
         <v>1</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="59">
         <v>4</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51" t="s">
+      <c r="C5" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="51"/>
+      <c r="F5" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="54">
+      <c r="G5" s="53">
         <v>43125</v>
       </c>
       <c r="H5" s="48">
@@ -2065,21 +2118,23 @@
       <c r="R5" s="11"/>
     </row>
     <row r="6" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="48">
+      <c r="A6" s="59">
         <v>1</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="59">
         <v>5</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="54">
+      <c r="C6" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="F6" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="53">
         <v>43125</v>
       </c>
       <c r="H6" s="48">
@@ -2097,21 +2152,23 @@
       <c r="R6" s="11"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="48">
+      <c r="A7" s="59">
         <v>1</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="59">
         <v>6</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="54">
+      <c r="C7" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="51"/>
+      <c r="F7" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="53">
         <v>43125</v>
       </c>
       <c r="H7" s="48">
@@ -2129,21 +2186,23 @@
       <c r="R7" s="11"/>
     </row>
     <row r="8" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48">
+      <c r="A8" s="59">
         <v>1</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="59">
         <v>7</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="54">
+      <c r="C8" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="51"/>
+      <c r="F8" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="53">
         <v>43127</v>
       </c>
       <c r="H8" s="48">
@@ -2161,21 +2220,23 @@
       <c r="R8" s="11"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="48">
+      <c r="A9" s="59">
         <v>1</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="59">
         <v>8</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51" t="s">
+      <c r="C9" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="54">
+      <c r="E9" s="51"/>
+      <c r="F9" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="53">
         <v>43125</v>
       </c>
       <c r="H9" s="48">
@@ -2193,25 +2254,25 @@
       <c r="R9" s="11"/>
     </row>
     <row r="10" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="48">
+      <c r="A10" s="59">
         <v>1</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="59">
         <v>9</v>
       </c>
-      <c r="C10" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="52">
+      <c r="C10" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="51">
         <v>2</v>
       </c>
-      <c r="F10" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G10" s="54">
+      <c r="F10" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="53">
         <v>43132</v>
       </c>
       <c r="H10" s="48">
@@ -2229,14 +2290,14 @@
       <c r="R10" s="11"/>
     </row>
     <row r="11" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="60">
         <v>2</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="60">
         <v>1</v>
       </c>
-      <c r="C11" s="58" t="s">
-        <v>52</v>
+      <c r="C11" s="56" t="s">
+        <v>51</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>21</v>
@@ -2245,7 +2306,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G11" s="5">
         <v>43137</v>
@@ -2264,14 +2325,16 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+    <row r="12" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="60">
         <v>2</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="60">
         <v>2</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="56" t="s">
+        <v>51</v>
+      </c>
       <c r="D12" s="4" t="s">
         <v>22</v>
       </c>
@@ -2279,7 +2342,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G12" s="5">
         <v>43137</v>
@@ -2299,23 +2362,23 @@
       <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="60">
         <v>2</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="60">
         <v>3</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="21">
         <v>6</v>
       </c>
-      <c r="F13" s="60" t="s">
-        <v>146</v>
+      <c r="F13" s="58" t="s">
+        <v>144</v>
       </c>
       <c r="G13" s="5">
         <v>43133</v>
@@ -2335,21 +2398,23 @@
       <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="60">
         <v>2</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="60">
         <v>4</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="21">
         <v>7</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G14" s="5">
         <v>43137</v>
@@ -2369,21 +2434,23 @@
       <c r="R14" s="11"/>
     </row>
     <row r="15" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="60">
         <v>2</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="60">
         <v>5</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E15" s="21">
         <v>7</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="5">
         <v>43134</v>
@@ -2403,21 +2470,23 @@
       <c r="R15" s="11"/>
     </row>
     <row r="16" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="60">
         <v>2</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="60">
         <v>6</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D16" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" s="21">
         <v>7</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="5">
         <v>43137</v>
@@ -2437,21 +2506,23 @@
       <c r="R16" s="11"/>
     </row>
     <row r="17" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="60">
         <v>2</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="60">
         <v>7</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="21">
         <v>2</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" s="5">
         <v>43141</v>
@@ -2470,21 +2541,24 @@
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="18" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="60">
         <v>2</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="60">
         <v>8</v>
       </c>
+      <c r="C18" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D18" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E18" s="21">
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="5">
         <v>43144</v>
@@ -2504,29 +2578,29 @@
       <c r="R18" s="11"/>
     </row>
     <row r="19" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="48">
+      <c r="A19" s="59">
         <v>3</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="59">
         <v>1</v>
       </c>
-      <c r="C19" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="52">
+      <c r="C19" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="51">
         <v>5</v>
       </c>
-      <c r="F19" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="G19" s="54">
+      <c r="F19" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" s="53">
         <v>43145</v>
       </c>
       <c r="H19" s="48">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -2539,28 +2613,28 @@
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
     </row>
-    <row r="20" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="48">
+    <row r="20" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="59">
         <v>3</v>
       </c>
-      <c r="B20" s="49">
-        <v>2</v>
-      </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="52">
-        <v>5</v>
-      </c>
-      <c r="F20" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="G20" s="54">
-        <v>43151</v>
+      <c r="B20" s="59">
+        <v>3</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="51"/>
+      <c r="F20" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="53">
+        <v>43143</v>
       </c>
       <c r="H20" s="48">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
@@ -2573,28 +2647,28 @@
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
     </row>
-    <row r="21" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="48">
-        <v>3</v>
-      </c>
-      <c r="B21" s="49">
-        <v>3</v>
-      </c>
-      <c r="C21" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="54">
-        <v>43143</v>
-      </c>
-      <c r="H21" s="48">
-        <v>10</v>
+    <row r="21" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="60">
+        <v>4</v>
+      </c>
+      <c r="B21" s="60">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="5">
+        <v>43146</v>
+      </c>
+      <c r="H21" s="6">
+        <v>20</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -2608,27 +2682,29 @@
       <c r="R21" s="11"/>
     </row>
     <row r="22" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="61">
         <v>4</v>
       </c>
-      <c r="B22" s="10">
-        <v>1</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G22" s="5">
-        <v>43146</v>
-      </c>
-      <c r="H22" s="6">
-        <v>40</v>
+      <c r="B22" s="61">
+        <v>2</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>170</v>
+      </c>
+      <c r="E22" s="63">
+        <v>5</v>
+      </c>
+      <c r="F22" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="64">
+        <v>43151</v>
+      </c>
+      <c r="H22" s="65">
+        <v>50</v>
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -2641,25 +2717,28 @@
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
     </row>
-    <row r="23" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="10">
-        <v>2</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" s="5">
-        <v>43151</v>
-      </c>
-      <c r="H23" s="6">
-        <v>20</v>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="61">
+        <v>4</v>
+      </c>
+      <c r="B23" s="61">
+        <v>3</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="63"/>
+      <c r="F23" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="G23" s="64">
+        <v>43158</v>
+      </c>
+      <c r="H23" s="65">
+        <v>30</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
@@ -2673,22 +2752,27 @@
       <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
-        <v>3</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="60" t="s">
-        <v>150</v>
-      </c>
-      <c r="G24" s="5">
-        <v>43146</v>
-      </c>
-      <c r="H24" s="6">
-        <v>10</v>
+      <c r="A24" s="59">
+        <v>5</v>
+      </c>
+      <c r="B24" s="59">
+        <v>1</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51">
+        <v>5</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="53">
+        <v>43159</v>
+      </c>
+      <c r="H24" s="48">
+        <v>30</v>
       </c>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -2701,21 +2785,28 @@
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
     </row>
-    <row r="25" spans="1:18" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="10">
-        <v>4</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5">
-        <v>43158</v>
-      </c>
-      <c r="H25" s="6">
-        <v>40</v>
+    <row r="25" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="59">
+        <v>5</v>
+      </c>
+      <c r="B25" s="59">
+        <v>2</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="51"/>
+      <c r="F25" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25" s="53">
+        <v>43151</v>
+      </c>
+      <c r="H25" s="48">
+        <v>20</v>
       </c>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
@@ -2728,24 +2819,28 @@
       <c r="Q25" s="11"/>
       <c r="R25" s="11"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="48">
+    <row r="26" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="59">
         <v>5</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52">
-        <v>5</v>
-      </c>
-      <c r="F26" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="57"/>
+      <c r="B26" s="59">
+        <v>3</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="E26" s="51"/>
+      <c r="F26" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="G26" s="53">
+        <v>43153</v>
+      </c>
       <c r="H26" s="48">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
@@ -2758,24 +2853,28 @@
       <c r="Q26" s="11"/>
       <c r="R26" s="11"/>
     </row>
-    <row r="27" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27" s="52"/>
-      <c r="F27" s="51" t="s">
-        <v>154</v>
-      </c>
-      <c r="G27" s="54">
+    <row r="27" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="59">
+        <v>5</v>
+      </c>
+      <c r="B27" s="59">
+        <v>4</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="51"/>
+      <c r="F27" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" s="53">
         <v>43153</v>
       </c>
       <c r="H27" s="48">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -2789,18 +2888,18 @@
       <c r="R27" s="11"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="60">
         <v>6</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G28" s="7"/>
       <c r="I28" s="11"/>
@@ -2820,7 +2919,7 @@
         <v>25</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G29" s="7"/>
       <c r="I29" s="11"/>
@@ -2835,11 +2934,18 @@
       <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="17"/>
-      <c r="D30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="21"/>
+      <c r="A30" s="60">
+        <v>7</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
@@ -2853,17 +2959,12 @@
       <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>7</v>
-      </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>57</v>
-      </c>
       <c r="F31" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G31" s="7"/>
       <c r="I31" s="11"/>
@@ -2878,12 +2979,18 @@
       <c r="R31" s="11"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C32" s="17"/>
-      <c r="D32" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="A32" s="60">
+        <v>8</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="23"/>
       <c r="F32" s="13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="G32" s="7"/>
       <c r="I32" s="11"/>
@@ -2898,18 +3005,13 @@
       <c r="R32" s="11"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>8</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>58</v>
+      <c r="C33" s="19"/>
+      <c r="D33" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="E33" s="23"/>
       <c r="F33" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G33" s="7"/>
       <c r="I33" s="11"/>
@@ -2924,13 +3026,18 @@
       <c r="R33" s="11"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C34" s="19"/>
-      <c r="D34" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="23"/>
+      <c r="A34" s="60">
+        <v>9</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="21"/>
       <c r="F34" s="13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="G34" s="7"/>
       <c r="I34" s="11"/>
@@ -2945,18 +3052,13 @@
       <c r="R34" s="11"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>9</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>59</v>
+      <c r="C35" s="14"/>
+      <c r="D35" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G35" s="7"/>
       <c r="I35" s="11"/>
@@ -2971,13 +3073,18 @@
       <c r="R35" s="11"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C36" s="14"/>
-      <c r="D36" s="13" t="s">
-        <v>71</v>
+      <c r="A36" s="60">
+        <v>10</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="G36" s="7"/>
       <c r="I36" s="11"/>
@@ -2992,18 +3099,13 @@
       <c r="R36" s="11"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>10</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>60</v>
+      <c r="C37" s="14"/>
+      <c r="D37" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G37" s="7"/>
       <c r="I37" s="11"/>
@@ -3018,13 +3120,18 @@
       <c r="R37" s="11"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C38" s="14"/>
-      <c r="D38" s="13" t="s">
-        <v>72</v>
+      <c r="A38" s="60">
+        <v>11</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="G38" s="7"/>
       <c r="I38" s="11"/>
@@ -3039,18 +3146,13 @@
       <c r="R38" s="11"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
-        <v>11</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>61</v>
+      <c r="C39" s="14"/>
+      <c r="D39" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G39" s="7"/>
       <c r="I39" s="11"/>
@@ -3065,13 +3167,18 @@
       <c r="R39" s="11"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C40" s="14"/>
-      <c r="D40" s="13" t="s">
-        <v>73</v>
+      <c r="A40" s="60">
+        <v>12</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E40" s="21"/>
       <c r="F40" s="13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="G40" s="7"/>
       <c r="I40" s="11"/>
@@ -3086,18 +3193,13 @@
       <c r="R40" s="11"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
-        <v>12</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>62</v>
+      <c r="C41" s="14"/>
+      <c r="D41" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G41" s="7"/>
       <c r="I41" s="11"/>
@@ -3112,13 +3214,18 @@
       <c r="R41" s="11"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C42" s="14"/>
-      <c r="D42" s="13" t="s">
-        <v>74</v>
+      <c r="A42" s="60">
+        <v>13</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="E42" s="21"/>
       <c r="F42" s="13" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="G42" s="7"/>
       <c r="I42" s="11"/>
@@ -3133,18 +3240,13 @@
       <c r="R42" s="11"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>13</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>63</v>
+      <c r="C43" s="14"/>
+      <c r="D43" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="13" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="G43" s="7"/>
       <c r="I43" s="11"/>
@@ -3159,13 +3261,15 @@
       <c r="R43" s="11"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C44" s="14"/>
-      <c r="D44" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="13" t="s">
-        <v>27</v>
+      <c r="C44" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G44" s="7"/>
       <c r="I44" s="11"/>
@@ -3180,17 +3284,13 @@
       <c r="R44" s="11"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C45" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="C45" s="20"/>
       <c r="D45" s="12" t="s">
         <v>34</v>
       </c>
       <c r="E45" s="6"/>
-      <c r="F45" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="7"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
@@ -3204,11 +3304,11 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C46" s="20"/>
-      <c r="D46" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="12"/>
+      <c r="D46" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="8"/>
       <c r="G46" s="11"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
@@ -3224,7 +3324,7 @@
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C47" s="20"/>
       <c r="D47" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E47" s="21"/>
       <c r="F47" s="8"/>
@@ -3241,13 +3341,15 @@
       <c r="R47" s="11"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C48" s="20"/>
-      <c r="D48" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="21"/>
+      <c r="C48" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="23"/>
       <c r="F48" s="8"/>
-      <c r="G48" s="11"/>
+      <c r="G48" s="7"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
@@ -3260,15 +3362,13 @@
       <c r="R48" s="11"/>
     </row>
     <row r="49" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C49" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="C49" s="20"/>
       <c r="D49" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="7"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
@@ -3281,11 +3381,11 @@
       <c r="R49" s="11"/>
     </row>
     <row r="50" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C50" s="20"/>
-      <c r="D50" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E50" s="6"/>
+      <c r="C50" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="21"/>
       <c r="F50" s="4"/>
       <c r="G50" s="11"/>
       <c r="I50" s="11"/>
@@ -3300,13 +3400,11 @@
       <c r="R50" s="11"/>
     </row>
     <row r="51" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C51" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="11"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="7"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
@@ -3323,7 +3421,7 @@
       <c r="D52" s="12"/>
       <c r="E52" s="6"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="7"/>
+      <c r="G52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
@@ -3336,11 +3434,11 @@
       <c r="R52" s="11"/>
     </row>
     <row r="53" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C53" s="16"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="11"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="10"/>
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
@@ -3353,10 +3451,10 @@
       <c r="R53" s="11"/>
     </row>
     <row r="54" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C54" s="20"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="8"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="4"/>
       <c r="G54" s="10"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
@@ -3374,7 +3472,7 @@
       <c r="D55" s="4"/>
       <c r="E55" s="21"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="10"/>
+      <c r="G55" s="7"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
@@ -3391,7 +3489,7 @@
       <c r="D56" s="4"/>
       <c r="E56" s="21"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="7"/>
+      <c r="G56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
@@ -3408,7 +3506,7 @@
       <c r="D57" s="4"/>
       <c r="E57" s="21"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="11"/>
+      <c r="G57" s="7"/>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
@@ -3425,7 +3523,7 @@
       <c r="D58" s="4"/>
       <c r="E58" s="21"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="7"/>
+      <c r="G58" s="11"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
@@ -3439,10 +3537,10 @@
     </row>
     <row r="59" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C59" s="16"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="11"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="10"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
       <c r="K59" s="11"/>
@@ -3456,10 +3554,10 @@
     </row>
     <row r="60" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C60" s="16"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="10"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="11"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
       <c r="K60" s="11"/>
@@ -3476,7 +3574,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="21"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="11"/>
+      <c r="G61" s="7"/>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
       <c r="K61" s="11"/>
@@ -3490,10 +3588,7 @@
     </row>
     <row r="62" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C62" s="16"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="7"/>
+      <c r="G62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
@@ -3506,8 +3601,10 @@
       <c r="R62" s="11"/>
     </row>
     <row r="63" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C63" s="16"/>
-      <c r="G63" s="11"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="8"/>
       <c r="I63" s="11"/>
       <c r="J63" s="11"/>
       <c r="K63" s="11"/>
@@ -3524,6 +3621,7 @@
       <c r="D64" s="8"/>
       <c r="E64" s="23"/>
       <c r="F64" s="8"/>
+      <c r="G64" s="11"/>
       <c r="I64" s="11"/>
       <c r="J64" s="11"/>
       <c r="K64" s="11"/>
@@ -20315,10 +20413,6 @@
       <c r="R1051" s="11"/>
     </row>
     <row r="1052" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C1052" s="20"/>
-      <c r="D1052" s="8"/>
-      <c r="E1052" s="23"/>
-      <c r="F1052" s="8"/>
       <c r="G1052" s="11"/>
       <c r="I1052" s="11"/>
       <c r="J1052" s="11"/>
@@ -20357,32 +20451,34 @@
       <c r="Q1054" s="11"/>
       <c r="R1054" s="11"/>
     </row>
-    <row r="1055" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="G1055" s="11"/>
-      <c r="I1055" s="11"/>
-      <c r="J1055" s="11"/>
-      <c r="K1055" s="11"/>
-      <c r="L1055" s="11"/>
-      <c r="M1055" s="11"/>
-      <c r="N1055" s="11"/>
-      <c r="O1055" s="11"/>
-      <c r="P1055" s="11"/>
-      <c r="Q1055" s="11"/>
-      <c r="R1055" s="11"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="last7Days">
+  <conditionalFormatting sqref="G27:G1048576 G1:G21 G24">
+    <cfRule type="timePeriod" dxfId="3" priority="4" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G1,1)&lt;=6,FLOOR(G1,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G25:G26">
+    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G25,1)&lt;=6,FLOOR(G25,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G22,1)&lt;=6,FLOOR(G22,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G23,1)&lt;=6,FLOOR(G23,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F45" r:id="rId1" xr:uid="{2D8093C6-6A70-4C38-B09F-3BB0227B641A}"/>
+    <hyperlink ref="F44" r:id="rId1" xr:uid="{2D8093C6-6A70-4C38-B09F-3BB0227B641A}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{6E565947-21CF-47F9-8CA2-995C0C03266C}"/>
     <hyperlink ref="F8" r:id="rId3" xr:uid="{0259A5C9-8486-4A9E-9B9D-E5C611482C63}"/>
     <hyperlink ref="F10" r:id="rId4" xr:uid="{0C554C86-504E-4A7E-88CF-9B00A46FCBEC}"/>
     <hyperlink ref="F13" r:id="rId5" xr:uid="{6FBC17D8-3990-459E-9B48-3EDCD7C3D037}"/>
-    <hyperlink ref="F24" r:id="rId6" xr:uid="{ECC4227F-EDBE-41A5-B8DC-A3B400F5C6AF}"/>
+    <hyperlink ref="F26" r:id="rId6" xr:uid="{FCAC682D-62FD-4125-86A8-F60487A7CA26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
compile wk5 go back to html table
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979832D6-52D5-42E5-BE21-DB2038BBEEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C942E5-AD8A-4539-BE91-3B1FD8499E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -1930,7 +1930,7 @@
   <dimension ref="A1:R1054"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2668,7 +2668,7 @@
         <v>43146</v>
       </c>
       <c r="H21" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
@@ -2738,7 +2738,7 @@
         <v>43158</v>
       </c>
       <c r="H23" s="65">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>

</xml_diff>

<commit_message>
prep week 6 and 7
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C52CA6-B202-4CB8-BFC0-5BF391848A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE0E5B-EE7A-4270-A032-B6E16D65A1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1980" windowWidth="23820" windowHeight="13635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="213">
   <si>
     <t>SLO</t>
   </si>
@@ -163,12 +163,6 @@
 * Get all the things</t>
   </si>
   <si>
-    <t xml:space="preserve">* Describe the difference between training and testing data sets  
-* Describe the difference between a parametric and non-parametric model  
-* Identify  and describe situations where classification, regression, and clustering models are appropriate.   
-* Explain the concept of overfitting, and bias-variance tradeoff. </t>
-  </si>
-  <si>
     <t>Creating a professional website</t>
   </si>
   <si>
@@ -181,9 +175,6 @@
     <t>Email?</t>
   </si>
   <si>
-    <t>ISLR Ch 4 - Collaborative notes</t>
-  </si>
-  <si>
     <t>ISLR Ch 5 - Collaborative notes</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
   </si>
   <si>
     <t>Linear Regression</t>
-  </si>
-  <si>
-    <t>ISLR Ch 4 - Practice Exercises</t>
   </si>
   <si>
     <t>ISLR Ch 5 - Practice Exercises</t>
@@ -338,9 +326,6 @@
     <t xml:space="preserve">What is Statistical Learning? </t>
   </si>
   <si>
-    <t>ISLR Ch 3</t>
-  </si>
-  <si>
     <t>ISLR Ch 4</t>
   </si>
   <si>
@@ -356,9 +341,6 @@
     <t>ISLR Ch 8</t>
   </si>
   <si>
-    <t>ISLR Ch 10</t>
-  </si>
-  <si>
     <t>Understand what the New Jim Code is and how it impacts our society</t>
   </si>
   <si>
@@ -369,9 +351,6 @@
   </si>
   <si>
     <t xml:space="preserve">Get connected to the class learning tools </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identify cases where a non-parametric approach would be more appropriate than a parametric approach.   </t>
   </si>
   <si>
     <t>Read Doing Data Science Ch 2</t>
@@ -461,21 +440,6 @@
     <t>Being open to new ways of thinking and viewing the world</t>
   </si>
   <si>
-    <t>[3](wk03-notes.html)</t>
-  </si>
-  <si>
-    <t>[4](wk04-notes.html)</t>
-  </si>
-  <si>
-    <t>[1](wk01-notes.html)</t>
-  </si>
-  <si>
-    <t>[2](wk02-notes.html)</t>
-  </si>
-  <si>
-    <t>[5](wk05-notes.html)</t>
-  </si>
-  <si>
     <t>Send final report to Dr. D via Discord</t>
   </si>
   <si>
@@ -555,9 +519,6 @@
   </si>
   <si>
     <t>Technological benevolence</t>
-  </si>
-  <si>
-    <t>Retoolign Solidarity, Reimagining Justice</t>
   </si>
   <si>
     <t>Race as a predictor</t>
@@ -595,13 +556,6 @@
     <t>ADS Website</t>
   </si>
   <si>
-    <t>[6](wk06-notes.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read/watch [[ISLR Ch 1]](https://www.youtube.com/playlist?list=PLAOUn-KLSAVOPE3yQ04EZCbt0ycTib6OH) before class on Tuesday.
-Pull your ISLR github classroom repo. Prepare Chapter 2 answers per [Week 6 notes](wk06-notes.html). Finish all questions before Thursday. </t>
-  </si>
-  <si>
     <t>Learning Tidymodels</t>
   </si>
   <si>
@@ -671,16 +625,78 @@
     <t>ISLR Ch2  Notes &amp; Exercises</t>
   </si>
   <si>
-    <t>ISLR Ch 3 Notes &amp; Exercises</t>
-  </si>
-  <si>
     <t>Classwide &amp; Client project share out</t>
   </si>
   <si>
     <t>Preprocessing your data with recipies</t>
   </si>
   <si>
-    <t>ISLR Repo: ch3-lin-reg</t>
+    <t>Unsupervised Learning</t>
+  </si>
+  <si>
+    <t>ISLR Ch 12</t>
+  </si>
+  <si>
+    <t>Model Selection and Regularization</t>
+  </si>
+  <si>
+    <t>Retooling Solidarity, Reimagining Justice</t>
+  </si>
+  <si>
+    <t>Special Topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skim ISLR Ch 3. Start on the Tidymodels lab. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write a tutorial for your website on how to use Tidymodels to build and assess a linear regression model. Data &amp; Topic is your choice. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leverage your knowledge of linear models and write a tutorial on how to fit a regression model in the Tidy models framework. The data and model you fit is your choice. </t>
+  </si>
+  <si>
+    <t>Reading discussion</t>
+  </si>
+  <si>
+    <t>Project share out</t>
+  </si>
+  <si>
+    <t>Open work</t>
+  </si>
+  <si>
+    <t>Review another classmates tutorial and provide comments &amp; feedback in Discord. Is there something that isn't clear? Did you spot a mistake they can fix? What did you find helpful &amp; useful about their tutorial (be specific)</t>
+  </si>
+  <si>
+    <t>Peer review</t>
+  </si>
+  <si>
+    <t>ISLR Ch 4 - Notes &amp; Exercises</t>
+  </si>
+  <si>
+    <t>[Notes](wk01-notes.html)</t>
+  </si>
+  <si>
+    <t>[Notes](wk02-notes.html)</t>
+  </si>
+  <si>
+    <t>[Notes](wk03-notes.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read/watch [[ISLR Ch 1]](https://www.youtube.com/playlist?list=PLAOUn-KLSAVOPE3yQ04EZCbt0ycTib6OH) before class on Tuesday.  
+Pull your [ISLR github classroom repo](https://classroom.github.com/a/E2rqFG9T).   
+Prepare Chapter 2 answers per [Week 6 notes](wk06-notes.html). Finish all questions before Thursday.   </t>
+  </si>
+  <si>
+    <t>[Notes](wk06-notes.html)</t>
+  </si>
+  <si>
+    <t>[Notes](wk07-notes.html)</t>
+  </si>
+  <si>
+    <t>[Notes](wk05-notes.html)</t>
+  </si>
+  <si>
+    <t>[Notes](wk04-notes.html)</t>
   </si>
 </sst>
 </file>
@@ -927,7 +943,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1151,6 +1167,24 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1247,7 +1281,27 @@
     <cellStyle name="Normal 3 2" xfId="91" xr:uid="{20B637C8-DD27-499C-BEC0-85B72C712ADD}"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1638,11 +1692,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F1" s="28" t="s">
         <v>37</v>
@@ -1689,29 +1743,29 @@
     </row>
     <row r="2" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>136</v>
+        <v>205</v>
       </c>
       <c r="B2" s="31">
         <v>43124</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1720,76 +1774,76 @@
         <v>43126</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E3" s="36"/>
       <c r="F3" s="36" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H3" s="36"/>
       <c r="I3" s="36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
-        <v>137</v>
+        <v>206</v>
       </c>
       <c r="B4" s="38">
         <v>43131</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I4" s="40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="B5" s="31">
         <v>43138</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H5" s="42" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I5" s="42"/>
     </row>
@@ -1805,34 +1859,34 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>135</v>
+        <v>212</v>
       </c>
       <c r="B7" s="31">
         <v>43145</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I7" s="42" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1841,28 +1895,28 @@
         <v>43147</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="B9" s="31">
         <v>43152</v>
@@ -1871,7 +1925,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
@@ -1883,13 +1937,13 @@
       <c r="A10" s="30"/>
       <c r="B10" s="31"/>
       <c r="C10" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="42" t="s">
         <v>158</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>170</v>
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
@@ -1902,36 +1956,34 @@
         <v>43154</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
       <c r="I11" s="43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="141.75" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="189" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="B12" s="31">
         <v>43159</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>40</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D12" s="42"/>
       <c r="E12" s="42" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
@@ -1946,11 +1998,11 @@
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
       <c r="C13" s="16" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D13" s="42"/>
       <c r="E13" s="42" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
@@ -1961,10 +2013,10 @@
       <c r="A14" s="33"/>
       <c r="B14" s="34"/>
       <c r="C14" s="72" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="E14" s="43"/>
       <c r="F14" s="43"/>
@@ -1972,40 +2024,44 @@
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
     </row>
-    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
-        <v>7</v>
+    <row r="15" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="B15" s="31">
         <v>43166</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="H15" s="42" t="s">
+        <v>201</v>
+      </c>
       <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="31"/>
       <c r="C16" s="16" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D16" s="42"/>
       <c r="E16" s="42" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="H16" s="42" t="s">
+        <v>199</v>
+      </c>
       <c r="I16" s="42"/>
     </row>
     <row r="17" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2016,12 +2072,14 @@
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
       <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="I17" s="43" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="44">
@@ -2035,7 +2093,7 @@
       </c>
       <c r="D18" s="46"/>
       <c r="E18" s="42" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F18" s="46"/>
       <c r="G18" s="42"/>
@@ -2046,13 +2104,13 @@
       <c r="A19" s="44"/>
       <c r="B19" s="45"/>
       <c r="C19" s="46" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F19" s="46"/>
       <c r="G19" s="42"/>
@@ -2084,7 +2142,7 @@
       </c>
       <c r="D21" s="42"/>
       <c r="E21" s="42" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
@@ -2100,10 +2158,10 @@
         <v>10</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
@@ -2114,11 +2172,11 @@
       <c r="A23" s="73"/>
       <c r="B23" s="74"/>
       <c r="C23" s="43" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="43" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
@@ -2131,28 +2189,28 @@
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="42" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
       <c r="D24" s="42"/>
       <c r="E24" s="42" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
         <v>11</v>
       </c>
       <c r="B25" s="31"/>
       <c r="C25" s="42" t="s">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="D25" s="42"/>
       <c r="E25" s="42" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
@@ -2163,11 +2221,11 @@
       <c r="A26" s="30"/>
       <c r="B26" s="31"/>
       <c r="C26" s="42" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D26" s="42"/>
       <c r="E26" s="42" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="42"/>
@@ -2180,28 +2238,28 @@
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="42" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D27" s="42"/>
       <c r="E27" s="42" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
       <c r="I27" s="42"/>
     </row>
-    <row r="28" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="30">
         <v>13</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="42" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D28" s="42"/>
       <c r="E28" s="42" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
@@ -2212,50 +2270,65 @@
       <c r="A29" s="30"/>
       <c r="B29" s="31"/>
       <c r="C29" s="42" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D29" s="42"/>
       <c r="E29" s="42" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
     </row>
-    <row r="30" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="30">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="42" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="D30" s="42"/>
-      <c r="E30" s="42" t="s">
-        <v>199</v>
-      </c>
+      <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
-        <v>73</v>
+    <row r="31" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="A31" s="30">
+        <v>15</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="42"/>
+        <v>194</v>
+      </c>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42" t="s">
+        <v>185</v>
+      </c>
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
       <c r="I31" s="42"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="31"/>
+      <c r="C32" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -2269,8 +2342,8 @@
   <dimension ref="A1:R1061"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2363,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>17</v>
@@ -2299,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>23</v>
@@ -2336,7 +2409,7 @@
       </c>
       <c r="E2" s="50"/>
       <c r="F2" s="51" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G2" s="52">
         <v>43125</v>
@@ -2396,7 +2469,7 @@
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="52">
         <v>43125</v>
@@ -2422,11 +2495,11 @@
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="49" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="51" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G5" s="52">
         <v>43125</v>
@@ -2452,7 +2525,7 @@
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="49" t="s">
@@ -2482,11 +2555,11 @@
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="49" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G7" s="52">
         <v>43125</v>
@@ -2512,11 +2585,11 @@
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E8" s="50"/>
       <c r="F8" s="51" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G8" s="52">
         <v>43127</v>
@@ -2571,16 +2644,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E10" s="50">
         <v>2</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G10" s="52">
         <v>43132</v>
@@ -2607,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>21</v>
@@ -2616,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="G11" s="5">
         <v>43137</v>
@@ -2647,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G12" s="5">
         <v>43137</v>
@@ -2671,16 +2744,16 @@
         <v>3</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E13" s="20">
         <v>6</v>
       </c>
       <c r="F13" s="57" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G13" s="5">
         <v>43133</v>
@@ -2705,13 +2778,13 @@
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E14" s="20">
         <v>7</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G14" s="5">
         <v>43137</v>
@@ -2736,13 +2809,13 @@
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" s="20">
         <v>7</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G15" s="5">
         <v>43134</v>
@@ -2767,13 +2840,13 @@
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E16" s="20">
         <v>7</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G16" s="5">
         <v>43137</v>
@@ -2798,13 +2871,13 @@
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E17" s="20">
         <v>2</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G17" s="5">
         <v>43141</v>
@@ -2829,13 +2902,13 @@
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E18" s="20">
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G18" s="5">
         <v>43144</v>
@@ -2862,16 +2935,16 @@
         <v>1</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="49" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E19" s="50">
         <v>5</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G19" s="52">
         <v>43145</v>
@@ -2899,11 +2972,11 @@
         <v>29</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="49" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G20" s="52">
         <v>43143</v>
@@ -2930,14 +3003,14 @@
         <v>1</v>
       </c>
       <c r="C21" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="4" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="G21" s="5">
         <v>43146</v>
@@ -2962,16 +3035,16 @@
         <v>2</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E22" s="62">
         <v>5</v>
       </c>
       <c r="F22" s="61" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G22" s="63">
         <v>43151</v>
@@ -2999,11 +3072,11 @@
         <v>29</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E23" s="62"/>
       <c r="F23" s="66" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G23" s="63">
         <v>43158</v>
@@ -3033,13 +3106,13 @@
         <v>8</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E24" s="50">
         <v>5</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="G24" s="52">
         <v>43159</v>
@@ -3064,14 +3137,14 @@
         <v>2</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E25" s="50"/>
       <c r="F25" s="51" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G25" s="52">
         <v>43153</v>
@@ -3099,11 +3172,11 @@
         <v>29</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="49" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="G26" s="52">
         <v>43151</v>
@@ -3129,11 +3202,11 @@
       </c>
       <c r="C27" s="48"/>
       <c r="D27" s="49" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E27" s="50"/>
       <c r="F27" s="56" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="G27" s="52">
         <v>43153</v>
@@ -3160,14 +3233,14 @@
         <v>1</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G28" s="5">
         <v>43165</v>
@@ -3191,13 +3264,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="G29" s="5">
         <v>43165</v>
@@ -3224,10 +3297,10 @@
         <v>29</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="G30" s="63">
         <v>43160</v>
@@ -3251,13 +3324,13 @@
         <v>4</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G31" s="5">
         <v>43165</v>
@@ -3276,25 +3349,25 @@
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="58">
         <v>7</v>
       </c>
       <c r="B32" s="58">
         <v>1</v>
       </c>
-      <c r="C32" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="69" t="s">
-        <v>203</v>
+      <c r="C32" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="76" t="s">
+        <v>178</v>
       </c>
       <c r="E32" s="70"/>
       <c r="F32" s="69" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="G32" s="52">
-        <v>43179</v>
+        <v>43166</v>
       </c>
       <c r="H32" s="47"/>
       <c r="I32" s="10"/>
@@ -3314,17 +3387,15 @@
         <v>2</v>
       </c>
       <c r="C33" s="68" t="s">
-        <v>181</v>
+        <v>29</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="E33" s="70"/>
-      <c r="F33" s="69" t="s">
-        <v>182</v>
-      </c>
+      <c r="F33" s="69"/>
       <c r="G33" s="52">
-        <v>43179</v>
+        <v>43168</v>
       </c>
       <c r="H33" s="47"/>
       <c r="I33" s="10"/>
@@ -3338,21 +3409,19 @@
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
     </row>
-    <row r="34" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="63" x14ac:dyDescent="0.25">
       <c r="A34" s="58"/>
       <c r="B34" s="58">
         <v>3</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="76" t="s">
-        <v>192</v>
+      <c r="C34" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="69" t="s">
+        <v>198</v>
       </c>
       <c r="E34" s="70"/>
-      <c r="F34" s="69" t="s">
-        <v>187</v>
-      </c>
+      <c r="F34" s="69"/>
       <c r="G34" s="52">
         <v>43179</v>
       </c>
@@ -3368,21 +3437,23 @@
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A35" s="58"/>
       <c r="B35" s="58">
         <v>4</v>
       </c>
       <c r="C35" s="68" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E35" s="70"/>
-      <c r="F35" s="69"/>
+      <c r="F35" s="69" t="s">
+        <v>69</v>
+      </c>
       <c r="G35" s="52">
-        <v>43168</v>
+        <v>43182</v>
       </c>
       <c r="H35" s="47"/>
       <c r="I35" s="10"/>
@@ -3397,20 +3468,24 @@
       <c r="R35" s="10"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="59">
-        <v>8</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="22"/>
-      <c r="F36" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="7"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="58">
+        <v>5</v>
+      </c>
+      <c r="C36" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" s="70"/>
+      <c r="F36" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" s="52">
+        <v>43179</v>
+      </c>
+      <c r="H36" s="47"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -3423,14 +3498,16 @@
       <c r="R36" s="10"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C37" s="18"/>
-      <c r="D37" s="12" t="s">
-        <v>56</v>
+      <c r="A37" s="59">
+        <v>8</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>204</v>
       </c>
       <c r="E37" s="22"/>
-      <c r="F37" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="G37" s="7"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -3445,7 +3522,7 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C38" s="18" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E38" s="22"/>
       <c r="G38" s="7"/>
@@ -3460,12 +3537,17 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C39" s="18" t="s">
+    <row r="39" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="22"/>
-      <c r="G39" s="7"/>
+      <c r="D39" s="79"/>
+      <c r="E39" s="80"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="82"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
@@ -3486,11 +3568,11 @@
         <v>11</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E40" s="50"/>
       <c r="F40" s="69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G40" s="71"/>
       <c r="H40" s="47"/>
@@ -3510,7 +3592,7 @@
       <c r="B41" s="58"/>
       <c r="C41" s="54"/>
       <c r="D41" s="69" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E41" s="50"/>
       <c r="F41" s="69" t="s">
@@ -3533,14 +3615,14 @@
       <c r="A42" s="58"/>
       <c r="B42" s="58"/>
       <c r="C42" s="48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D42" s="69" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="E42" s="50"/>
       <c r="F42" s="69" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="G42" s="71"/>
       <c r="H42" s="47"/>
@@ -3563,11 +3645,11 @@
         <v>15</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G43" s="7"/>
       <c r="I43" s="10"/>
@@ -3584,7 +3666,7 @@
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C44" s="13"/>
       <c r="D44" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="12" t="s">
@@ -3611,11 +3693,11 @@
         <v>16</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E45" s="50"/>
       <c r="F45" s="69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G45" s="71"/>
       <c r="H45" s="47"/>
@@ -3635,7 +3717,7 @@
       <c r="B46" s="58"/>
       <c r="C46" s="54"/>
       <c r="D46" s="69" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E46" s="50"/>
       <c r="F46" s="69" t="s">
@@ -3658,14 +3740,14 @@
       <c r="A47" s="58"/>
       <c r="B47" s="58"/>
       <c r="C47" s="48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D47" s="69" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E47" s="50"/>
       <c r="F47" s="69" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G47" s="71"/>
       <c r="H47" s="47"/>
@@ -3688,11 +3770,11 @@
         <v>12</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G48" s="7"/>
       <c r="I48" s="10"/>
@@ -3709,7 +3791,7 @@
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C49" s="13"/>
       <c r="D49" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="12" t="s">
@@ -3736,11 +3818,11 @@
         <v>31</v>
       </c>
       <c r="D50" s="49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E50" s="50"/>
       <c r="F50" s="69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G50" s="71"/>
       <c r="H50" s="47"/>
@@ -3760,7 +3842,7 @@
       <c r="B51" s="58"/>
       <c r="C51" s="54"/>
       <c r="D51" s="69" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E51" s="50"/>
       <c r="F51" s="69" t="s">
@@ -3783,14 +3865,14 @@
       <c r="A52" s="58"/>
       <c r="B52" s="58"/>
       <c r="C52" s="48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D52" s="69" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="E52" s="50"/>
       <c r="F52" s="69" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="G52" s="71"/>
       <c r="H52" s="47"/>
@@ -3830,14 +3912,14 @@
       </c>
       <c r="B54" s="58"/>
       <c r="C54" s="48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D54" s="69" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E54" s="50"/>
       <c r="F54" s="69" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="G54" s="71"/>
       <c r="H54" s="47"/>
@@ -3854,10 +3936,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C55" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="8"/>
@@ -3876,7 +3958,7 @@
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C56" s="19"/>
       <c r="D56" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="4"/>
@@ -3894,7 +3976,7 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C57" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="20"/>
@@ -20964,29 +21046,39 @@
       <c r="R1061" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31:G1048576">
-    <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="last7Days">
+  <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31 G37:G1048576">
+    <cfRule type="timePeriod" dxfId="6" priority="8" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G1,1)&lt;=6,FLOOR(G1,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="timePeriod" dxfId="3" priority="5" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G26,1)&lt;=6,FLOOR(G26,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="timePeriod" dxfId="2" priority="4" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G22,1)&lt;=6,FLOOR(G22,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="timePeriod" dxfId="1" priority="3" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="3" priority="5" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G23,1)&lt;=6,FLOOR(G23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="2" priority="4" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G30,1)&lt;=6,FLOOR(G30,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34:G36">
+    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G34,1)&lt;=6,FLOOR(G34,1)&lt;=TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:G33">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G32,1)&lt;=6,FLOOR(G32,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
update schedule and deliverables
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FCA564-4821-4221-8365-0EFBED9959B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4225A441-5FA7-433D-A5F5-169D32D9BE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="1620" windowWidth="21600" windowHeight="14580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30795" yWindow="1260" windowWidth="22905" windowHeight="13815" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="232">
   <si>
     <t>SLO</t>
   </si>
@@ -674,9 +674,6 @@
     <t>Final project presentation for stakeholders</t>
   </si>
   <si>
-    <t>Project Poster - Very solid Draft</t>
-  </si>
-  <si>
     <t>Project repo</t>
   </si>
   <si>
@@ -687,9 +684,6 @@
   </si>
   <si>
     <t>Client share out</t>
-  </si>
-  <si>
-    <t>ISLR Ch 5 - Notes &amp; Exercises</t>
   </si>
   <si>
     <t xml:space="preserve">Read/watch ISLR Chapter 5 content &amp; prepare answers to questions to discuss in class. We'll spend half the class each day on this topic. </t>
@@ -734,6 +728,33 @@
   </si>
   <si>
     <t>Your blog website</t>
+  </si>
+  <si>
+    <t>cesar chavez day no school</t>
+  </si>
+  <si>
+    <t>ISLR Ch 5 - Exercises</t>
+  </si>
+  <si>
+    <t>ISLR Ch 5 - Notes</t>
+  </si>
+  <si>
+    <t>Project Poster - Very solid Draft to present &amp; peer review</t>
+  </si>
+  <si>
+    <t>Returning to the learning bridge</t>
+  </si>
+  <si>
+    <t>Post semester reflection</t>
+  </si>
+  <si>
+    <t>What's next?</t>
+  </si>
+  <si>
+    <t>Cesar Chavez day</t>
+  </si>
+  <si>
+    <t>No class on Thursday</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1019,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1310,7 +1331,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="4" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1860,11 +1884,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2303,7 +2327,7 @@
     </row>
     <row r="18" spans="1:10" ht="63.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B18" s="95">
         <v>8.1</v>
@@ -2316,7 +2340,7 @@
       </c>
       <c r="E18" s="45"/>
       <c r="F18" s="41" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="41"/>
@@ -2336,7 +2360,7 @@
         <v>148</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G19" s="72"/>
       <c r="H19" s="42"/>
@@ -2358,54 +2382,58 @@
       </c>
       <c r="E20" s="41"/>
       <c r="F20" s="41" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
       <c r="I20" s="41"/>
       <c r="J20" s="41"/>
     </row>
-    <row r="21" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="95">
-        <v>9.1999999999999993</v>
+        <v>4.5</v>
       </c>
       <c r="C21" s="44">
-        <v>43190</v>
+        <v>43189</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>96</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="E21" s="41"/>
       <c r="F21" s="41" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
       <c r="I21" s="41"/>
       <c r="J21" s="41"/>
     </row>
-    <row r="22" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="70"/>
       <c r="B22" s="96">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C22" s="71"/>
+      <c r="C22" s="71">
+        <v>43190</v>
+      </c>
       <c r="D22" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="42"/>
+        <v>210</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>96</v>
+      </c>
       <c r="F22" s="42" t="s">
-        <v>213</v>
+        <v>141</v>
       </c>
       <c r="G22" s="42"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="42" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>10</v>
       </c>
@@ -2414,165 +2442,161 @@
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="41" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="41" t="s">
-        <v>208</v>
+        <v>87</v>
       </c>
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
       <c r="I23" s="41"/>
       <c r="J23" s="41"/>
     </row>
-    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>11</v>
-      </c>
+    <row r="24" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
       <c r="B24" s="91">
-        <v>11.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="41" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="E24" s="41"/>
       <c r="F24" s="41" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
       <c r="I24" s="41"/>
       <c r="J24" s="41"/>
     </row>
-    <row r="25" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>11</v>
+      </c>
       <c r="B25" s="91">
-        <v>11.2</v>
+        <v>11.1</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="41" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
       <c r="E25" s="41"/>
       <c r="F25" s="41" t="s">
-        <v>166</v>
+        <v>88</v>
       </c>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
       <c r="I25" s="41"/>
       <c r="J25" s="41"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
-        <v>12</v>
-      </c>
+    <row r="26" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
       <c r="B26" s="91">
-        <v>12.1</v>
+        <v>11.2</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="41" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="E26" s="41"/>
       <c r="F26" s="41" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
       <c r="I26" s="41"/>
       <c r="J26" s="41"/>
     </row>
-    <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="91">
-        <v>13.1</v>
+        <v>12.1</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="41" t="s">
-        <v>217</v>
+        <v>11</v>
       </c>
       <c r="E27" s="41"/>
       <c r="F27" s="41" t="s">
-        <v>218</v>
+        <v>89</v>
       </c>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
       <c r="I27" s="41"/>
       <c r="J27" s="41"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
-        <v>14</v>
-      </c>
+    <row r="28" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
       <c r="B28" s="91">
-        <v>14.1</v>
+        <v>12.2</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="41" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="E28" s="41"/>
       <c r="F28" s="41" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
       <c r="I28" s="41"/>
       <c r="J28" s="41"/>
     </row>
-    <row r="29" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>13</v>
+      </c>
       <c r="B29" s="91">
-        <v>14.2</v>
+        <v>13.1</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="41" t="s">
-        <v>146</v>
+        <v>215</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41" t="s">
-        <v>174</v>
+        <v>216</v>
       </c>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
       <c r="I29" s="41"/>
       <c r="J29" s="41"/>
     </row>
-    <row r="30" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="91">
-        <v>15.1</v>
+        <v>14.1</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E30" s="41"/>
       <c r="F30" s="41" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
       <c r="I30" s="41"/>
       <c r="J30" s="41"/>
     </row>
-    <row r="31" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
-      <c r="B31" s="91">
-        <v>15.2</v>
-      </c>
+      <c r="B31" s="91"/>
       <c r="C31" s="30"/>
       <c r="D31" s="41" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="E31" s="41"/>
       <c r="F31" s="41" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
@@ -2580,24 +2604,60 @@
       <c r="J31" s="41"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
-        <v>64</v>
+      <c r="A32" s="29">
+        <v>15</v>
       </c>
       <c r="B32" s="91">
-        <v>16.100000000000001</v>
+        <v>15.1</v>
       </c>
       <c r="C32" s="30"/>
-      <c r="D32" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="41"/>
+      <c r="D32" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
       <c r="I32" s="41"/>
       <c r="J32" s="41"/>
+    </row>
+    <row r="33" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="91">
+        <v>15.2</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="91">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
@@ -2608,11 +2668,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBC2D3D-FE18-4FBF-825C-8A0A6D387E1B}">
-  <dimension ref="A1:R1068"/>
+  <dimension ref="A1:R1070"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2668,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="56">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="46" t="s">
         <v>19</v>
@@ -2702,7 +2762,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="56">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="47" t="s">
@@ -2734,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="56">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="47" t="s">
@@ -2766,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="56">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="47" t="s">
@@ -2798,7 +2858,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="56">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="47" t="s">
@@ -2830,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="56">
-        <v>6</v>
+        <v>1.6</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="47" t="s">
@@ -2862,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="56">
-        <v>7</v>
+        <v>1.7</v>
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="47" t="s">
@@ -2894,7 +2954,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="56">
-        <v>8</v>
+        <v>1.8</v>
       </c>
       <c r="C9" s="46"/>
       <c r="D9" s="47" t="s">
@@ -2926,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="56">
-        <v>9</v>
+        <v>1.9</v>
       </c>
       <c r="C10" s="51" t="s">
         <v>38</v>
@@ -2962,7 +3022,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="57">
-        <v>1</v>
+        <v>2.1</v>
       </c>
       <c r="C11" s="53" t="s">
         <v>38</v>
@@ -2998,7 +3058,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="57">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="3" t="s">
@@ -3032,7 +3092,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="57">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>62</v>
@@ -3068,7 +3128,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="57">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="3" t="s">
@@ -3102,7 +3162,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="57">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="3" t="s">
@@ -3136,7 +3196,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="57">
-        <v>6</v>
+        <v>2.6</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="3" t="s">
@@ -3170,7 +3230,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="57">
-        <v>7</v>
+        <v>2.7</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="3" t="s">
@@ -3204,7 +3264,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="57">
-        <v>8</v>
+        <v>2.8</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="3" t="s">
@@ -3238,7 +3298,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="56">
-        <v>1</v>
+        <v>3.1</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>47</v>
@@ -3274,7 +3334,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="56">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="C20" s="52" t="s">
         <v>27</v>
@@ -3308,7 +3368,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="57">
-        <v>1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>80</v>
@@ -3342,7 +3402,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="58">
-        <v>2</v>
+        <v>4.2</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>47</v>
@@ -3378,7 +3438,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="58">
-        <v>3</v>
+        <v>4.3</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>27</v>
@@ -3412,7 +3472,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="56">
-        <v>1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C24" s="46" t="s">
         <v>8</v>
@@ -3448,7 +3508,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="56">
-        <v>2</v>
+        <v>5.2</v>
       </c>
       <c r="C25" s="46" t="s">
         <v>80</v>
@@ -3482,7 +3542,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="56">
-        <v>3</v>
+        <v>5.3</v>
       </c>
       <c r="C26" s="46" t="s">
         <v>27</v>
@@ -3516,7 +3576,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="56">
-        <v>4</v>
+        <v>5.4</v>
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="47" t="s">
@@ -3548,7 +3608,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="57">
-        <v>1</v>
+        <v>6.1</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>48</v>
@@ -3582,7 +3642,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="57">
-        <v>2</v>
+        <v>6.2</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>158</v>
@@ -3615,7 +3675,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="57">
-        <v>3</v>
+        <v>6.3</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>27</v>
@@ -3648,7 +3708,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="57">
-        <v>4</v>
+        <v>6.4</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>153</v>
@@ -3681,7 +3741,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="56">
-        <v>1</v>
+        <v>7.1</v>
       </c>
       <c r="C32" s="46" t="s">
         <v>80</v>
@@ -3715,7 +3775,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="56">
-        <v>2</v>
+        <v>7.2</v>
       </c>
       <c r="C33" s="65" t="s">
         <v>27</v>
@@ -3747,7 +3807,7 @@
         <v>7</v>
       </c>
       <c r="B34" s="56">
-        <v>3</v>
+        <v>7.3</v>
       </c>
       <c r="C34" s="65" t="s">
         <v>49</v>
@@ -3757,7 +3817,7 @@
       </c>
       <c r="E34" s="67"/>
       <c r="F34" s="66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G34" s="50">
         <v>43179</v>
@@ -3781,7 +3841,7 @@
         <v>7</v>
       </c>
       <c r="B35" s="56">
-        <v>4</v>
+        <v>7.4</v>
       </c>
       <c r="C35" s="65" t="s">
         <v>191</v>
@@ -3814,8 +3874,8 @@
       <c r="A36" s="74">
         <v>7</v>
       </c>
-      <c r="B36" s="74">
-        <v>5</v>
+      <c r="B36" s="56">
+        <v>7.5</v>
       </c>
       <c r="C36" s="75" t="s">
         <v>158</v>
@@ -3849,13 +3909,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="57">
-        <v>1</v>
+        <v>8.1</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="11" t="s">
@@ -3883,13 +3943,13 @@
         <v>8</v>
       </c>
       <c r="B38" s="57">
-        <v>2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="11" t="s">
@@ -3917,13 +3977,13 @@
         <v>8</v>
       </c>
       <c r="B39" s="57">
-        <v>3</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="11" t="s">
@@ -3951,19 +4011,21 @@
         <v>9</v>
       </c>
       <c r="B40" s="56">
-        <v>1</v>
+        <v>9.1</v>
       </c>
       <c r="C40" s="52" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="47" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="E40" s="48"/>
       <c r="F40" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="G40" s="68"/>
+      <c r="G40" s="79">
+        <v>43193</v>
+      </c>
       <c r="H40" s="62"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
@@ -3981,20 +4043,20 @@
         <v>9</v>
       </c>
       <c r="B41" s="56">
-        <v>2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="66" t="s">
-        <v>201</v>
+        <v>10</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>224</v>
       </c>
       <c r="E41" s="48"/>
       <c r="F41" s="66" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G41" s="79">
-        <v>43188</v>
+        <v>43193</v>
       </c>
       <c r="H41" s="62"/>
       <c r="I41" s="9"/>
@@ -4013,18 +4075,20 @@
         <v>9</v>
       </c>
       <c r="B42" s="56">
-        <v>3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C42" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="66" t="s">
-        <v>209</v>
+        <v>153</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>227</v>
       </c>
       <c r="E42" s="48"/>
-      <c r="F42" s="66"/>
+      <c r="F42" s="66" t="s">
+        <v>81</v>
+      </c>
       <c r="G42" s="79">
-        <v>43189</v>
+        <v>43187</v>
       </c>
       <c r="H42" s="62"/>
       <c r="I42" s="9"/>
@@ -4038,27 +4102,29 @@
       <c r="Q42" s="9"/>
       <c r="R42" s="9"/>
     </row>
-    <row r="43" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="56">
         <v>9</v>
       </c>
       <c r="B43" s="56">
-        <v>4</v>
-      </c>
-      <c r="C43" s="46" t="s">
-        <v>80</v>
+        <v>9.4</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>27</v>
       </c>
       <c r="D43" s="66" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="E43" s="48"/>
       <c r="F43" s="66" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="G43" s="79">
-        <v>43189</v>
-      </c>
-      <c r="H43" s="62"/>
+        <v>43188</v>
+      </c>
+      <c r="H43" s="62">
+        <v>10</v>
+      </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -4070,24 +4136,26 @@
       <c r="Q43" s="9"/>
       <c r="R43" s="9"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="57">
         <v>10</v>
       </c>
       <c r="B44" s="57">
-        <v>1</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="19"/>
-      <c r="F44" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G44" s="6"/>
+        <v>10.1</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="E44" s="60"/>
+      <c r="F44" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="G44" s="82">
+        <v>43194</v>
+      </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -4104,17 +4172,19 @@
         <v>10</v>
       </c>
       <c r="B45" s="57">
-        <v>2</v>
-      </c>
-      <c r="C45" s="17"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="D45" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G45" s="6"/>
+        <v>208</v>
+      </c>
+      <c r="E45" s="60"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="82">
+        <v>43194</v>
+      </c>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -4131,7 +4201,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="57">
-        <v>3</v>
+        <v>10.3</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>27</v>
@@ -4158,24 +4228,25 @@
       <c r="R46" s="9"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="56">
-        <v>11</v>
-      </c>
-      <c r="B47" s="56">
-        <v>1</v>
-      </c>
-      <c r="C47" s="52" t="s">
+      <c r="A47" s="57">
+        <v>10</v>
+      </c>
+      <c r="B47" s="57">
+        <v>10.4</v>
+      </c>
+      <c r="C47" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="47" t="s">
+      <c r="D47" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="E47" s="48"/>
-      <c r="F47" s="66" t="s">
+      <c r="E47" s="19"/>
+      <c r="F47" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="G47" s="68"/>
-      <c r="H47" s="62"/>
+      <c r="G47" s="80">
+        <v>43200</v>
+      </c>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -4188,22 +4259,23 @@
       <c r="R47" s="9"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="56">
-        <v>11</v>
-      </c>
-      <c r="B48" s="56">
-        <v>2</v>
-      </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="66" t="s">
+      <c r="A48" s="57">
+        <v>10</v>
+      </c>
+      <c r="B48" s="57">
+        <v>10.5</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="66" t="s">
+      <c r="E48" s="19"/>
+      <c r="F48" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="G48" s="68"/>
-      <c r="H48" s="62"/>
+      <c r="G48" s="80">
+        <v>43200</v>
+      </c>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -4215,25 +4287,25 @@
       <c r="Q48" s="9"/>
       <c r="R48" s="9"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="56">
         <v>11</v>
       </c>
       <c r="B49" s="56">
-        <v>3</v>
-      </c>
-      <c r="C49" s="52" t="s">
-        <v>27</v>
+        <v>11.1</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="D49" s="66" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="E49" s="48"/>
       <c r="F49" s="66" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="G49" s="79">
-        <v>43202</v>
+        <v>43201</v>
       </c>
       <c r="H49" s="62"/>
       <c r="I49" s="9"/>
@@ -4247,24 +4319,24 @@
       <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
     </row>
-    <row r="50" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="56">
         <v>11</v>
       </c>
       <c r="B50" s="56">
-        <v>4</v>
-      </c>
-      <c r="C50" s="46" t="s">
-        <v>80</v>
+        <v>11.2</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>27</v>
       </c>
       <c r="D50" s="66" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="E50" s="48"/>
       <c r="F50" s="66" t="s">
-        <v>167</v>
-      </c>
-      <c r="G50" s="68"/>
+        <v>200</v>
+      </c>
+      <c r="G50" s="79"/>
       <c r="H50" s="62"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
@@ -4278,23 +4350,24 @@
       <c r="R50" s="9"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="57">
-        <v>12</v>
-      </c>
-      <c r="B51" s="57">
-        <v>1</v>
-      </c>
-      <c r="C51" s="17" t="s">
+      <c r="A51" s="56">
+        <v>11</v>
+      </c>
+      <c r="B51" s="56">
+        <v>11.3</v>
+      </c>
+      <c r="C51" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="59" t="s">
+      <c r="D51" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="E51" s="60"/>
-      <c r="F51" s="81" t="s">
+      <c r="E51" s="48"/>
+      <c r="F51" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="G51" s="6"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="62"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -4307,21 +4380,22 @@
       <c r="R51" s="9"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="57">
-        <v>12</v>
-      </c>
-      <c r="B52" s="57">
-        <v>2</v>
-      </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="81" t="s">
+      <c r="A52" s="56">
+        <v>11</v>
+      </c>
+      <c r="B52" s="56">
+        <v>11.4</v>
+      </c>
+      <c r="C52" s="52"/>
+      <c r="D52" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="E52" s="60"/>
-      <c r="F52" s="81" t="s">
+      <c r="E52" s="48"/>
+      <c r="F52" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="G52" s="6"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="62"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -4338,20 +4412,20 @@
         <v>12</v>
       </c>
       <c r="B53" s="57">
-        <v>3</v>
+        <v>12.1</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="E53" s="19"/>
-      <c r="F53" s="11" t="s">
-        <v>200</v>
+        <v>11</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="60"/>
+      <c r="F53" s="81" t="s">
+        <v>202</v>
       </c>
       <c r="G53" s="80">
-        <v>43209</v>
+        <v>43221</v>
       </c>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
@@ -4365,26 +4439,23 @@
       <c r="R53" s="9"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="56">
-        <v>13</v>
-      </c>
-      <c r="B54" s="56">
-        <v>1</v>
-      </c>
-      <c r="C54" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="E54" s="48"/>
-      <c r="F54" s="66" t="s">
-        <v>200</v>
-      </c>
-      <c r="G54" s="79">
-        <v>43216</v>
-      </c>
-      <c r="H54" s="62"/>
+      <c r="A54" s="57">
+        <v>12</v>
+      </c>
+      <c r="B54" s="57">
+        <v>12.2</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="60"/>
+      <c r="F54" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="G54" s="80">
+        <v>43221</v>
+      </c>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -4397,26 +4468,23 @@
       <c r="R54" s="9"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="56">
-        <v>13</v>
-      </c>
-      <c r="B55" s="56">
-        <v>2</v>
-      </c>
-      <c r="C55" s="52" t="s">
+      <c r="A55" s="57">
+        <v>12</v>
+      </c>
+      <c r="B55" s="57">
+        <v>12.3</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="66" t="s">
-        <v>205</v>
-      </c>
-      <c r="E55" s="48"/>
-      <c r="F55" s="66" t="s">
-        <v>206</v>
-      </c>
-      <c r="G55" s="79">
-        <v>43214</v>
-      </c>
-      <c r="H55" s="62"/>
+      <c r="D55" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E55" s="19"/>
+      <c r="F55" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G55" s="80"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -4428,27 +4496,26 @@
       <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="56">
-        <v>13</v>
-      </c>
-      <c r="B56" s="56">
-        <v>3</v>
-      </c>
-      <c r="C56" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="E56" s="48"/>
-      <c r="F56" s="66" t="s">
-        <v>206</v>
-      </c>
-      <c r="G56" s="79">
-        <v>43218</v>
-      </c>
-      <c r="H56" s="62"/>
+    <row r="56" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="57">
+        <v>12</v>
+      </c>
+      <c r="B56" s="57">
+        <v>12.4</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="81" t="s">
+        <v>172</v>
+      </c>
+      <c r="E56" s="60"/>
+      <c r="F56" s="81" t="s">
+        <v>173</v>
+      </c>
+      <c r="G56" s="82">
+        <v>43208</v>
+      </c>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -4460,23 +4527,27 @@
       <c r="Q56" s="9"/>
       <c r="R56" s="9"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="57">
-        <v>14</v>
-      </c>
-      <c r="B57" s="57">
-        <v>1</v>
-      </c>
-      <c r="C57" s="12" t="s">
+    <row r="57" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="56">
+        <v>13</v>
+      </c>
+      <c r="B57" s="56">
+        <v>13.1</v>
+      </c>
+      <c r="C57" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E57" s="19"/>
-      <c r="G57" s="80">
-        <v>43221</v>
-      </c>
+      <c r="D57" s="66" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" s="48"/>
+      <c r="F57" s="66" t="s">
+        <v>205</v>
+      </c>
+      <c r="G57" s="79">
+        <v>43214</v>
+      </c>
+      <c r="H57" s="62"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -4489,23 +4560,26 @@
       <c r="R57" s="9"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="57">
-        <v>14</v>
-      </c>
-      <c r="B58" s="57">
-        <v>2</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E58" s="19"/>
-      <c r="F58" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G58" s="80"/>
+      <c r="A58" s="56">
+        <v>13</v>
+      </c>
+      <c r="B58" s="56">
+        <v>13.2</v>
+      </c>
+      <c r="C58" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="E58" s="48"/>
+      <c r="F58" s="66" t="s">
+        <v>205</v>
+      </c>
+      <c r="G58" s="79">
+        <v>43218</v>
+      </c>
+      <c r="H58" s="62"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -4522,17 +4596,18 @@
         <v>14</v>
       </c>
       <c r="B59" s="57">
-        <v>3</v>
-      </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="11" t="s">
-        <v>52</v>
+        <v>14.1</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="E59" s="19"/>
-      <c r="F59" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G59" s="80"/>
+      <c r="G59" s="80">
+        <v>43221</v>
+      </c>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -4545,26 +4620,27 @@
       <c r="R59" s="9"/>
     </row>
     <row r="60" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="57">
+      <c r="A60" s="58">
         <v>14</v>
       </c>
-      <c r="B60" s="57">
-        <v>4</v>
+      <c r="B60" s="58">
+        <v>14.2</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>80</v>
       </c>
       <c r="D60" s="81" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E60" s="60"/>
       <c r="F60" s="81" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G60" s="82">
-        <v>43210</v>
-      </c>
-      <c r="I60" s="9"/>
+        <v>43222</v>
+      </c>
+      <c r="H60" s="88"/>
+      <c r="I60" s="107"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
@@ -4575,25 +4651,26 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
     </row>
-    <row r="61" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="56">
-        <v>15</v>
-      </c>
-      <c r="B61" s="56">
-        <v>1</v>
-      </c>
-      <c r="C61" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D61" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="E61" s="48"/>
-      <c r="F61" s="66" t="s">
-        <v>177</v>
-      </c>
-      <c r="G61" s="68"/>
-      <c r="H61" s="62"/>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="57">
+        <v>14</v>
+      </c>
+      <c r="B61" s="57">
+        <v>14.3</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="E61" s="19"/>
+      <c r="F61" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="G61" s="80">
+        <v>43228</v>
+      </c>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -4606,22 +4683,23 @@
       <c r="R61" s="9"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="56">
-        <v>15</v>
-      </c>
-      <c r="B62" s="56">
-        <v>1</v>
-      </c>
-      <c r="C62" s="104" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="E62" s="105"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="68"/>
-      <c r="H62" s="62"/>
+      <c r="A62" s="57">
+        <v>14</v>
+      </c>
+      <c r="B62" s="57">
+        <v>14.4</v>
+      </c>
+      <c r="C62" s="17"/>
+      <c r="D62" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="E62" s="19"/>
+      <c r="F62" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="G62" s="80">
+        <v>43228</v>
+      </c>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -4638,15 +4716,19 @@
         <v>15</v>
       </c>
       <c r="B63" s="56">
-        <v>2</v>
-      </c>
-      <c r="C63" s="104"/>
+        <v>15.1</v>
+      </c>
+      <c r="C63" s="104" t="s">
+        <v>46</v>
+      </c>
       <c r="D63" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="E63" s="106"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="107"/>
+        <v>78</v>
+      </c>
+      <c r="E63" s="105"/>
+      <c r="F63" s="73"/>
+      <c r="G63" s="79">
+        <v>43231</v>
+      </c>
       <c r="H63" s="62"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
@@ -4660,22 +4742,22 @@
       <c r="R63" s="9"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="98">
-        <v>16</v>
-      </c>
-      <c r="B64" s="98">
-        <v>1</v>
-      </c>
-      <c r="C64" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="D64" s="100" t="s">
-        <v>204</v>
-      </c>
-      <c r="E64" s="101"/>
-      <c r="F64" s="100"/>
-      <c r="G64" s="102"/>
-      <c r="H64" s="103"/>
+      <c r="A64" s="56">
+        <v>15</v>
+      </c>
+      <c r="B64" s="56">
+        <v>15.2</v>
+      </c>
+      <c r="C64" s="104"/>
+      <c r="D64" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="E64" s="106"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="108">
+        <v>43238</v>
+      </c>
+      <c r="H64" s="62"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -4687,12 +4769,27 @@
       <c r="Q64" s="9"/>
       <c r="R64" s="9"/>
     </row>
-    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C65" s="14"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="6"/>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="56">
+        <v>15</v>
+      </c>
+      <c r="B65" s="56">
+        <v>15.3</v>
+      </c>
+      <c r="C65" s="104" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" s="73" t="s">
+        <v>228</v>
+      </c>
+      <c r="E65" s="106"/>
+      <c r="F65" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="G65" s="108">
+        <v>43229</v>
+      </c>
+      <c r="H65" s="62"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -4704,12 +4801,23 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="9"/>
     </row>
-    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="9"/>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="98">
+        <v>16</v>
+      </c>
+      <c r="B66" s="98">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C66" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="100" t="s">
+        <v>204</v>
+      </c>
+      <c r="E66" s="101"/>
+      <c r="F66" s="100"/>
+      <c r="G66" s="102"/>
+      <c r="H66" s="103"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -4721,12 +4829,12 @@
       <c r="Q66" s="9"/>
       <c r="R66" s="9"/>
     </row>
-    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C67" s="10"/>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C67" s="14"/>
       <c r="D67" s="10"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="8"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="6"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -4738,12 +4846,10 @@
       <c r="Q67" s="9"/>
       <c r="R67" s="9"/>
     </row>
-    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C68" s="14"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="8"/>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E68" s="5"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="9"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
@@ -4755,12 +4861,10 @@
       <c r="Q68" s="9"/>
       <c r="R68" s="9"/>
     </row>
-    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C69" s="14"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="6"/>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E69" s="21"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="8"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
@@ -4772,12 +4876,12 @@
       <c r="Q69" s="9"/>
       <c r="R69" s="9"/>
     </row>
-    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C70" s="14"/>
       <c r="D70" s="3"/>
       <c r="E70" s="19"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="9"/>
+      <c r="G70" s="8"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -4789,7 +4893,7 @@
       <c r="Q70" s="9"/>
       <c r="R70" s="9"/>
     </row>
-    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C71" s="14"/>
       <c r="D71" s="3"/>
       <c r="E71" s="19"/>
@@ -4806,7 +4910,7 @@
       <c r="Q71" s="9"/>
       <c r="R71" s="9"/>
     </row>
-    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C72" s="14"/>
       <c r="D72" s="3"/>
       <c r="E72" s="19"/>
@@ -4823,12 +4927,12 @@
       <c r="Q72" s="9"/>
       <c r="R72" s="9"/>
     </row>
-    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C73" s="14"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="8"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="6"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
@@ -4840,7 +4944,7 @@
       <c r="Q73" s="9"/>
       <c r="R73" s="9"/>
     </row>
-    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C74" s="14"/>
       <c r="D74" s="3"/>
       <c r="E74" s="19"/>
@@ -4857,12 +4961,12 @@
       <c r="Q74" s="9"/>
       <c r="R74" s="9"/>
     </row>
-    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C75" s="14"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="6"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="8"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
@@ -4874,8 +4978,11 @@
       <c r="Q75" s="9"/>
       <c r="R75" s="9"/>
     </row>
-    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C76" s="14"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="3"/>
       <c r="G76" s="9"/>
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
@@ -4888,11 +4995,12 @@
       <c r="Q76" s="9"/>
       <c r="R76" s="9"/>
     </row>
-    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C77" s="18"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="7"/>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C77" s="14"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="6"/>
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
@@ -4904,11 +5012,8 @@
       <c r="Q77" s="9"/>
       <c r="R77" s="9"/>
     </row>
-    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C78" s="18"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="7"/>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C78" s="14"/>
       <c r="G78" s="9"/>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
@@ -4921,12 +5026,11 @@
       <c r="Q78" s="9"/>
       <c r="R78" s="9"/>
     </row>
-    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C79" s="18"/>
       <c r="D79" s="7"/>
       <c r="E79" s="21"/>
       <c r="F79" s="7"/>
-      <c r="G79" s="9"/>
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
@@ -4938,7 +5042,7 @@
       <c r="Q79" s="9"/>
       <c r="R79" s="9"/>
     </row>
-    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C80" s="18"/>
       <c r="D80" s="7"/>
       <c r="E80" s="21"/>
@@ -21701,6 +21805,10 @@
       <c r="R1065" s="9"/>
     </row>
     <row r="1066" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C1066" s="18"/>
+      <c r="D1066" s="7"/>
+      <c r="E1066" s="21"/>
+      <c r="F1066" s="7"/>
       <c r="G1066" s="9"/>
       <c r="I1066" s="9"/>
       <c r="J1066" s="9"/>
@@ -21714,6 +21822,10 @@
       <c r="R1066" s="9"/>
     </row>
     <row r="1067" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C1067" s="18"/>
+      <c r="D1067" s="7"/>
+      <c r="E1067" s="21"/>
+      <c r="F1067" s="7"/>
       <c r="G1067" s="9"/>
       <c r="I1067" s="9"/>
       <c r="J1067" s="9"/>
@@ -21739,60 +21851,90 @@
       <c r="Q1068" s="9"/>
       <c r="R1068" s="9"/>
     </row>
+    <row r="1069" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="G1069" s="9"/>
+      <c r="I1069" s="9"/>
+      <c r="J1069" s="9"/>
+      <c r="K1069" s="9"/>
+      <c r="L1069" s="9"/>
+      <c r="M1069" s="9"/>
+      <c r="N1069" s="9"/>
+      <c r="O1069" s="9"/>
+      <c r="P1069" s="9"/>
+      <c r="Q1069" s="9"/>
+      <c r="R1069" s="9"/>
+    </row>
+    <row r="1070" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="G1070" s="9"/>
+      <c r="I1070" s="9"/>
+      <c r="J1070" s="9"/>
+      <c r="K1070" s="9"/>
+      <c r="L1070" s="9"/>
+      <c r="M1070" s="9"/>
+      <c r="N1070" s="9"/>
+      <c r="O1070" s="9"/>
+      <c r="P1070" s="9"/>
+      <c r="Q1070" s="9"/>
+      <c r="R1070" s="9"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31 G55 G61:G1048576 G57:G59 G37:G52">
-    <cfRule type="timePeriod" dxfId="10" priority="12" timePeriod="last7Days">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R1074">
+    <sortCondition ref="A2:A1074"/>
+    <sortCondition ref="B2:B1074"/>
+  </sortState>
+  <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31 G56 G62:G1048576 G58:G60 G37:G46 G49:G54">
+    <cfRule type="timePeriod" dxfId="10" priority="13" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G1,1)&lt;=6,FLOOR(G1,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="timePeriod" dxfId="9" priority="11" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="9" priority="12" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G26,1)&lt;=6,FLOOR(G26,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="timePeriod" dxfId="8" priority="10" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="8" priority="11" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G22,1)&lt;=6,FLOOR(G22,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="timePeriod" dxfId="7" priority="9" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="7" priority="10" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G23,1)&lt;=6,FLOOR(G23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="timePeriod" dxfId="6" priority="8" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="6" priority="9" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G30,1)&lt;=6,FLOOR(G30,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:G36">
-    <cfRule type="timePeriod" dxfId="5" priority="6" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G34,1)&lt;=6,FLOOR(G34,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G33">
-    <cfRule type="timePeriod" dxfId="4" priority="5" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G32,1)&lt;=6,FLOOR(G32,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
-    <cfRule type="timePeriod" dxfId="3" priority="4" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(G53,1)&lt;=6,FLOOR(G53,1)&lt;=TODAY())</formula>
+  <conditionalFormatting sqref="G55">
+    <cfRule type="timePeriod" dxfId="3" priority="5" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G55,1)&lt;=6,FLOOR(G55,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(G56,1)&lt;=6,FLOOR(G56,1)&lt;=TODAY())</formula>
+  <conditionalFormatting sqref="G57">
+    <cfRule type="timePeriod" dxfId="2" priority="4" timePeriod="last7Days">
+      <formula>AND(TODAY()-FLOOR(G57,1)&lt;=6,FLOOR(G57,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G54">
+  <conditionalFormatting sqref="G61">
     <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(G54,1)&lt;=6,FLOOR(G54,1)&lt;=TODAY())</formula>
+      <formula>AND(TODAY()-FLOOR(G61,1)&lt;=6,FLOOR(G61,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G60">
+  <conditionalFormatting sqref="G47:G48">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="last7Days">
-      <formula>AND(TODAY()-FLOOR(G60,1)&lt;=6,FLOOR(G60,1)&lt;=TODAY())</formula>
+      <formula>AND(TODAY()-FLOOR(G47,1)&lt;=6,FLOOR(G47,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
update week 8 and add week 10
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4225A441-5FA7-433D-A5F5-169D32D9BE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76BD80C-35F2-4B3C-A358-C6B72E34D48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30795" yWindow="1260" windowWidth="22905" windowHeight="13815" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -692,9 +692,6 @@
     <t>DataFest (Optional)</t>
   </si>
   <si>
-    <t>Read RAT Part 2 and answer discussion questions in [HackMD](https://hackmd.io/@norcalbiostat/default_discrimination). We'll discuss in class on 3/31</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pull an update to your ISLR repo. Read/watch ISLR Chapter 4 content &amp; prepare answers to questions to discuss in class. We'll spend half the class each day on this topic. </t>
   </si>
   <si>
@@ -755,6 +752,9 @@
   </si>
   <si>
     <t>No class on Thursday</t>
+  </si>
+  <si>
+    <t>Read RAT Part 2 and answer discussion questions in [HackMD](https://hackmd.io/@norcalbiostat/default_discrimination). We'll discuss in class on 4/05</t>
   </si>
 </sst>
 </file>
@@ -1887,8 +1887,8 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="18" spans="1:10" ht="63.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B18" s="95">
         <v>8.1</v>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="E18" s="45"/>
       <c r="F18" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G18" s="45"/>
       <c r="H18" s="41"/>
@@ -2360,7 +2360,7 @@
         <v>148</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G19" s="72"/>
       <c r="H19" s="42"/>
@@ -2398,11 +2398,11 @@
         <v>43189</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E21" s="41"/>
       <c r="F21" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
@@ -2430,7 +2430,7 @@
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2453,23 +2453,23 @@
       <c r="I23" s="41"/>
       <c r="J23" s="41"/>
     </row>
-    <row r="24" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="91">
+    <row r="24" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
+      <c r="B24" s="92">
         <v>10.199999999999999</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="41" t="s">
+      <c r="C24" s="33"/>
+      <c r="D24" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41" t="s">
-        <v>211</v>
-      </c>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
@@ -2556,11 +2556,11 @@
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -2628,11 +2628,11 @@
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E33" s="41"/>
       <c r="F33" s="41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G33" s="41"/>
       <c r="H33" s="41"/>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="E34" s="67"/>
       <c r="F34" s="66" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G34" s="50">
         <v>43179</v>
@@ -3915,7 +3915,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="11" t="s">
@@ -3949,7 +3949,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="11" t="s">
@@ -3983,7 +3983,7 @@
         <v>147</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="11" t="s">
@@ -4017,7 +4017,7 @@
         <v>10</v>
       </c>
       <c r="D40" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E40" s="48"/>
       <c r="F40" s="66" t="s">
@@ -4049,7 +4049,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E41" s="48"/>
       <c r="F41" s="66" t="s">
@@ -4081,7 +4081,7 @@
         <v>153</v>
       </c>
       <c r="D42" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E42" s="48"/>
       <c r="F42" s="66" t="s">
@@ -4538,7 +4538,7 @@
         <v>27</v>
       </c>
       <c r="D57" s="66" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E57" s="48"/>
       <c r="F57" s="66" t="s">
@@ -4780,7 +4780,7 @@
         <v>153</v>
       </c>
       <c r="D65" s="73" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E65" s="106"/>
       <c r="F65" s="47" t="s">

</xml_diff>

<commit_message>
add notes to wk11
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16908FF1-A5BC-40A7-87E9-F590DE32B790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83216D79-5C1D-4D55-8B73-945850182D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -791,7 +791,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -883,6 +883,12 @@
     <font>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1053,7 +1059,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1383,6 +1389,9 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1479,17 +1488,7 @@
     <cellStyle name="Normal 3 2" xfId="91" xr:uid="{20B637C8-DD27-499C-BEC0-85B72C712ADD}"/>
     <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2737,8 +2736,8 @@
   <dimension ref="A1:R1071"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A2:A52"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4309,7 +4308,7 @@
       <c r="R46" s="7"/>
     </row>
     <row r="47" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="109">
+      <c r="A47" s="113">
         <v>11</v>
       </c>
       <c r="B47" s="53">
@@ -4343,7 +4342,7 @@
       <c r="R47" s="7"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="109">
+      <c r="A48" s="113">
         <v>11</v>
       </c>
       <c r="B48" s="53">
@@ -4377,7 +4376,7 @@
       <c r="R48" s="7"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="109">
+      <c r="A49" s="113">
         <v>11</v>
       </c>
       <c r="B49" s="53">
@@ -4411,7 +4410,7 @@
       <c r="R49" s="7"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="109">
+      <c r="A50" s="113">
         <v>11</v>
       </c>
       <c r="B50" s="53">
@@ -4443,7 +4442,7 @@
       <c r="R50" s="7"/>
     </row>
     <row r="51" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="109">
+      <c r="A51" s="113">
         <v>11</v>
       </c>
       <c r="B51" s="53">
@@ -4477,7 +4476,7 @@
       <c r="R51" s="7"/>
     </row>
     <row r="52" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A52" s="109">
+      <c r="A52" s="113">
         <v>11</v>
       </c>
       <c r="B52" s="53">
@@ -21051,52 +21050,52 @@
     <sortCondition ref="B2:B1075"/>
   </sortState>
   <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31 G55:G56 G63:G1048576 G59:G61 G37:G53">
-    <cfRule type="timePeriod" dxfId="10" priority="13" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="9" priority="13" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G1,1)&lt;=6,FLOOR(G1,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="timePeriod" dxfId="9" priority="12" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="8" priority="12" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G26,1)&lt;=6,FLOOR(G26,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="timePeriod" dxfId="8" priority="11" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="7" priority="11" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G22,1)&lt;=6,FLOOR(G22,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="timePeriod" dxfId="7" priority="10" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="6" priority="10" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G23,1)&lt;=6,FLOOR(G23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="timePeriod" dxfId="6" priority="9" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="5" priority="9" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G30,1)&lt;=6,FLOOR(G30,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:G36">
-    <cfRule type="timePeriod" dxfId="5" priority="7" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="4" priority="7" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G34,1)&lt;=6,FLOOR(G34,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G33">
-    <cfRule type="timePeriod" dxfId="4" priority="6" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="3" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G32,1)&lt;=6,FLOOR(G32,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="timePeriod" dxfId="3" priority="5" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="2" priority="5" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G54,1)&lt;=6,FLOOR(G54,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G58">
-    <cfRule type="timePeriod" dxfId="2" priority="4" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="1" priority="4" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G57,1)&lt;=6,FLOOR(G57,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G62,1)&lt;=6,FLOOR(G62,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
remove ch12 from lesson plan
</commit_message>
<xml_diff>
--- a/schedule_485.xlsx
+++ b/schedule_485.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FA42D6-1691-4749-A3B5-4289847E9581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A387E723-7FFA-4C6C-9BA7-602C579F85EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="246">
   <si>
     <t>SLO</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Accept invite to github classroom</t>
-  </si>
-  <si>
-    <t>Unsupervised Clustering</t>
   </si>
   <si>
     <t>Send via Discord</t>
@@ -558,9 +555,6 @@
     <t>Classwide &amp; Client project share out</t>
   </si>
   <si>
-    <t>Unsupervised Learning</t>
-  </si>
-  <si>
     <t>Retooling Solidarity, Reimagining Justice</t>
   </si>
   <si>
@@ -745,12 +739,6 @@
     <t>In class</t>
   </si>
   <si>
-    <t>ISLR Ch 12 - Collaborative notes</t>
-  </si>
-  <si>
-    <t>ISLR Ch 12 - Practice Exercises</t>
-  </si>
-  <si>
     <t xml:space="preserve">Communicate your project as parts/whole of the data science lifecycle to a scientific, but non technical audience. </t>
   </si>
   <si>
@@ -794,9 +782,6 @@
   </si>
   <si>
     <t>Formal 30 minute stakeholder presentations. 12pm - 2pm. (15 minute presentation, 10 minute discussion / Q&amp;A)</t>
-  </si>
-  <si>
-    <t>ISLR Ch 12</t>
   </si>
   <si>
     <t>Project Reflection</t>
@@ -1089,7 +1074,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1366,9 +1351,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,6 +1403,12 @@
     </xf>
     <xf numFmtId="16" fontId="7" fillId="5" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="93">
@@ -1959,11 +1947,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1982,10 +1970,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="81" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>1</v>
@@ -1997,10 +1985,10 @@
         <v>0</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>22</v>
@@ -2014,7 +2002,7 @@
     </row>
     <row r="2" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" s="82">
         <v>1.1000000000000001</v>
@@ -2023,23 +2011,23 @@
         <v>43124</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2051,26 +2039,26 @@
         <v>43126</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="33"/>
       <c r="G3" s="33" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="33"/>
       <c r="J3" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B4" s="84">
         <v>2.1</v>
@@ -2079,30 +2067,30 @@
         <v>43131</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>86</v>
-      </c>
       <c r="I4" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B5" s="82">
         <v>3.1</v>
@@ -2111,22 +2099,22 @@
         <v>43138</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>93</v>
-      </c>
       <c r="I5" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J5" s="39"/>
     </row>
@@ -2145,16 +2133,16 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
       <c r="H6" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="40"/>
       <c r="J6" s="40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" s="82">
         <v>4.0999999999999996</v>
@@ -2163,19 +2151,19 @@
         <v>43145</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
       <c r="I7" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -2187,28 +2175,28 @@
         <v>43147</v>
       </c>
       <c r="D8" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="40" t="s">
-        <v>106</v>
-      </c>
       <c r="F8" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" s="40"/>
       <c r="J8" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B9" s="82">
         <v>5.0999999999999996</v>
@@ -2220,7 +2208,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
@@ -2235,13 +2223,13 @@
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="39" t="s">
-        <v>127</v>
-      </c>
       <c r="F10" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G10" s="39"/>
       <c r="H10" s="39"/>
@@ -2257,24 +2245,24 @@
         <v>43154</v>
       </c>
       <c r="D11" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="40" t="s">
         <v>99</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>100</v>
       </c>
       <c r="G11" s="40"/>
       <c r="H11" s="40"/>
       <c r="I11" s="40"/>
       <c r="J11" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="189" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B12" s="82">
         <v>6.1</v>
@@ -2283,11 +2271,11 @@
         <v>43159</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
@@ -2305,11 +2293,11 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
@@ -2323,10 +2311,10 @@
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="64" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
@@ -2336,7 +2324,7 @@
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B15" s="82">
         <v>7.1</v>
@@ -2345,18 +2333,18 @@
         <v>43166</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J15" s="39"/>
     </row>
@@ -2367,16 +2355,16 @@
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J16" s="39"/>
     </row>
@@ -2391,18 +2379,18 @@
       </c>
       <c r="E17" s="77"/>
       <c r="F17" s="77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G17" s="77"/>
       <c r="H17" s="77"/>
       <c r="I17" s="77"/>
       <c r="J17" s="77" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="63.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B18" s="86">
         <v>8.1</v>
@@ -2415,7 +2403,7 @@
       </c>
       <c r="E18" s="43"/>
       <c r="F18" s="39" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G18" s="43"/>
       <c r="H18" s="39"/>
@@ -2429,13 +2417,13 @@
       </c>
       <c r="C19" s="66"/>
       <c r="D19" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="67" t="s">
-        <v>135</v>
-      </c>
       <c r="F19" s="40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G19" s="67"/>
       <c r="H19" s="40"/>
@@ -2444,7 +2432,7 @@
     </row>
     <row r="20" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B20" s="86">
         <v>9.1</v>
@@ -2457,7 +2445,7 @@
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
@@ -2473,11 +2461,11 @@
         <v>43189</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="39" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
@@ -2493,24 +2481,24 @@
         <v>43190</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E22" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G22" s="40"/>
       <c r="H22" s="40"/>
       <c r="I22" s="40"/>
       <c r="J22" s="40" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B23" s="83">
         <v>10.1</v>
@@ -2519,11 +2507,11 @@
         <v>43194</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" s="40"/>
       <c r="F23" s="40" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G23" s="40"/>
       <c r="H23" s="40"/>
@@ -2532,7 +2520,7 @@
     </row>
     <row r="24" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B24" s="82">
         <v>11.1</v>
@@ -2545,7 +2533,7 @@
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
@@ -2561,11 +2549,11 @@
         <v>43203</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" s="40"/>
       <c r="F25" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G25" s="40"/>
       <c r="H25" s="40"/>
@@ -2587,7 +2575,7 @@
       </c>
       <c r="E26" s="39"/>
       <c r="F26" s="39" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
@@ -2601,11 +2589,11 @@
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="39" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
@@ -2623,11 +2611,11 @@
         <v>43215</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
@@ -2636,7 +2624,7 @@
     </row>
     <row r="29" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B29" s="82">
         <v>14.1</v>
@@ -2645,11 +2633,11 @@
         <v>43222</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
@@ -2657,55 +2645,55 @@
       <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="27" t="s">
+        <v>242</v>
+      </c>
       <c r="B30" s="82">
-        <v>14.2</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39" t="s">
-        <v>161</v>
-      </c>
+        <v>15.1</v>
+      </c>
+      <c r="C30" s="28">
+        <v>43229</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
       <c r="I30" s="39"/>
       <c r="J30" s="39"/>
     </row>
-    <row r="31" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>247</v>
-      </c>
+    <row r="31" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
       <c r="B31" s="82">
-        <v>15.1</v>
-      </c>
-      <c r="C31" s="28">
-        <v>43229</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+        <v>15.2</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39" t="s">
+        <v>227</v>
+      </c>
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
       <c r="J31" s="39"/>
     </row>
-    <row r="32" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="82">
-        <v>15.2</v>
+        <v>15.3</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="39" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="E32" s="39"/>
       <c r="F32" s="39" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
@@ -2713,56 +2701,38 @@
       <c r="J32" s="39"/>
     </row>
     <row r="33" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="27" t="s">
+        <v>237</v>
+      </c>
       <c r="B33" s="82">
-        <v>15.3</v>
-      </c>
-      <c r="C33" s="28"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C33" s="28">
+        <v>43236</v>
+      </c>
       <c r="D33" s="39" t="s">
-        <v>168</v>
-      </c>
-      <c r="E33" s="39"/>
+        <v>12</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>226</v>
+      </c>
       <c r="F33" s="39" t="s">
-        <v>162</v>
+        <v>240</v>
       </c>
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
       <c r="I33" s="39"/>
       <c r="J33" s="39"/>
     </row>
-    <row r="34" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="B34" s="82">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="C34" s="28">
-        <v>43236</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="F34" s="39" t="s">
-        <v>244</v>
-      </c>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="88">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="88">
         <v>16.2</v>
       </c>
-      <c r="D35" s="43" t="s">
-        <v>242</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>243</v>
+      <c r="D34" s="43" t="s">
+        <v>238</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2774,11 +2744,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBC2D3D-FE18-4FBF-825C-8A0A6D387E1B}">
-  <dimension ref="A1:R1071"/>
+  <dimension ref="A1:R1069"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2788,17 +2758,17 @@
     <col min="4" max="4" width="46.625" style="9" customWidth="1"/>
     <col min="5" max="5" width="15.375" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="9.375" style="107" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="106" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.375" style="6" customWidth="1"/>
     <col min="9" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>14</v>
@@ -2807,7 +2777,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>20</v>
@@ -2830,7 +2800,7 @@
       <c r="R1" s="7"/>
     </row>
     <row r="2" spans="1:18" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="108">
+      <c r="A2" s="107">
         <v>1</v>
       </c>
       <c r="B2" s="53">
@@ -2840,13 +2810,13 @@
         <v>17</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="46"/>
       <c r="F2" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="99">
+        <v>115</v>
+      </c>
+      <c r="G2" s="98">
         <v>43125</v>
       </c>
       <c r="H2" s="58">
@@ -2864,7 +2834,7 @@
       <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="108">
+      <c r="A3" s="107">
         <v>1</v>
       </c>
       <c r="B3" s="53">
@@ -2876,9 +2846,9 @@
       </c>
       <c r="E3" s="46"/>
       <c r="F3" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="99">
+        <v>30</v>
+      </c>
+      <c r="G3" s="98">
         <v>43125</v>
       </c>
       <c r="H3" s="58">
@@ -2896,7 +2866,7 @@
       <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="108">
+      <c r="A4" s="107">
         <v>1</v>
       </c>
       <c r="B4" s="53">
@@ -2908,9 +2878,9 @@
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="99">
+        <v>37</v>
+      </c>
+      <c r="G4" s="98">
         <v>43125</v>
       </c>
       <c r="H4" s="58">
@@ -2928,7 +2898,7 @@
       <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A5" s="108">
+      <c r="A5" s="107">
         <v>1</v>
       </c>
       <c r="B5" s="53">
@@ -2936,13 +2906,13 @@
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="46"/>
       <c r="F5" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" s="99">
+        <v>114</v>
+      </c>
+      <c r="G5" s="98">
         <v>43125</v>
       </c>
       <c r="H5" s="58">
@@ -2960,7 +2930,7 @@
       <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A6" s="108">
+      <c r="A6" s="107">
         <v>1</v>
       </c>
       <c r="B6" s="53">
@@ -2968,13 +2938,13 @@
       </c>
       <c r="C6" s="44"/>
       <c r="D6" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="99">
+        <v>27</v>
+      </c>
+      <c r="G6" s="98">
         <v>43125</v>
       </c>
       <c r="H6" s="58">
@@ -2992,7 +2962,7 @@
       <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="108">
+      <c r="A7" s="107">
         <v>1</v>
       </c>
       <c r="B7" s="53">
@@ -3000,13 +2970,13 @@
       </c>
       <c r="C7" s="44"/>
       <c r="D7" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="99">
+        <v>116</v>
+      </c>
+      <c r="G7" s="98">
         <v>43125</v>
       </c>
       <c r="H7" s="58">
@@ -3024,7 +2994,7 @@
       <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="108">
+      <c r="A8" s="107">
         <v>1</v>
       </c>
       <c r="B8" s="53">
@@ -3032,13 +3002,13 @@
       </c>
       <c r="C8" s="44"/>
       <c r="D8" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="G8" s="99">
+        <v>117</v>
+      </c>
+      <c r="G8" s="98">
         <v>43127</v>
       </c>
       <c r="H8" s="58">
@@ -3056,7 +3026,7 @@
       <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="108">
+      <c r="A9" s="107">
         <v>1</v>
       </c>
       <c r="B9" s="53">
@@ -3068,9 +3038,9 @@
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="99">
+        <v>26</v>
+      </c>
+      <c r="G9" s="98">
         <v>43125</v>
       </c>
       <c r="H9" s="58">
@@ -3088,25 +3058,25 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="108">
+      <c r="A10" s="107">
         <v>1</v>
       </c>
       <c r="B10" s="53">
         <v>1.9</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="46">
         <v>2</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="G10" s="99">
+        <v>118</v>
+      </c>
+      <c r="G10" s="98">
         <v>43132</v>
       </c>
       <c r="H10" s="58">
@@ -3124,14 +3094,14 @@
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="109">
+      <c r="A11" s="108">
         <v>2</v>
       </c>
       <c r="B11" s="54">
         <v>2.1</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>18</v>
@@ -3140,9 +3110,9 @@
         <v>2</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11" s="100">
+        <v>119</v>
+      </c>
+      <c r="G11" s="99">
         <v>43137</v>
       </c>
       <c r="H11" s="6">
@@ -3160,7 +3130,7 @@
       <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="109">
+      <c r="A12" s="108">
         <v>2</v>
       </c>
       <c r="B12" s="54">
@@ -3174,9 +3144,9 @@
         <v>2</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="100">
+        <v>120</v>
+      </c>
+      <c r="G12" s="99">
         <v>43137</v>
       </c>
       <c r="H12" s="6">
@@ -3194,25 +3164,25 @@
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="109">
+      <c r="A13" s="108">
         <v>2</v>
       </c>
       <c r="B13" s="54">
         <v>2.2999999999999998</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="17">
         <v>6</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13" s="100">
+        <v>121</v>
+      </c>
+      <c r="G13" s="99">
         <v>43133</v>
       </c>
       <c r="H13" s="6">
@@ -3230,7 +3200,7 @@
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="109">
+      <c r="A14" s="108">
         <v>2</v>
       </c>
       <c r="B14" s="54">
@@ -3238,15 +3208,15 @@
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="17">
         <v>7</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="100">
+        <v>93</v>
+      </c>
+      <c r="G14" s="99">
         <v>43137</v>
       </c>
       <c r="H14" s="6">
@@ -3264,7 +3234,7 @@
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="109">
+      <c r="A15" s="108">
         <v>2</v>
       </c>
       <c r="B15" s="54">
@@ -3272,15 +3242,15 @@
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="17">
         <v>7</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="100">
+        <v>53</v>
+      </c>
+      <c r="G15" s="99">
         <v>43134</v>
       </c>
       <c r="H15" s="6">
@@ -3298,7 +3268,7 @@
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="109">
+      <c r="A16" s="108">
         <v>2</v>
       </c>
       <c r="B16" s="54">
@@ -3306,15 +3276,15 @@
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="17">
         <v>7</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="100">
+        <v>53</v>
+      </c>
+      <c r="G16" s="99">
         <v>43137</v>
       </c>
       <c r="H16" s="6">
@@ -3332,7 +3302,7 @@
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="109">
+      <c r="A17" s="108">
         <v>2</v>
       </c>
       <c r="B17" s="54">
@@ -3340,15 +3310,15 @@
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="17">
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="100">
+        <v>65</v>
+      </c>
+      <c r="G17" s="99">
         <v>43141</v>
       </c>
       <c r="H17" s="6">
@@ -3366,7 +3336,7 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="109">
+      <c r="A18" s="108">
         <v>2</v>
       </c>
       <c r="B18" s="54">
@@ -3374,15 +3344,15 @@
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="17">
         <v>6</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="100">
+        <v>53</v>
+      </c>
+      <c r="G18" s="99">
         <v>43144</v>
       </c>
       <c r="H18" s="6">
@@ -3400,25 +3370,25 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="108">
+      <c r="A19" s="107">
         <v>3</v>
       </c>
       <c r="B19" s="53">
         <v>3.1</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="46">
         <v>5</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" s="99">
+        <v>122</v>
+      </c>
+      <c r="G19" s="98">
         <v>43145</v>
       </c>
       <c r="H19" s="58">
@@ -3436,7 +3406,7 @@
       <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="108">
+      <c r="A20" s="107">
         <v>3</v>
       </c>
       <c r="B20" s="53">
@@ -3446,13 +3416,13 @@
         <v>24</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="99">
+        <v>69</v>
+      </c>
+      <c r="G20" s="98">
         <v>43143</v>
       </c>
       <c r="H20" s="58">
@@ -3470,23 +3440,23 @@
       <c r="R20" s="7"/>
     </row>
     <row r="21" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A21" s="109">
+      <c r="A21" s="108">
         <v>4</v>
       </c>
       <c r="B21" s="54">
         <v>4.0999999999999996</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G21" s="100">
+        <v>136</v>
+      </c>
+      <c r="G21" s="99">
         <v>43146</v>
       </c>
       <c r="H21" s="6">
@@ -3504,25 +3474,25 @@
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="110">
+      <c r="A22" s="109">
         <v>4</v>
       </c>
       <c r="B22" s="55">
         <v>4.2</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" s="57">
         <v>5</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="101">
+        <v>106</v>
+      </c>
+      <c r="G22" s="100">
         <v>43151</v>
       </c>
       <c r="H22" s="79">
@@ -3540,7 +3510,7 @@
       <c r="R22" s="7"/>
     </row>
     <row r="23" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="110">
+      <c r="A23" s="109">
         <v>4</v>
       </c>
       <c r="B23" s="55">
@@ -3550,13 +3520,13 @@
         <v>24</v>
       </c>
       <c r="D23" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" s="57"/>
       <c r="F23" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="G23" s="101">
+        <v>123</v>
+      </c>
+      <c r="G23" s="100">
         <v>43158</v>
       </c>
       <c r="H23" s="79">
@@ -3574,7 +3544,7 @@
       <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="108">
+      <c r="A24" s="107">
         <v>5</v>
       </c>
       <c r="B24" s="53">
@@ -3584,15 +3554,15 @@
         <v>8</v>
       </c>
       <c r="D24" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" s="46">
         <v>5</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="G24" s="99">
+        <v>124</v>
+      </c>
+      <c r="G24" s="98">
         <v>43159</v>
       </c>
       <c r="H24" s="58">
@@ -3610,23 +3580,23 @@
       <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A25" s="108">
+      <c r="A25" s="107">
         <v>5</v>
       </c>
       <c r="B25" s="53">
         <v>5.2</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25" s="46"/>
       <c r="F25" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="G25" s="99">
+        <v>137</v>
+      </c>
+      <c r="G25" s="98">
         <v>43153</v>
       </c>
       <c r="H25" s="58">
@@ -3644,7 +3614,7 @@
       <c r="R25" s="7"/>
     </row>
     <row r="26" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="108">
+      <c r="A26" s="107">
         <v>5</v>
       </c>
       <c r="B26" s="53">
@@ -3654,13 +3624,13 @@
         <v>24</v>
       </c>
       <c r="D26" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E26" s="46"/>
       <c r="F26" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="G26" s="99">
+        <v>109</v>
+      </c>
+      <c r="G26" s="98">
         <v>43151</v>
       </c>
       <c r="H26" s="58">
@@ -3678,7 +3648,7 @@
       <c r="R26" s="7"/>
     </row>
     <row r="27" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="108">
+      <c r="A27" s="107">
         <v>5</v>
       </c>
       <c r="B27" s="53">
@@ -3686,13 +3656,13 @@
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E27" s="46"/>
       <c r="F27" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="G27" s="99">
+        <v>138</v>
+      </c>
+      <c r="G27" s="98">
         <v>43153</v>
       </c>
       <c r="H27" s="58">
@@ -3710,23 +3680,23 @@
       <c r="R27" s="7"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="109">
+      <c r="A28" s="108">
         <v>6</v>
       </c>
       <c r="B28" s="54">
         <v>6.1</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" s="100">
+        <v>146</v>
+      </c>
+      <c r="G28" s="99">
         <v>43165</v>
       </c>
       <c r="H28" s="6">
@@ -3744,22 +3714,22 @@
       <c r="R28" s="7"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="109">
+      <c r="A29" s="108">
         <v>6</v>
       </c>
       <c r="B29" s="54">
         <v>6.2</v>
       </c>
       <c r="C29" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G29" s="100">
+      <c r="G29" s="99">
         <v>43165</v>
       </c>
       <c r="H29" s="6">
@@ -3777,7 +3747,7 @@
       <c r="R29" s="7"/>
     </row>
     <row r="30" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="109">
+      <c r="A30" s="108">
         <v>6</v>
       </c>
       <c r="B30" s="54">
@@ -3787,12 +3757,12 @@
         <v>24</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G30" s="101">
+      <c r="G30" s="100">
         <v>43160</v>
       </c>
       <c r="H30" s="6">
@@ -3810,22 +3780,22 @@
       <c r="R30" s="7"/>
     </row>
     <row r="31" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="109">
+      <c r="A31" s="108">
         <v>6</v>
       </c>
       <c r="B31" s="54">
         <v>6.4</v>
       </c>
       <c r="C31" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="39" t="s">
-        <v>141</v>
-      </c>
       <c r="F31" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G31" s="100">
+        <v>69</v>
+      </c>
+      <c r="G31" s="99">
         <v>43165</v>
       </c>
       <c r="H31" s="6">
@@ -3843,23 +3813,23 @@
       <c r="R31" s="7"/>
     </row>
     <row r="32" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="108">
+      <c r="A32" s="107">
         <v>7</v>
       </c>
       <c r="B32" s="53">
         <v>7.1</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E32" s="63"/>
       <c r="F32" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="99">
+        <v>150</v>
+      </c>
+      <c r="G32" s="98">
         <v>43166</v>
       </c>
       <c r="H32" s="58">
@@ -3877,7 +3847,7 @@
       <c r="R32" s="7"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="108">
+      <c r="A33" s="107">
         <v>7</v>
       </c>
       <c r="B33" s="53">
@@ -3887,11 +3857,11 @@
         <v>24</v>
       </c>
       <c r="D33" s="62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E33" s="63"/>
       <c r="F33" s="62"/>
-      <c r="G33" s="99">
+      <c r="G33" s="98">
         <v>43168</v>
       </c>
       <c r="H33" s="58">
@@ -3909,23 +3879,23 @@
       <c r="R33" s="7"/>
     </row>
     <row r="34" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A34" s="108">
+      <c r="A34" s="107">
         <v>7</v>
       </c>
       <c r="B34" s="53">
         <v>7.3</v>
       </c>
       <c r="C34" s="61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="62" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E34" s="63"/>
       <c r="F34" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="G34" s="99">
+        <v>200</v>
+      </c>
+      <c r="G34" s="98">
         <v>43179</v>
       </c>
       <c r="H34" s="58">
@@ -3943,23 +3913,23 @@
       <c r="R34" s="7"/>
     </row>
     <row r="35" spans="1:18" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="108">
+      <c r="A35" s="107">
         <v>7</v>
       </c>
       <c r="B35" s="53">
         <v>7.4</v>
       </c>
       <c r="C35" s="61" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D35" s="62" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E35" s="63"/>
       <c r="F35" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" s="99">
+        <v>53</v>
+      </c>
+      <c r="G35" s="98">
         <v>43182</v>
       </c>
       <c r="H35" s="58">
@@ -3977,23 +3947,23 @@
       <c r="R35" s="7"/>
     </row>
     <row r="36" spans="1:18" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="111">
+      <c r="A36" s="110">
         <v>7</v>
       </c>
       <c r="B36" s="69">
         <v>7.5</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D36" s="71" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E36" s="72"/>
       <c r="F36" s="71" t="s">
-        <v>212</v>
-      </c>
-      <c r="G36" s="102">
+        <v>210</v>
+      </c>
+      <c r="G36" s="101">
         <v>43179</v>
       </c>
       <c r="H36" s="80">
@@ -4011,7 +3981,7 @@
       <c r="R36" s="7"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="109">
+      <c r="A37" s="108">
         <v>8</v>
       </c>
       <c r="B37" s="54">
@@ -4021,13 +3991,13 @@
         <v>9</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E37" s="19"/>
       <c r="F37" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G37" s="103">
+        <v>185</v>
+      </c>
+      <c r="G37" s="102">
         <v>43186</v>
       </c>
       <c r="H37" s="6">
@@ -4045,7 +4015,7 @@
       <c r="R37" s="7"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="109">
+      <c r="A38" s="108">
         <v>8</v>
       </c>
       <c r="B38" s="54">
@@ -4055,13 +4025,13 @@
         <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G38" s="103">
+        <v>185</v>
+      </c>
+      <c r="G38" s="102">
         <v>43186</v>
       </c>
       <c r="H38" s="6">
@@ -4079,23 +4049,23 @@
       <c r="R38" s="7"/>
     </row>
     <row r="39" spans="1:18" ht="126" x14ac:dyDescent="0.25">
-      <c r="A39" s="109">
+      <c r="A39" s="108">
         <v>8</v>
       </c>
       <c r="B39" s="54">
         <v>8.3000000000000007</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="103">
+        <v>69</v>
+      </c>
+      <c r="G39" s="102">
         <v>43182</v>
       </c>
       <c r="H39" s="6">
@@ -4113,7 +4083,7 @@
       <c r="R39" s="7"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="108">
+      <c r="A40" s="107">
         <v>9</v>
       </c>
       <c r="B40" s="53">
@@ -4123,13 +4093,13 @@
         <v>10</v>
       </c>
       <c r="D40" s="45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E40" s="46"/>
       <c r="F40" s="62" t="s">
-        <v>187</v>
-      </c>
-      <c r="G40" s="98">
+        <v>185</v>
+      </c>
+      <c r="G40" s="97">
         <v>43193</v>
       </c>
       <c r="H40" s="58">
@@ -4147,7 +4117,7 @@
       <c r="R40" s="7"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="108">
+      <c r="A41" s="107">
         <v>9</v>
       </c>
       <c r="B41" s="53">
@@ -4157,13 +4127,13 @@
         <v>10</v>
       </c>
       <c r="D41" s="45" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="62" t="s">
-        <v>187</v>
-      </c>
-      <c r="G41" s="98">
+        <v>185</v>
+      </c>
+      <c r="G41" s="97">
         <v>43193</v>
       </c>
       <c r="H41" s="58">
@@ -4181,23 +4151,23 @@
       <c r="R41" s="7"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="108">
+      <c r="A42" s="107">
         <v>9</v>
       </c>
       <c r="B42" s="53">
         <v>9.3000000000000007</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D42" s="45" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E42" s="46"/>
       <c r="F42" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="G42" s="98">
+        <v>69</v>
+      </c>
+      <c r="G42" s="97">
         <v>43187</v>
       </c>
       <c r="H42" s="58">
@@ -4215,7 +4185,7 @@
       <c r="R42" s="7"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="108">
+      <c r="A43" s="107">
         <v>9</v>
       </c>
       <c r="B43" s="53">
@@ -4225,13 +4195,13 @@
         <v>24</v>
       </c>
       <c r="D43" s="62" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E43" s="46"/>
       <c r="F43" s="62" t="s">
-        <v>185</v>
-      </c>
-      <c r="G43" s="98">
+        <v>183</v>
+      </c>
+      <c r="G43" s="97">
         <v>43188</v>
       </c>
       <c r="H43" s="58">
@@ -4249,23 +4219,23 @@
       <c r="R43" s="7"/>
     </row>
     <row r="44" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="109">
+      <c r="A44" s="108">
         <v>10</v>
       </c>
       <c r="B44" s="54">
         <v>10.1</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="73" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E44" s="57"/>
       <c r="F44" s="73" t="s">
-        <v>156</v>
-      </c>
-      <c r="G44" s="104">
+        <v>155</v>
+      </c>
+      <c r="G44" s="103">
         <v>43194</v>
       </c>
       <c r="H44" s="6">
@@ -4283,7 +4253,7 @@
       <c r="R44" s="7"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="109">
+      <c r="A45" s="108">
         <v>10</v>
       </c>
       <c r="B45" s="54">
@@ -4293,11 +4263,11 @@
         <v>24</v>
       </c>
       <c r="D45" s="73" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E45" s="57"/>
       <c r="F45" s="73"/>
-      <c r="G45" s="104">
+      <c r="G45" s="103">
         <v>43194</v>
       </c>
       <c r="H45" s="6">
@@ -4315,7 +4285,7 @@
       <c r="R45" s="7"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="109">
+      <c r="A46" s="108">
         <v>10</v>
       </c>
       <c r="B46" s="54">
@@ -4325,13 +4295,13 @@
         <v>24</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G46" s="103">
+        <v>183</v>
+      </c>
+      <c r="G46" s="102">
         <v>43195</v>
       </c>
       <c r="H46" s="6">
@@ -4349,23 +4319,23 @@
       <c r="R46" s="7"/>
     </row>
     <row r="47" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="112">
+      <c r="A47" s="111">
         <v>11</v>
       </c>
       <c r="B47" s="53">
         <v>11.1</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D47" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E47" s="46"/>
       <c r="F47" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="G47" s="98">
+        <v>153</v>
+      </c>
+      <c r="G47" s="97">
         <v>43203</v>
       </c>
       <c r="H47" s="58">
@@ -4383,7 +4353,7 @@
       <c r="R47" s="7"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="112">
+      <c r="A48" s="111">
         <v>11</v>
       </c>
       <c r="B48" s="53">
@@ -4393,13 +4363,13 @@
         <v>24</v>
       </c>
       <c r="D48" s="62" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E48" s="46"/>
       <c r="F48" s="62" t="s">
-        <v>185</v>
-      </c>
-      <c r="G48" s="98">
+        <v>183</v>
+      </c>
+      <c r="G48" s="97">
         <v>43202</v>
       </c>
       <c r="H48" s="58">
@@ -4417,7 +4387,7 @@
       <c r="R48" s="7"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="112">
+      <c r="A49" s="111">
         <v>11</v>
       </c>
       <c r="B49" s="53">
@@ -4427,13 +4397,13 @@
         <v>11</v>
       </c>
       <c r="D49" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E49" s="46"/>
       <c r="F49" s="62" t="s">
-        <v>187</v>
-      </c>
-      <c r="G49" s="98">
+        <v>185</v>
+      </c>
+      <c r="G49" s="97">
         <v>43214</v>
       </c>
       <c r="H49" s="58">
@@ -4451,7 +4421,7 @@
       <c r="R49" s="7"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="112">
+      <c r="A50" s="111">
         <v>11</v>
       </c>
       <c r="B50" s="53">
@@ -4461,13 +4431,13 @@
         <v>11</v>
       </c>
       <c r="D50" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E50" s="46"/>
       <c r="F50" s="62" t="s">
-        <v>187</v>
-      </c>
-      <c r="G50" s="98">
+        <v>185</v>
+      </c>
+      <c r="G50" s="97">
         <v>43214</v>
       </c>
       <c r="H50" s="58">
@@ -4485,7 +4455,7 @@
       <c r="R50" s="7"/>
     </row>
     <row r="51" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="112">
+      <c r="A51" s="111">
         <v>11</v>
       </c>
       <c r="B51" s="53">
@@ -4495,13 +4465,13 @@
         <v>24</v>
       </c>
       <c r="D51" s="62" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E51" s="46"/>
       <c r="F51" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="G51" s="98">
+        <v>217</v>
+      </c>
+      <c r="G51" s="97">
         <v>43203</v>
       </c>
       <c r="H51" s="58">
@@ -4519,7 +4489,7 @@
       <c r="R51" s="7"/>
     </row>
     <row r="52" spans="1:18" ht="63" x14ac:dyDescent="0.25">
-      <c r="A52" s="112">
+      <c r="A52" s="111">
         <v>11</v>
       </c>
       <c r="B52" s="53">
@@ -4529,13 +4499,13 @@
         <v>24</v>
       </c>
       <c r="D52" s="45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E52" s="46"/>
       <c r="F52" s="62" t="s">
-        <v>217</v>
-      </c>
-      <c r="G52" s="98">
+        <v>215</v>
+      </c>
+      <c r="G52" s="97">
         <v>43204</v>
       </c>
       <c r="H52" s="58">
@@ -4563,13 +4533,13 @@
         <v>24</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E53" s="57"/>
       <c r="F53" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="G53" s="104">
+        <v>213</v>
+      </c>
+      <c r="G53" s="103">
         <v>43208</v>
       </c>
       <c r="H53" s="6">
@@ -4597,13 +4567,13 @@
         <v>24</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G54" s="103">
+        <v>183</v>
+      </c>
+      <c r="G54" s="102">
         <v>43209</v>
       </c>
       <c r="H54" s="6">
@@ -4628,16 +4598,16 @@
         <v>12.3</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D55" s="73" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E55" s="57"/>
       <c r="F55" s="73" t="s">
-        <v>31</v>
-      </c>
-      <c r="G55" s="104">
+        <v>30</v>
+      </c>
+      <c r="G55" s="103">
         <v>43211</v>
       </c>
       <c r="H55" s="6">
@@ -4665,13 +4635,13 @@
         <v>24</v>
       </c>
       <c r="D56" s="62" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E56" s="46"/>
       <c r="F56" s="62" t="s">
-        <v>190</v>
-      </c>
-      <c r="G56" s="98">
+        <v>188</v>
+      </c>
+      <c r="G56" s="97">
         <v>43215</v>
       </c>
       <c r="H56" s="58">
@@ -4699,13 +4669,13 @@
         <v>24</v>
       </c>
       <c r="D57" s="62" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E57" s="46"/>
       <c r="F57" s="62" t="s">
-        <v>227</v>
-      </c>
-      <c r="G57" s="98">
+        <v>225</v>
+      </c>
+      <c r="G57" s="97">
         <v>43217</v>
       </c>
       <c r="H57" s="58">
@@ -4733,13 +4703,13 @@
         <v>24</v>
       </c>
       <c r="D58" s="62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E58" s="46"/>
       <c r="F58" s="62" t="s">
-        <v>190</v>
-      </c>
-      <c r="G58" s="98">
+        <v>188</v>
+      </c>
+      <c r="G58" s="97">
         <v>43218</v>
       </c>
       <c r="H58" s="58">
@@ -4767,17 +4737,17 @@
         <v>24</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E59" s="17"/>
       <c r="F59" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="G59" s="103">
+        <v>245</v>
+      </c>
+      <c r="G59" s="102">
         <v>43221</v>
       </c>
       <c r="H59" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
@@ -4798,22 +4768,22 @@
         <v>14.2</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D60" s="73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E60" s="57"/>
       <c r="F60" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="G60" s="104">
+        <v>159</v>
+      </c>
+      <c r="G60" s="103">
         <v>43222</v>
       </c>
       <c r="H60" s="79">
-        <v>20</v>
-      </c>
-      <c r="I60" s="97"/>
+        <v>30</v>
+      </c>
+      <c r="I60" s="96"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
@@ -4825,29 +4795,27 @@
       <c r="R60" s="7"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="54">
+      <c r="A61" s="55">
         <v>14</v>
       </c>
-      <c r="B61" s="54">
+      <c r="B61" s="55">
         <v>14.3</v>
       </c>
-      <c r="C61" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D61" s="56" t="s">
-        <v>228</v>
-      </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="9" t="s">
-        <v>187</v>
-      </c>
+      <c r="C61" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="113" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" s="114"/>
+      <c r="F61" s="113"/>
       <c r="G61" s="103">
-        <v>43235</v>
-      </c>
-      <c r="H61" s="6">
-        <v>35</v>
-      </c>
-      <c r="I61" s="7"/>
+        <v>43232</v>
+      </c>
+      <c r="H61" s="79">
+        <v>50</v>
+      </c>
+      <c r="I61" s="96"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -4859,27 +4827,25 @@
       <c r="R61" s="7"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="54">
-        <v>14</v>
-      </c>
-      <c r="B62" s="54">
-        <v>14.4</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" s="73" t="s">
-        <v>229</v>
-      </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G62" s="103">
-        <v>43235</v>
-      </c>
-      <c r="H62" s="6">
-        <v>35</v>
+      <c r="A62" s="53">
+        <v>15</v>
+      </c>
+      <c r="B62" s="53">
+        <v>15.2</v>
+      </c>
+      <c r="C62" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="95"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="104">
+        <v>43239</v>
+      </c>
+      <c r="H62" s="58">
+        <v>50</v>
       </c>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
@@ -4897,18 +4863,20 @@
         <v>15</v>
       </c>
       <c r="B63" s="53">
-        <v>15.1</v>
+        <v>15.3</v>
       </c>
       <c r="C63" s="94" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="D63" s="68" t="s">
-        <v>67</v>
+        <v>235</v>
       </c>
       <c r="E63" s="95"/>
-      <c r="F63" s="68"/>
-      <c r="G63" s="98">
-        <v>43232</v>
+      <c r="F63" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" s="104">
+        <v>43231</v>
       </c>
       <c r="H63" s="58">
         <v>25</v>
@@ -4924,23 +4892,25 @@
       <c r="Q63" s="7"/>
       <c r="R63" s="7"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" s="53">
         <v>15</v>
       </c>
       <c r="B64" s="53">
-        <v>15.2</v>
+        <v>15.4</v>
       </c>
       <c r="C64" s="94" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="D64" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="E64" s="96"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="105">
-        <v>43239</v>
+        <v>162</v>
+      </c>
+      <c r="E64" s="95"/>
+      <c r="F64" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="G64" s="104">
+        <v>43229</v>
       </c>
       <c r="H64" s="58">
         <v>25</v>
@@ -4957,26 +4927,26 @@
       <c r="R64" s="7"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="53">
-        <v>15</v>
-      </c>
-      <c r="B65" s="53">
-        <v>15.3</v>
-      </c>
-      <c r="C65" s="94" t="s">
-        <v>140</v>
-      </c>
-      <c r="D65" s="68" t="s">
-        <v>239</v>
-      </c>
-      <c r="E65" s="96"/>
-      <c r="F65" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="G65" s="105">
-        <v>43231</v>
-      </c>
-      <c r="H65" s="58">
+      <c r="A65" s="89">
+        <v>16</v>
+      </c>
+      <c r="B65" s="89">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C65" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="E65" s="92"/>
+      <c r="F65" s="91" t="s">
+        <v>243</v>
+      </c>
+      <c r="G65" s="112">
+        <v>43236</v>
+      </c>
+      <c r="H65" s="93">
         <v>25</v>
       </c>
       <c r="I65" s="7"/>
@@ -4990,27 +4960,27 @@
       <c r="Q65" s="7"/>
       <c r="R65" s="7"/>
     </row>
-    <row r="66" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="53">
-        <v>15</v>
-      </c>
-      <c r="B66" s="53">
-        <v>15.4</v>
-      </c>
-      <c r="C66" s="94" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="E66" s="96"/>
-      <c r="F66" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="G66" s="105">
-        <v>43229</v>
-      </c>
-      <c r="H66" s="58">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="89">
+        <v>16</v>
+      </c>
+      <c r="B66" s="89">
+        <v>16.2</v>
+      </c>
+      <c r="C66" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="91" t="s">
+        <v>233</v>
+      </c>
+      <c r="E66" s="92"/>
+      <c r="F66" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="G66" s="112">
+        <v>43239</v>
+      </c>
+      <c r="H66" s="93">
         <v>25</v>
       </c>
       <c r="I66" s="7"/>
@@ -5024,28 +4994,28 @@
       <c r="Q66" s="7"/>
       <c r="R66" s="7"/>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A67" s="89">
         <v>16</v>
       </c>
       <c r="B67" s="89">
-        <v>16.100000000000001</v>
+        <v>16.3</v>
       </c>
       <c r="C67" s="90" t="s">
-        <v>24</v>
+        <v>241</v>
       </c>
       <c r="D67" s="91" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="E67" s="92"/>
       <c r="F67" s="91" t="s">
-        <v>248</v>
-      </c>
-      <c r="G67" s="113">
-        <v>43236</v>
+        <v>69</v>
+      </c>
+      <c r="G67" s="112">
+        <v>43239</v>
       </c>
       <c r="H67" s="93">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -5059,28 +5029,9 @@
       <c r="R67" s="7"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="89">
-        <v>16</v>
-      </c>
-      <c r="B68" s="89">
-        <v>16.2</v>
-      </c>
-      <c r="C68" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="91" t="s">
-        <v>237</v>
-      </c>
-      <c r="E68" s="92"/>
-      <c r="F68" s="91" t="s">
-        <v>249</v>
-      </c>
-      <c r="G68" s="113">
-        <v>43239</v>
-      </c>
-      <c r="H68" s="93">
-        <v>25</v>
-      </c>
+      <c r="E68" s="19"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="6"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
@@ -5092,29 +5043,12 @@
       <c r="Q68" s="7"/>
       <c r="R68" s="7"/>
     </row>
-    <row r="69" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="89">
-        <v>16</v>
-      </c>
-      <c r="B69" s="89">
-        <v>16.3</v>
-      </c>
-      <c r="C69" s="90" t="s">
-        <v>246</v>
-      </c>
-      <c r="D69" s="91" t="s">
-        <v>238</v>
-      </c>
-      <c r="E69" s="92"/>
-      <c r="F69" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="G69" s="113">
-        <v>43239</v>
-      </c>
-      <c r="H69" s="93">
-        <v>50</v>
-      </c>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C69" s="12"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="6"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
@@ -5127,9 +5061,11 @@
       <c r="R69" s="7"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E70" s="19"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="6"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="105"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
@@ -5146,7 +5082,6 @@
       <c r="D71" s="3"/>
       <c r="E71" s="17"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="6"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
@@ -5163,7 +5098,7 @@
       <c r="D72" s="3"/>
       <c r="E72" s="17"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="106"/>
+      <c r="G72" s="105"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
@@ -5193,10 +5128,10 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C74" s="12"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="106"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="8"/>
+      <c r="G74" s="6"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
@@ -5226,10 +5161,10 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C76" s="12"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="6"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="105"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
@@ -5243,9 +5178,6 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C77" s="12"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="3"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -5258,11 +5190,10 @@
       <c r="R77" s="7"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C78" s="12"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="106"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="5"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
@@ -5275,7 +5206,10 @@
       <c r="R78" s="7"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C79" s="12"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="5"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
@@ -21080,10 +21014,6 @@
       <c r="R1066" s="7"/>
     </row>
     <row r="1067" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C1067" s="16"/>
-      <c r="D1067" s="5"/>
-      <c r="E1067" s="19"/>
-      <c r="F1067" s="5"/>
       <c r="I1067" s="7"/>
       <c r="J1067" s="7"/>
       <c r="K1067" s="7"/>
@@ -21096,10 +21026,6 @@
       <c r="R1067" s="7"/>
     </row>
     <row r="1068" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C1068" s="16"/>
-      <c r="D1068" s="5"/>
-      <c r="E1068" s="19"/>
-      <c r="F1068" s="5"/>
       <c r="I1068" s="7"/>
       <c r="J1068" s="7"/>
       <c r="K1068" s="7"/>
@@ -21123,82 +21049,58 @@
       <c r="Q1069" s="7"/>
       <c r="R1069" s="7"/>
     </row>
-    <row r="1070" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="I1070" s="7"/>
-      <c r="J1070" s="7"/>
-      <c r="K1070" s="7"/>
-      <c r="L1070" s="7"/>
-      <c r="M1070" s="7"/>
-      <c r="N1070" s="7"/>
-      <c r="O1070" s="7"/>
-      <c r="P1070" s="7"/>
-      <c r="Q1070" s="7"/>
-      <c r="R1070" s="7"/>
-    </row>
-    <row r="1071" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="I1071" s="7"/>
-      <c r="J1071" s="7"/>
-      <c r="K1071" s="7"/>
-      <c r="L1071" s="7"/>
-      <c r="M1071" s="7"/>
-      <c r="N1071" s="7"/>
-      <c r="O1071" s="7"/>
-      <c r="P1071" s="7"/>
-      <c r="Q1071" s="7"/>
-      <c r="R1071" s="7"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R1075">
-    <sortCondition ref="A2:A1075"/>
-    <sortCondition ref="B2:B1075"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R1073">
+    <sortCondition ref="A2:A1073"/>
+    <sortCondition ref="B2:B1073"/>
   </sortState>
-  <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31 G58:G60 G37:G53 G55 G63:G1048576">
-    <cfRule type="timePeriod" dxfId="9" priority="13" timePeriod="last7Days">
+  <conditionalFormatting sqref="G1:G21 G24:G25 G28:G29 G31 G37:G53 G55 G58:G60 G62:G1048576">
+    <cfRule type="timePeriod" dxfId="9" priority="14" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G1,1)&lt;=6,FLOOR(G1,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:G27">
-    <cfRule type="timePeriod" dxfId="8" priority="12" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="8" priority="13" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G26,1)&lt;=6,FLOOR(G26,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="timePeriod" dxfId="7" priority="11" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="7" priority="12" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G22,1)&lt;=6,FLOOR(G22,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="timePeriod" dxfId="6" priority="10" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="6" priority="11" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G23,1)&lt;=6,FLOOR(G23,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="timePeriod" dxfId="5" priority="9" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="5" priority="10" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G30,1)&lt;=6,FLOOR(G30,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:G36">
-    <cfRule type="timePeriod" dxfId="4" priority="7" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="4" priority="8" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G34,1)&lt;=6,FLOOR(G34,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G33">
-    <cfRule type="timePeriod" dxfId="3" priority="6" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="3" priority="7" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G32,1)&lt;=6,FLOOR(G32,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="timePeriod" dxfId="2" priority="5" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="2" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G54,1)&lt;=6,FLOOR(G54,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:G57">
-    <cfRule type="timePeriod" dxfId="1" priority="4" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="1" priority="5" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G56,1)&lt;=6,FLOOR(G56,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G61:G62">
-    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="last7Days">
+  <conditionalFormatting sqref="G61">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(G61,1)&lt;=6,FLOOR(G61,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>